<commit_message>
new gender gap data 06-14 (US & CN)
json file created by
https://www.jsoneditoronline.org/#
http://shancarter.github.io/mr-data-converter/
There are two kinds of json - properties & dictionary
</commit_message>
<xml_diff>
--- a/GenderGap_Data/GenderGap_Find4Hourglass.xlsx
+++ b/GenderGap_Data/GenderGap_Find4Hourglass.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="0" windowWidth="28980" windowHeight="21500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22860" windowHeight="12480" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="13C_csv" sheetId="10" r:id="rId1"/>
@@ -1177,7 +1177,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="175">
+  <cellStyleXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1287,6 +1287,14 @@
     <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1675,7 +1683,43 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="106" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="2" xfId="106" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="3" xfId="106" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="4" xfId="106" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" xfId="108" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="16" xfId="108" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1690,7 +1734,19 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1705,54 +1761,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="2" xfId="106" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="3" xfId="106" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="4" xfId="106" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="106" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" xfId="108" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="16" xfId="108" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1760,7 +1768,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="175">
+  <cellStyles count="183">
     <cellStyle name="Bad" xfId="107" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="108" builtinId="23"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1848,6 +1856,10 @@
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="106" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1934,6 +1946,10 @@
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="105"/>
   </cellStyles>
@@ -2310,11 +2326,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="-2076543688"/>
-        <c:axId val="-2076540664"/>
+        <c:axId val="-2123193160"/>
+        <c:axId val="-2123196200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2076543688"/>
+        <c:axId val="-2123193160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2323,7 +2339,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076540664"/>
+        <c:crossAx val="-2123196200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2331,7 +2347,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2076540664"/>
+        <c:axId val="-2123196200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2347,7 +2363,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2076543688"/>
+        <c:crossAx val="-2123193160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2562,11 +2578,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2073854008"/>
-        <c:axId val="-2073851016"/>
+        <c:axId val="-2123271464"/>
+        <c:axId val="-2123274424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2073854008"/>
+        <c:axId val="-2123271464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2575,7 +2591,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073851016"/>
+        <c:crossAx val="-2123274424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2583,7 +2599,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2073851016"/>
+        <c:axId val="-2123274424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2594,7 +2610,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="-2073854008"/>
+        <c:crossAx val="-2123271464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3020,8 +3036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA6" sqref="AA6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6070,8 +6086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6100,37 +6116,37 @@
     <row r="1" spans="1:27" ht="34" customHeight="1">
       <c r="A1" s="97"/>
       <c r="B1" s="97"/>
-      <c r="C1" s="118" t="s">
+      <c r="C1" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="118" t="s">
+      <c r="D1" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="118" t="s">
+      <c r="E1" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="139" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="119" t="s">
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="134" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
-      <c r="N1" s="119"/>
-      <c r="O1" s="114" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="114"/>
-      <c r="Q1" s="119" t="s">
+      <c r="L1" s="134"/>
+      <c r="M1" s="134"/>
+      <c r="N1" s="134"/>
+      <c r="O1" s="135" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="135"/>
+      <c r="Q1" s="134" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="119"/>
-      <c r="S1" s="119"/>
+      <c r="R1" s="134"/>
+      <c r="S1" s="134"/>
       <c r="T1" s="71" t="s">
         <v>92</v>
       </c>
@@ -6147,9 +6163,9 @@
     <row r="2" spans="1:27" ht="113" customHeight="1">
       <c r="A2" s="97"/>
       <c r="B2" s="97"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -6218,13 +6234,13 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="136" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="115">
-        <v>1</v>
-      </c>
-      <c r="C3" s="118" t="s">
+      <c r="B3" s="127">
+        <v>1</v>
+      </c>
+      <c r="C3" s="130" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="92">
@@ -6292,9 +6308,9 @@
       </c>
     </row>
     <row r="4" spans="1:27">
-      <c r="A4" s="121"/>
-      <c r="B4" s="116"/>
-      <c r="C4" s="118"/>
+      <c r="A4" s="137"/>
+      <c r="B4" s="128"/>
+      <c r="C4" s="130"/>
       <c r="D4" s="92">
         <v>2010</v>
       </c>
@@ -6360,9 +6376,9 @@
       </c>
     </row>
     <row r="5" spans="1:27">
-      <c r="A5" s="121"/>
-      <c r="B5" s="117"/>
-      <c r="C5" s="118"/>
+      <c r="A5" s="137"/>
+      <c r="B5" s="129"/>
+      <c r="C5" s="130"/>
       <c r="D5" s="25">
         <v>2014</v>
       </c>
@@ -6428,7 +6444,7 @@
       </c>
     </row>
     <row r="6" spans="1:27">
-      <c r="A6" s="121"/>
+      <c r="A6" s="137"/>
       <c r="B6" s="91"/>
       <c r="C6" s="92"/>
       <c r="D6" s="25"/>
@@ -6450,11 +6466,11 @@
       <c r="X6" s="106"/>
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1">
-      <c r="A7" s="121"/>
-      <c r="B7" s="115">
+      <c r="A7" s="137"/>
+      <c r="B7" s="127">
         <v>2</v>
       </c>
-      <c r="C7" s="118" t="s">
+      <c r="C7" s="130" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="92">
@@ -6522,9 +6538,9 @@
       </c>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="121"/>
-      <c r="B8" s="116"/>
-      <c r="C8" s="118"/>
+      <c r="A8" s="137"/>
+      <c r="B8" s="128"/>
+      <c r="C8" s="130"/>
       <c r="D8" s="92">
         <v>2010</v>
       </c>
@@ -6590,9 +6606,9 @@
       </c>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="121"/>
-      <c r="B9" s="117"/>
-      <c r="C9" s="118"/>
+      <c r="A9" s="137"/>
+      <c r="B9" s="129"/>
+      <c r="C9" s="130"/>
       <c r="D9" s="25">
         <v>2014</v>
       </c>
@@ -6658,7 +6674,7 @@
       </c>
     </row>
     <row r="10" spans="1:27">
-      <c r="A10" s="121"/>
+      <c r="A10" s="137"/>
       <c r="B10" s="91"/>
       <c r="C10" s="92"/>
       <c r="D10" s="25"/>
@@ -6680,11 +6696,11 @@
       <c r="X10" s="106"/>
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A11" s="121"/>
-      <c r="B11" s="115">
+      <c r="A11" s="137"/>
+      <c r="B11" s="127">
         <v>3</v>
       </c>
-      <c r="C11" s="118" t="s">
+      <c r="C11" s="130" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="92">
@@ -6752,9 +6768,9 @@
       </c>
     </row>
     <row r="12" spans="1:27">
-      <c r="A12" s="121"/>
-      <c r="B12" s="116"/>
-      <c r="C12" s="118"/>
+      <c r="A12" s="137"/>
+      <c r="B12" s="128"/>
+      <c r="C12" s="130"/>
       <c r="D12" s="92">
         <v>2010</v>
       </c>
@@ -6820,9 +6836,9 @@
       </c>
     </row>
     <row r="13" spans="1:27">
-      <c r="A13" s="121"/>
-      <c r="B13" s="117"/>
-      <c r="C13" s="118"/>
+      <c r="A13" s="137"/>
+      <c r="B13" s="129"/>
+      <c r="C13" s="130"/>
       <c r="D13" s="25">
         <v>2014</v>
       </c>
@@ -6888,7 +6904,7 @@
       </c>
     </row>
     <row r="14" spans="1:27">
-      <c r="A14" s="121"/>
+      <c r="A14" s="137"/>
       <c r="B14" s="91"/>
       <c r="C14" s="92"/>
       <c r="D14" s="25"/>
@@ -6910,11 +6926,11 @@
       <c r="X14" s="106"/>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="121"/>
-      <c r="B15" s="115">
+      <c r="A15" s="137"/>
+      <c r="B15" s="127">
         <v>4</v>
       </c>
-      <c r="C15" s="118" t="s">
+      <c r="C15" s="130" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="92">
@@ -6982,9 +6998,9 @@
       </c>
     </row>
     <row r="16" spans="1:27">
-      <c r="A16" s="121"/>
-      <c r="B16" s="116"/>
-      <c r="C16" s="118"/>
+      <c r="A16" s="137"/>
+      <c r="B16" s="128"/>
+      <c r="C16" s="130"/>
       <c r="D16" s="92">
         <v>2010</v>
       </c>
@@ -7050,9 +7066,9 @@
       </c>
     </row>
     <row r="17" spans="1:24">
-      <c r="A17" s="121"/>
-      <c r="B17" s="117"/>
-      <c r="C17" s="118"/>
+      <c r="A17" s="137"/>
+      <c r="B17" s="129"/>
+      <c r="C17" s="130"/>
       <c r="D17" s="25">
         <v>2014</v>
       </c>
@@ -7118,7 +7134,7 @@
       </c>
     </row>
     <row r="18" spans="1:24">
-      <c r="A18" s="121"/>
+      <c r="A18" s="137"/>
       <c r="B18" s="91"/>
       <c r="C18" s="92"/>
       <c r="D18" s="25"/>
@@ -7140,11 +7156,11 @@
       <c r="X18" s="106"/>
     </row>
     <row r="19" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A19" s="121"/>
-      <c r="B19" s="115">
+      <c r="A19" s="137"/>
+      <c r="B19" s="127">
         <v>5</v>
       </c>
-      <c r="C19" s="118" t="s">
+      <c r="C19" s="130" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="92">
@@ -7212,9 +7228,9 @@
       </c>
     </row>
     <row r="20" spans="1:24">
-      <c r="A20" s="121"/>
-      <c r="B20" s="116"/>
-      <c r="C20" s="118"/>
+      <c r="A20" s="137"/>
+      <c r="B20" s="128"/>
+      <c r="C20" s="130"/>
       <c r="D20" s="92">
         <v>2010</v>
       </c>
@@ -7280,9 +7296,9 @@
       </c>
     </row>
     <row r="21" spans="1:24">
-      <c r="A21" s="121"/>
-      <c r="B21" s="117"/>
-      <c r="C21" s="118"/>
+      <c r="A21" s="137"/>
+      <c r="B21" s="129"/>
+      <c r="C21" s="130"/>
       <c r="D21" s="25">
         <v>2014</v>
       </c>
@@ -7348,7 +7364,7 @@
       </c>
     </row>
     <row r="22" spans="1:24">
-      <c r="A22" s="121"/>
+      <c r="A22" s="137"/>
       <c r="B22" s="91"/>
       <c r="C22" s="92"/>
       <c r="D22" s="25"/>
@@ -7370,11 +7386,11 @@
       <c r="X22" s="106"/>
     </row>
     <row r="23" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A23" s="121"/>
-      <c r="B23" s="115">
+      <c r="A23" s="137"/>
+      <c r="B23" s="127">
         <v>6</v>
       </c>
-      <c r="C23" s="118" t="s">
+      <c r="C23" s="130" t="s">
         <v>25</v>
       </c>
       <c r="D23" s="92">
@@ -7442,9 +7458,9 @@
       </c>
     </row>
     <row r="24" spans="1:24">
-      <c r="A24" s="121"/>
-      <c r="B24" s="116"/>
-      <c r="C24" s="118"/>
+      <c r="A24" s="137"/>
+      <c r="B24" s="128"/>
+      <c r="C24" s="130"/>
       <c r="D24" s="92">
         <v>2010</v>
       </c>
@@ -7510,9 +7526,9 @@
       </c>
     </row>
     <row r="25" spans="1:24">
-      <c r="A25" s="121"/>
-      <c r="B25" s="117"/>
-      <c r="C25" s="118"/>
+      <c r="A25" s="137"/>
+      <c r="B25" s="129"/>
+      <c r="C25" s="130"/>
       <c r="D25" s="25">
         <v>2014</v>
       </c>
@@ -7578,7 +7594,7 @@
       </c>
     </row>
     <row r="26" spans="1:24">
-      <c r="A26" s="121"/>
+      <c r="A26" s="137"/>
       <c r="B26" s="91"/>
       <c r="C26" s="92"/>
       <c r="D26" s="25"/>
@@ -7600,11 +7616,11 @@
       <c r="X26" s="106"/>
     </row>
     <row r="27" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A27" s="121"/>
-      <c r="B27" s="115">
+      <c r="A27" s="137"/>
+      <c r="B27" s="127">
         <v>7</v>
       </c>
-      <c r="C27" s="118" t="s">
+      <c r="C27" s="130" t="s">
         <v>70</v>
       </c>
       <c r="D27" s="92">
@@ -7672,9 +7688,9 @@
       </c>
     </row>
     <row r="28" spans="1:24">
-      <c r="A28" s="121"/>
-      <c r="B28" s="116"/>
-      <c r="C28" s="118"/>
+      <c r="A28" s="137"/>
+      <c r="B28" s="128"/>
+      <c r="C28" s="130"/>
       <c r="D28" s="92">
         <v>2010</v>
       </c>
@@ -7740,9 +7756,9 @@
       </c>
     </row>
     <row r="29" spans="1:24">
-      <c r="A29" s="121"/>
-      <c r="B29" s="117"/>
-      <c r="C29" s="118"/>
+      <c r="A29" s="137"/>
+      <c r="B29" s="129"/>
+      <c r="C29" s="130"/>
       <c r="D29" s="25">
         <v>2014</v>
       </c>
@@ -7808,7 +7824,7 @@
       </c>
     </row>
     <row r="30" spans="1:24">
-      <c r="A30" s="121"/>
+      <c r="A30" s="137"/>
       <c r="B30" s="91"/>
       <c r="C30" s="95"/>
       <c r="D30" s="25"/>
@@ -7830,11 +7846,11 @@
       <c r="X30" s="106"/>
     </row>
     <row r="31" spans="1:24">
-      <c r="A31" s="121"/>
-      <c r="B31" s="115">
+      <c r="A31" s="137"/>
+      <c r="B31" s="127">
         <v>8</v>
       </c>
-      <c r="C31" s="124" t="s">
+      <c r="C31" s="131" t="s">
         <v>54</v>
       </c>
       <c r="D31" s="92">
@@ -7902,9 +7918,9 @@
       </c>
     </row>
     <row r="32" spans="1:24">
-      <c r="A32" s="121"/>
-      <c r="B32" s="116"/>
-      <c r="C32" s="125"/>
+      <c r="A32" s="137"/>
+      <c r="B32" s="128"/>
+      <c r="C32" s="132"/>
       <c r="D32" s="92">
         <v>2010</v>
       </c>
@@ -7970,9 +7986,9 @@
       </c>
     </row>
     <row r="33" spans="1:24">
-      <c r="A33" s="121"/>
-      <c r="B33" s="117"/>
-      <c r="C33" s="126"/>
+      <c r="A33" s="137"/>
+      <c r="B33" s="129"/>
+      <c r="C33" s="133"/>
       <c r="D33" s="25">
         <v>2014</v>
       </c>
@@ -8038,7 +8054,7 @@
       </c>
     </row>
     <row r="34" spans="1:24">
-      <c r="A34" s="121"/>
+      <c r="A34" s="137"/>
       <c r="B34" s="91"/>
       <c r="C34" s="96"/>
       <c r="D34" s="25"/>
@@ -8060,11 +8076,11 @@
       <c r="X34" s="106"/>
     </row>
     <row r="35" spans="1:24">
-      <c r="A35" s="121"/>
-      <c r="B35" s="115">
+      <c r="A35" s="137"/>
+      <c r="B35" s="127">
         <v>9</v>
       </c>
-      <c r="C35" s="118" t="s">
+      <c r="C35" s="130" t="s">
         <v>12</v>
       </c>
       <c r="D35" s="92">
@@ -8132,9 +8148,9 @@
       </c>
     </row>
     <row r="36" spans="1:24">
-      <c r="A36" s="121"/>
-      <c r="B36" s="116"/>
-      <c r="C36" s="118"/>
+      <c r="A36" s="137"/>
+      <c r="B36" s="128"/>
+      <c r="C36" s="130"/>
       <c r="D36" s="92">
         <v>2010</v>
       </c>
@@ -8200,9 +8216,9 @@
       </c>
     </row>
     <row r="37" spans="1:24">
-      <c r="A37" s="121"/>
-      <c r="B37" s="117"/>
-      <c r="C37" s="118"/>
+      <c r="A37" s="137"/>
+      <c r="B37" s="129"/>
+      <c r="C37" s="130"/>
       <c r="D37" s="25">
         <v>2014</v>
       </c>
@@ -8268,7 +8284,7 @@
       </c>
     </row>
     <row r="38" spans="1:24">
-      <c r="A38" s="121"/>
+      <c r="A38" s="137"/>
       <c r="B38" s="91"/>
       <c r="C38" s="92"/>
       <c r="D38" s="25"/>
@@ -8290,11 +8306,11 @@
       <c r="X38" s="106"/>
     </row>
     <row r="39" spans="1:24">
-      <c r="A39" s="121"/>
-      <c r="B39" s="115">
+      <c r="A39" s="137"/>
+      <c r="B39" s="127">
         <v>10</v>
       </c>
-      <c r="C39" s="118" t="s">
+      <c r="C39" s="130" t="s">
         <v>28</v>
       </c>
       <c r="D39" s="92">
@@ -8362,9 +8378,9 @@
       </c>
     </row>
     <row r="40" spans="1:24">
-      <c r="A40" s="121"/>
-      <c r="B40" s="116"/>
-      <c r="C40" s="118"/>
+      <c r="A40" s="137"/>
+      <c r="B40" s="128"/>
+      <c r="C40" s="130"/>
       <c r="D40" s="92">
         <v>2010</v>
       </c>
@@ -8430,9 +8446,9 @@
       </c>
     </row>
     <row r="41" spans="1:24">
-      <c r="A41" s="121"/>
-      <c r="B41" s="117"/>
-      <c r="C41" s="118"/>
+      <c r="A41" s="137"/>
+      <c r="B41" s="129"/>
+      <c r="C41" s="130"/>
       <c r="D41" s="25">
         <v>2014</v>
       </c>
@@ -8498,7 +8514,7 @@
       </c>
     </row>
     <row r="42" spans="1:24">
-      <c r="A42" s="121"/>
+      <c r="A42" s="137"/>
       <c r="B42" s="91"/>
       <c r="C42" s="92"/>
       <c r="D42" s="25"/>
@@ -8520,11 +8536,11 @@
       <c r="X42" s="106"/>
     </row>
     <row r="43" spans="1:24">
-      <c r="A43" s="121"/>
-      <c r="B43" s="115">
+      <c r="A43" s="137"/>
+      <c r="B43" s="127">
         <v>11</v>
       </c>
-      <c r="C43" s="118" t="s">
+      <c r="C43" s="130" t="s">
         <v>21</v>
       </c>
       <c r="D43" s="92">
@@ -8592,9 +8608,9 @@
       </c>
     </row>
     <row r="44" spans="1:24">
-      <c r="A44" s="121"/>
-      <c r="B44" s="116"/>
-      <c r="C44" s="118"/>
+      <c r="A44" s="137"/>
+      <c r="B44" s="128"/>
+      <c r="C44" s="130"/>
       <c r="D44" s="92">
         <v>2010</v>
       </c>
@@ -8660,9 +8676,9 @@
       </c>
     </row>
     <row r="45" spans="1:24">
-      <c r="A45" s="121"/>
-      <c r="B45" s="117"/>
-      <c r="C45" s="118"/>
+      <c r="A45" s="137"/>
+      <c r="B45" s="129"/>
+      <c r="C45" s="130"/>
       <c r="D45" s="25">
         <v>2014</v>
       </c>
@@ -8728,7 +8744,7 @@
       </c>
     </row>
     <row r="46" spans="1:24">
-      <c r="A46" s="121"/>
+      <c r="A46" s="137"/>
       <c r="B46" s="91"/>
       <c r="C46" s="92"/>
       <c r="D46" s="25"/>
@@ -8750,11 +8766,11 @@
       <c r="X46" s="106"/>
     </row>
     <row r="47" spans="1:24">
-      <c r="A47" s="121"/>
-      <c r="B47" s="115">
+      <c r="A47" s="137"/>
+      <c r="B47" s="127">
         <v>12</v>
       </c>
-      <c r="C47" s="118" t="s">
+      <c r="C47" s="130" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="92">
@@ -8822,9 +8838,9 @@
       </c>
     </row>
     <row r="48" spans="1:24">
-      <c r="A48" s="121"/>
-      <c r="B48" s="116"/>
-      <c r="C48" s="118"/>
+      <c r="A48" s="137"/>
+      <c r="B48" s="128"/>
+      <c r="C48" s="130"/>
       <c r="D48" s="92">
         <v>2010</v>
       </c>
@@ -8890,9 +8906,9 @@
       </c>
     </row>
     <row r="49" spans="1:41">
-      <c r="A49" s="121"/>
-      <c r="B49" s="117"/>
-      <c r="C49" s="118"/>
+      <c r="A49" s="137"/>
+      <c r="B49" s="129"/>
+      <c r="C49" s="130"/>
       <c r="D49" s="25">
         <v>2014</v>
       </c>
@@ -8958,7 +8974,7 @@
       </c>
     </row>
     <row r="50" spans="1:41">
-      <c r="A50" s="121"/>
+      <c r="A50" s="137"/>
       <c r="B50" s="91"/>
       <c r="C50" s="92"/>
       <c r="D50" s="25"/>
@@ -8980,11 +8996,11 @@
       <c r="X50" s="106"/>
     </row>
     <row r="51" spans="1:41">
-      <c r="A51" s="121"/>
-      <c r="B51" s="115">
+      <c r="A51" s="137"/>
+      <c r="B51" s="127">
         <v>13</v>
       </c>
-      <c r="C51" s="118" t="s">
+      <c r="C51" s="130" t="s">
         <v>8</v>
       </c>
       <c r="D51" s="92">
@@ -9052,9 +9068,9 @@
       </c>
     </row>
     <row r="52" spans="1:41">
-      <c r="A52" s="121"/>
-      <c r="B52" s="116"/>
-      <c r="C52" s="118"/>
+      <c r="A52" s="137"/>
+      <c r="B52" s="128"/>
+      <c r="C52" s="130"/>
       <c r="D52" s="92">
         <v>2010</v>
       </c>
@@ -9120,9 +9136,9 @@
       </c>
     </row>
     <row r="53" spans="1:41">
-      <c r="A53" s="121"/>
-      <c r="B53" s="117"/>
-      <c r="C53" s="118"/>
+      <c r="A53" s="137"/>
+      <c r="B53" s="129"/>
+      <c r="C53" s="130"/>
       <c r="D53" s="25">
         <v>2014</v>
       </c>
@@ -9188,79 +9204,79 @@
       </c>
     </row>
     <row r="54" spans="1:41">
-      <c r="A54" s="121"/>
+      <c r="A54" s="137"/>
     </row>
     <row r="55" spans="1:41" s="75" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A55" s="121"/>
+      <c r="A55" s="137"/>
       <c r="B55" s="86"/>
-      <c r="C55" s="130" t="s">
+      <c r="C55" s="114" t="s">
         <v>50</v>
       </c>
-      <c r="D55" s="130"/>
-      <c r="E55" s="130"/>
-      <c r="F55" s="130" t="s">
+      <c r="D55" s="114"/>
+      <c r="E55" s="114"/>
+      <c r="F55" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="G55" s="130"/>
-      <c r="H55" s="130"/>
-      <c r="I55" s="130" t="s">
+      <c r="G55" s="114"/>
+      <c r="H55" s="114"/>
+      <c r="I55" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="J55" s="130"/>
-      <c r="K55" s="130"/>
-      <c r="L55" s="130" t="s">
+      <c r="J55" s="114"/>
+      <c r="K55" s="114"/>
+      <c r="L55" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="M55" s="130"/>
-      <c r="N55" s="130"/>
-      <c r="O55" s="130" t="s">
+      <c r="M55" s="114"/>
+      <c r="N55" s="114"/>
+      <c r="O55" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="P55" s="130"/>
-      <c r="Q55" s="130"/>
-      <c r="R55" s="127" t="s">
+      <c r="P55" s="114"/>
+      <c r="Q55" s="114"/>
+      <c r="R55" s="122" t="s">
         <v>87</v>
       </c>
-      <c r="S55" s="128"/>
-      <c r="T55" s="129"/>
-      <c r="U55" s="130" t="s">
+      <c r="S55" s="123"/>
+      <c r="T55" s="124"/>
+      <c r="U55" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="V55" s="130"/>
-      <c r="W55" s="130"/>
-      <c r="X55" s="127" t="s">
+      <c r="V55" s="114"/>
+      <c r="W55" s="114"/>
+      <c r="X55" s="122" t="s">
         <v>54</v>
       </c>
-      <c r="Y55" s="128"/>
-      <c r="Z55" s="129"/>
-      <c r="AA55" s="130" t="s">
+      <c r="Y55" s="123"/>
+      <c r="Z55" s="124"/>
+      <c r="AA55" s="114" t="s">
         <v>105</v>
       </c>
-      <c r="AB55" s="130"/>
-      <c r="AC55" s="130"/>
-      <c r="AD55" s="130" t="s">
+      <c r="AB55" s="114"/>
+      <c r="AC55" s="114"/>
+      <c r="AD55" s="114" t="s">
         <v>109</v>
       </c>
-      <c r="AE55" s="130"/>
-      <c r="AF55" s="130"/>
-      <c r="AG55" s="130" t="s">
+      <c r="AE55" s="114"/>
+      <c r="AF55" s="114"/>
+      <c r="AG55" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="AH55" s="130"/>
-      <c r="AI55" s="130"/>
-      <c r="AJ55" s="130" t="s">
+      <c r="AH55" s="114"/>
+      <c r="AI55" s="114"/>
+      <c r="AJ55" s="114" t="s">
         <v>13</v>
       </c>
-      <c r="AK55" s="130"/>
-      <c r="AL55" s="130"/>
-      <c r="AM55" s="130" t="s">
+      <c r="AK55" s="114"/>
+      <c r="AL55" s="114"/>
+      <c r="AM55" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="AN55" s="130"/>
-      <c r="AO55" s="130"/>
+      <c r="AN55" s="114"/>
+      <c r="AO55" s="114"/>
     </row>
     <row r="56" spans="1:41" s="75" customFormat="1" ht="70">
-      <c r="A56" s="122"/>
+      <c r="A56" s="138"/>
       <c r="B56" s="86"/>
       <c r="C56" s="86" t="s">
         <v>72</v>
@@ -9501,10 +9517,10 @@
       </c>
     </row>
     <row r="58" spans="1:41" s="79" customFormat="1" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A58" s="131" t="s">
+      <c r="A58" s="125" t="s">
         <v>129</v>
       </c>
-      <c r="B58" s="132"/>
+      <c r="B58" s="126"/>
       <c r="C58" s="79">
         <v>2006</v>
       </c>
@@ -9541,10 +9557,10 @@
       <c r="Y58" s="105"/>
     </row>
     <row r="59" spans="1:41" ht="16" thickTop="1">
-      <c r="A59" s="133" t="s">
+      <c r="A59" s="119" t="s">
         <v>125</v>
       </c>
-      <c r="B59" s="133"/>
+      <c r="B59" s="119"/>
       <c r="C59">
         <f xml:space="preserve"> C57/115</f>
         <v>3.4782608695652174E-2</v>
@@ -9703,10 +9719,10 @@
       </c>
     </row>
     <row r="60" spans="1:41">
-      <c r="A60" s="134" t="s">
+      <c r="A60" s="120" t="s">
         <v>124</v>
       </c>
-      <c r="B60" s="134"/>
+      <c r="B60" s="120"/>
       <c r="C60">
         <f xml:space="preserve"> C59*72</f>
         <v>2.5043478260869567</v>
@@ -9865,10 +9881,10 @@
       </c>
     </row>
     <row r="61" spans="1:41" s="80" customFormat="1">
-      <c r="A61" s="135" t="s">
+      <c r="A61" s="121" t="s">
         <v>126</v>
       </c>
-      <c r="B61" s="135"/>
+      <c r="B61" s="121"/>
       <c r="C61" s="80">
         <f xml:space="preserve"> 72-C60</f>
         <v>69.495652173913044</v>
@@ -10178,77 +10194,77 @@
       <c r="X66" s="85"/>
     </row>
     <row r="67" spans="1:41">
-      <c r="C67" s="130" t="s">
+      <c r="C67" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="D67" s="130"/>
-      <c r="E67" s="130"/>
-      <c r="F67" s="127" t="s">
+      <c r="D67" s="114"/>
+      <c r="E67" s="114"/>
+      <c r="F67" s="122" t="s">
         <v>54</v>
       </c>
-      <c r="G67" s="128"/>
-      <c r="H67" s="129"/>
-      <c r="I67" s="130" t="s">
+      <c r="G67" s="123"/>
+      <c r="H67" s="124"/>
+      <c r="I67" s="114" t="s">
         <v>105</v>
       </c>
-      <c r="J67" s="130"/>
-      <c r="K67" s="130"/>
-      <c r="L67" s="130" t="s">
+      <c r="J67" s="114"/>
+      <c r="K67" s="114"/>
+      <c r="L67" s="114" t="s">
         <v>50</v>
       </c>
-      <c r="M67" s="130"/>
-      <c r="N67" s="130"/>
-      <c r="O67" s="130" t="s">
+      <c r="M67" s="114"/>
+      <c r="N67" s="114"/>
+      <c r="O67" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="P67" s="130"/>
-      <c r="Q67" s="130"/>
-      <c r="R67" s="127" t="s">
+      <c r="P67" s="114"/>
+      <c r="Q67" s="114"/>
+      <c r="R67" s="122" t="s">
         <v>87</v>
       </c>
-      <c r="S67" s="128"/>
-      <c r="T67" s="129"/>
-      <c r="U67" s="130" t="s">
+      <c r="S67" s="123"/>
+      <c r="T67" s="124"/>
+      <c r="U67" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="V67" s="130"/>
-      <c r="W67" s="130"/>
-      <c r="X67" s="130" t="s">
+      <c r="V67" s="114"/>
+      <c r="W67" s="114"/>
+      <c r="X67" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="Y67" s="130"/>
-      <c r="Z67" s="130"/>
-      <c r="AA67" s="130" t="s">
+      <c r="Y67" s="114"/>
+      <c r="Z67" s="114"/>
+      <c r="AA67" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="AB67" s="130"/>
-      <c r="AC67" s="130"/>
-      <c r="AD67" s="130" t="s">
+      <c r="AB67" s="114"/>
+      <c r="AC67" s="114"/>
+      <c r="AD67" s="114" t="s">
         <v>109</v>
       </c>
-      <c r="AE67" s="130"/>
-      <c r="AF67" s="130"/>
-      <c r="AG67" s="130" t="s">
+      <c r="AE67" s="114"/>
+      <c r="AF67" s="114"/>
+      <c r="AG67" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="AH67" s="130"/>
-      <c r="AI67" s="130"/>
-      <c r="AJ67" s="130" t="s">
+      <c r="AH67" s="114"/>
+      <c r="AI67" s="114"/>
+      <c r="AJ67" s="114" t="s">
         <v>13</v>
       </c>
-      <c r="AK67" s="130"/>
-      <c r="AL67" s="130"/>
-      <c r="AM67" s="130" t="s">
+      <c r="AK67" s="114"/>
+      <c r="AL67" s="114"/>
+      <c r="AM67" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="AN67" s="130"/>
-      <c r="AO67" s="130"/>
+      <c r="AN67" s="114"/>
+      <c r="AO67" s="114"/>
     </row>
     <row r="68" spans="1:41" ht="70">
-      <c r="A68" s="136" t="s">
+      <c r="A68" s="115" t="s">
         <v>128</v>
       </c>
-      <c r="B68" s="137"/>
+      <c r="B68" s="116"/>
       <c r="C68" s="86" t="s">
         <v>99</v>
       </c>
@@ -10368,8 +10384,8 @@
       </c>
     </row>
     <row r="69" spans="1:41" ht="16" thickBot="1">
-      <c r="A69" s="138"/>
-      <c r="B69" s="139"/>
+      <c r="A69" s="117"/>
+      <c r="B69" s="118"/>
       <c r="C69" s="86">
         <v>23</v>
       </c>
@@ -10489,10 +10505,10 @@
       </c>
     </row>
     <row r="70" spans="1:41" ht="16" thickTop="1">
-      <c r="A70" s="133" t="s">
+      <c r="A70" s="119" t="s">
         <v>125</v>
       </c>
-      <c r="B70" s="133"/>
+      <c r="B70" s="119"/>
       <c r="C70">
         <f xml:space="preserve"> C69/115</f>
         <v>0.2</v>
@@ -10651,10 +10667,10 @@
       </c>
     </row>
     <row r="71" spans="1:41">
-      <c r="A71" s="134" t="s">
+      <c r="A71" s="120" t="s">
         <v>124</v>
       </c>
-      <c r="B71" s="134"/>
+      <c r="B71" s="120"/>
       <c r="C71">
         <f xml:space="preserve"> C70*65</f>
         <v>13</v>
@@ -10813,10 +10829,10 @@
       </c>
     </row>
     <row r="72" spans="1:41">
-      <c r="A72" s="135" t="s">
+      <c r="A72" s="121" t="s">
         <v>126</v>
       </c>
-      <c r="B72" s="135"/>
+      <c r="B72" s="121"/>
       <c r="C72" s="80">
         <f xml:space="preserve"> 65-C71</f>
         <v>52</v>
@@ -10981,23 +10997,41 @@
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="AJ67:AL67"/>
-    <mergeCell ref="AM67:AO67"/>
-    <mergeCell ref="A68:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="AD67:AF67"/>
-    <mergeCell ref="AG67:AI67"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="R67:T67"/>
-    <mergeCell ref="U67:W67"/>
-    <mergeCell ref="X67:Z67"/>
-    <mergeCell ref="AA67:AC67"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="I67:K67"/>
-    <mergeCell ref="L67:N67"/>
-    <mergeCell ref="O67:Q67"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="A3:A56"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="R55:T55"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="C51:C53"/>
     <mergeCell ref="AM55:AO55"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A59:B59"/>
@@ -11014,41 +11048,23 @@
     <mergeCell ref="I55:K55"/>
     <mergeCell ref="L55:N55"/>
     <mergeCell ref="O55:Q55"/>
-    <mergeCell ref="R55:T55"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="B51:B53"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="A3:A56"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="R67:T67"/>
+    <mergeCell ref="U67:W67"/>
+    <mergeCell ref="X67:Z67"/>
+    <mergeCell ref="AA67:AC67"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="I67:K67"/>
+    <mergeCell ref="L67:N67"/>
+    <mergeCell ref="O67:Q67"/>
+    <mergeCell ref="AJ67:AL67"/>
+    <mergeCell ref="AM67:AO67"/>
+    <mergeCell ref="A68:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="AD67:AF67"/>
+    <mergeCell ref="AG67:AI67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -11065,8 +11081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Z39" sqref="Z39"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11092,37 +11108,37 @@
     <row r="1" spans="1:24" ht="34" customHeight="1">
       <c r="A1" s="57"/>
       <c r="B1" s="57"/>
-      <c r="C1" s="118" t="s">
+      <c r="C1" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="118" t="s">
+      <c r="D1" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="118" t="s">
+      <c r="E1" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="139" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="119" t="s">
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="134" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
-      <c r="N1" s="119"/>
-      <c r="O1" s="114" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="114"/>
-      <c r="Q1" s="119" t="s">
+      <c r="L1" s="134"/>
+      <c r="M1" s="134"/>
+      <c r="N1" s="134"/>
+      <c r="O1" s="135" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="135"/>
+      <c r="Q1" s="134" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="119"/>
-      <c r="S1" s="119"/>
+      <c r="R1" s="134"/>
+      <c r="S1" s="134"/>
       <c r="T1" s="71" t="s">
         <v>92</v>
       </c>
@@ -11135,16 +11151,16 @@
       <c r="W1" s="71" t="s">
         <v>133</v>
       </c>
-      <c r="X1" s="118" t="s">
+      <c r="X1" s="130" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="144">
       <c r="A2" s="57"/>
       <c r="B2" s="57"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -11199,16 +11215,16 @@
       <c r="W2" s="72" t="s">
         <v>98</v>
       </c>
-      <c r="X2" s="118"/>
+      <c r="X2" s="130"/>
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="136" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="115">
-        <v>1</v>
-      </c>
-      <c r="C3" s="118" t="s">
+      <c r="B3" s="127">
+        <v>1</v>
+      </c>
+      <c r="C3" s="130" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="54">
@@ -11276,9 +11292,9 @@
       </c>
     </row>
     <row r="4" spans="1:24">
-      <c r="A4" s="121"/>
-      <c r="B4" s="116"/>
-      <c r="C4" s="118"/>
+      <c r="A4" s="137"/>
+      <c r="B4" s="128"/>
+      <c r="C4" s="130"/>
       <c r="D4" s="54">
         <v>2010</v>
       </c>
@@ -11344,9 +11360,9 @@
       </c>
     </row>
     <row r="5" spans="1:24">
-      <c r="A5" s="121"/>
-      <c r="B5" s="117"/>
-      <c r="C5" s="118"/>
+      <c r="A5" s="137"/>
+      <c r="B5" s="129"/>
+      <c r="C5" s="130"/>
       <c r="D5" s="25">
         <v>2014</v>
       </c>
@@ -11412,11 +11428,11 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="15" customHeight="1">
-      <c r="A6" s="121"/>
-      <c r="B6" s="115">
+      <c r="A6" s="137"/>
+      <c r="B6" s="127">
         <v>2</v>
       </c>
-      <c r="C6" s="118" t="s">
+      <c r="C6" s="130" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="54">
@@ -11484,9 +11500,9 @@
       </c>
     </row>
     <row r="7" spans="1:24">
-      <c r="A7" s="121"/>
-      <c r="B7" s="116"/>
-      <c r="C7" s="118"/>
+      <c r="A7" s="137"/>
+      <c r="B7" s="128"/>
+      <c r="C7" s="130"/>
       <c r="D7" s="54">
         <v>2010</v>
       </c>
@@ -11552,9 +11568,9 @@
       </c>
     </row>
     <row r="8" spans="1:24">
-      <c r="A8" s="121"/>
-      <c r="B8" s="117"/>
-      <c r="C8" s="118"/>
+      <c r="A8" s="137"/>
+      <c r="B8" s="129"/>
+      <c r="C8" s="130"/>
       <c r="D8" s="25">
         <v>2014</v>
       </c>
@@ -11620,11 +11636,11 @@
       </c>
     </row>
     <row r="9" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A9" s="121"/>
-      <c r="B9" s="115">
+      <c r="A9" s="137"/>
+      <c r="B9" s="127">
         <v>3</v>
       </c>
-      <c r="C9" s="118" t="s">
+      <c r="C9" s="130" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="54">
@@ -11692,9 +11708,9 @@
       </c>
     </row>
     <row r="10" spans="1:24">
-      <c r="A10" s="121"/>
-      <c r="B10" s="116"/>
-      <c r="C10" s="118"/>
+      <c r="A10" s="137"/>
+      <c r="B10" s="128"/>
+      <c r="C10" s="130"/>
       <c r="D10" s="54">
         <v>2010</v>
       </c>
@@ -11760,9 +11776,9 @@
       </c>
     </row>
     <row r="11" spans="1:24">
-      <c r="A11" s="121"/>
-      <c r="B11" s="117"/>
-      <c r="C11" s="118"/>
+      <c r="A11" s="137"/>
+      <c r="B11" s="129"/>
+      <c r="C11" s="130"/>
       <c r="D11" s="25">
         <v>2014</v>
       </c>
@@ -11828,11 +11844,11 @@
       </c>
     </row>
     <row r="12" spans="1:24">
-      <c r="A12" s="121"/>
-      <c r="B12" s="115">
+      <c r="A12" s="137"/>
+      <c r="B12" s="127">
         <v>4</v>
       </c>
-      <c r="C12" s="118" t="s">
+      <c r="C12" s="130" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="54">
@@ -11900,9 +11916,9 @@
       </c>
     </row>
     <row r="13" spans="1:24">
-      <c r="A13" s="121"/>
-      <c r="B13" s="116"/>
-      <c r="C13" s="118"/>
+      <c r="A13" s="137"/>
+      <c r="B13" s="128"/>
+      <c r="C13" s="130"/>
       <c r="D13" s="54">
         <v>2010</v>
       </c>
@@ -11968,9 +11984,9 @@
       </c>
     </row>
     <row r="14" spans="1:24">
-      <c r="A14" s="121"/>
-      <c r="B14" s="117"/>
-      <c r="C14" s="118"/>
+      <c r="A14" s="137"/>
+      <c r="B14" s="129"/>
+      <c r="C14" s="130"/>
       <c r="D14" s="25">
         <v>2014</v>
       </c>
@@ -12036,11 +12052,11 @@
       </c>
     </row>
     <row r="15" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A15" s="121"/>
-      <c r="B15" s="115">
+      <c r="A15" s="137"/>
+      <c r="B15" s="127">
         <v>5</v>
       </c>
-      <c r="C15" s="118" t="s">
+      <c r="C15" s="130" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="54">
@@ -12108,9 +12124,9 @@
       </c>
     </row>
     <row r="16" spans="1:24">
-      <c r="A16" s="121"/>
-      <c r="B16" s="116"/>
-      <c r="C16" s="118"/>
+      <c r="A16" s="137"/>
+      <c r="B16" s="128"/>
+      <c r="C16" s="130"/>
       <c r="D16" s="54">
         <v>2010</v>
       </c>
@@ -12176,9 +12192,9 @@
       </c>
     </row>
     <row r="17" spans="1:24">
-      <c r="A17" s="121"/>
-      <c r="B17" s="117"/>
-      <c r="C17" s="118"/>
+      <c r="A17" s="137"/>
+      <c r="B17" s="129"/>
+      <c r="C17" s="130"/>
       <c r="D17" s="25">
         <v>2014</v>
       </c>
@@ -12244,11 +12260,11 @@
       </c>
     </row>
     <row r="18" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A18" s="121"/>
-      <c r="B18" s="115">
+      <c r="A18" s="137"/>
+      <c r="B18" s="127">
         <v>6</v>
       </c>
-      <c r="C18" s="118" t="s">
+      <c r="C18" s="130" t="s">
         <v>25</v>
       </c>
       <c r="D18" s="54">
@@ -12316,9 +12332,9 @@
       </c>
     </row>
     <row r="19" spans="1:24">
-      <c r="A19" s="121"/>
-      <c r="B19" s="116"/>
-      <c r="C19" s="118"/>
+      <c r="A19" s="137"/>
+      <c r="B19" s="128"/>
+      <c r="C19" s="130"/>
       <c r="D19" s="54">
         <v>2010</v>
       </c>
@@ -12384,9 +12400,9 @@
       </c>
     </row>
     <row r="20" spans="1:24">
-      <c r="A20" s="121"/>
-      <c r="B20" s="117"/>
-      <c r="C20" s="118"/>
+      <c r="A20" s="137"/>
+      <c r="B20" s="129"/>
+      <c r="C20" s="130"/>
       <c r="D20" s="25">
         <v>2014</v>
       </c>
@@ -12452,11 +12468,11 @@
       </c>
     </row>
     <row r="21" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A21" s="121"/>
-      <c r="B21" s="115">
+      <c r="A21" s="137"/>
+      <c r="B21" s="127">
         <v>7</v>
       </c>
-      <c r="C21" s="118" t="s">
+      <c r="C21" s="130" t="s">
         <v>70</v>
       </c>
       <c r="D21" s="54">
@@ -12524,9 +12540,9 @@
       </c>
     </row>
     <row r="22" spans="1:24">
-      <c r="A22" s="121"/>
-      <c r="B22" s="116"/>
-      <c r="C22" s="118"/>
+      <c r="A22" s="137"/>
+      <c r="B22" s="128"/>
+      <c r="C22" s="130"/>
       <c r="D22" s="54">
         <v>2010</v>
       </c>
@@ -12592,9 +12608,9 @@
       </c>
     </row>
     <row r="23" spans="1:24">
-      <c r="A23" s="121"/>
-      <c r="B23" s="117"/>
-      <c r="C23" s="118"/>
+      <c r="A23" s="137"/>
+      <c r="B23" s="129"/>
+      <c r="C23" s="130"/>
       <c r="D23" s="25">
         <v>2014</v>
       </c>
@@ -12660,11 +12676,11 @@
       </c>
     </row>
     <row r="24" spans="1:24">
-      <c r="A24" s="121"/>
-      <c r="B24" s="115">
+      <c r="A24" s="137"/>
+      <c r="B24" s="127">
         <v>8</v>
       </c>
-      <c r="C24" s="124" t="s">
+      <c r="C24" s="131" t="s">
         <v>54</v>
       </c>
       <c r="D24" s="54">
@@ -12732,9 +12748,9 @@
       </c>
     </row>
     <row r="25" spans="1:24">
-      <c r="A25" s="121"/>
-      <c r="B25" s="116"/>
-      <c r="C25" s="125"/>
+      <c r="A25" s="137"/>
+      <c r="B25" s="128"/>
+      <c r="C25" s="132"/>
       <c r="D25" s="54">
         <v>2010</v>
       </c>
@@ -12800,9 +12816,9 @@
       </c>
     </row>
     <row r="26" spans="1:24">
-      <c r="A26" s="121"/>
-      <c r="B26" s="117"/>
-      <c r="C26" s="126"/>
+      <c r="A26" s="137"/>
+      <c r="B26" s="129"/>
+      <c r="C26" s="133"/>
       <c r="D26" s="25">
         <v>2014</v>
       </c>
@@ -12868,11 +12884,11 @@
       </c>
     </row>
     <row r="27" spans="1:24">
-      <c r="A27" s="121"/>
-      <c r="B27" s="115">
+      <c r="A27" s="137"/>
+      <c r="B27" s="127">
         <v>9</v>
       </c>
-      <c r="C27" s="118" t="s">
+      <c r="C27" s="130" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="54">
@@ -12940,9 +12956,9 @@
       </c>
     </row>
     <row r="28" spans="1:24">
-      <c r="A28" s="121"/>
-      <c r="B28" s="116"/>
-      <c r="C28" s="118"/>
+      <c r="A28" s="137"/>
+      <c r="B28" s="128"/>
+      <c r="C28" s="130"/>
       <c r="D28" s="54">
         <v>2010</v>
       </c>
@@ -13008,9 +13024,9 @@
       </c>
     </row>
     <row r="29" spans="1:24">
-      <c r="A29" s="121"/>
-      <c r="B29" s="117"/>
-      <c r="C29" s="118"/>
+      <c r="A29" s="137"/>
+      <c r="B29" s="129"/>
+      <c r="C29" s="130"/>
       <c r="D29" s="25">
         <v>2014</v>
       </c>
@@ -13076,11 +13092,11 @@
       </c>
     </row>
     <row r="30" spans="1:24">
-      <c r="A30" s="121"/>
-      <c r="B30" s="115">
+      <c r="A30" s="137"/>
+      <c r="B30" s="127">
         <v>10</v>
       </c>
-      <c r="C30" s="118" t="s">
+      <c r="C30" s="130" t="s">
         <v>28</v>
       </c>
       <c r="D30" s="54">
@@ -13148,9 +13164,9 @@
       </c>
     </row>
     <row r="31" spans="1:24">
-      <c r="A31" s="121"/>
-      <c r="B31" s="116"/>
-      <c r="C31" s="118"/>
+      <c r="A31" s="137"/>
+      <c r="B31" s="128"/>
+      <c r="C31" s="130"/>
       <c r="D31" s="54">
         <v>2010</v>
       </c>
@@ -13216,9 +13232,9 @@
       </c>
     </row>
     <row r="32" spans="1:24">
-      <c r="A32" s="121"/>
-      <c r="B32" s="117"/>
-      <c r="C32" s="118"/>
+      <c r="A32" s="137"/>
+      <c r="B32" s="129"/>
+      <c r="C32" s="130"/>
       <c r="D32" s="25">
         <v>2014</v>
       </c>
@@ -13284,11 +13300,11 @@
       </c>
     </row>
     <row r="33" spans="1:41">
-      <c r="A33" s="121"/>
-      <c r="B33" s="115">
+      <c r="A33" s="137"/>
+      <c r="B33" s="127">
         <v>11</v>
       </c>
-      <c r="C33" s="118" t="s">
+      <c r="C33" s="130" t="s">
         <v>21</v>
       </c>
       <c r="D33" s="54">
@@ -13356,9 +13372,9 @@
       </c>
     </row>
     <row r="34" spans="1:41">
-      <c r="A34" s="121"/>
-      <c r="B34" s="116"/>
-      <c r="C34" s="118"/>
+      <c r="A34" s="137"/>
+      <c r="B34" s="128"/>
+      <c r="C34" s="130"/>
       <c r="D34" s="54">
         <v>2010</v>
       </c>
@@ -13424,9 +13440,9 @@
       </c>
     </row>
     <row r="35" spans="1:41">
-      <c r="A35" s="121"/>
-      <c r="B35" s="117"/>
-      <c r="C35" s="118"/>
+      <c r="A35" s="137"/>
+      <c r="B35" s="129"/>
+      <c r="C35" s="130"/>
       <c r="D35" s="25">
         <v>2014</v>
       </c>
@@ -13492,11 +13508,11 @@
       </c>
     </row>
     <row r="36" spans="1:41">
-      <c r="A36" s="121"/>
-      <c r="B36" s="115">
+      <c r="A36" s="137"/>
+      <c r="B36" s="127">
         <v>12</v>
       </c>
-      <c r="C36" s="118" t="s">
+      <c r="C36" s="130" t="s">
         <v>13</v>
       </c>
       <c r="D36" s="54">
@@ -13564,9 +13580,9 @@
       </c>
     </row>
     <row r="37" spans="1:41">
-      <c r="A37" s="121"/>
-      <c r="B37" s="116"/>
-      <c r="C37" s="118"/>
+      <c r="A37" s="137"/>
+      <c r="B37" s="128"/>
+      <c r="C37" s="130"/>
       <c r="D37" s="54">
         <v>2010</v>
       </c>
@@ -13632,9 +13648,9 @@
       </c>
     </row>
     <row r="38" spans="1:41">
-      <c r="A38" s="121"/>
-      <c r="B38" s="117"/>
-      <c r="C38" s="118"/>
+      <c r="A38" s="137"/>
+      <c r="B38" s="129"/>
+      <c r="C38" s="130"/>
       <c r="D38" s="25">
         <v>2014</v>
       </c>
@@ -13700,11 +13716,11 @@
       </c>
     </row>
     <row r="39" spans="1:41">
-      <c r="A39" s="121"/>
-      <c r="B39" s="115">
+      <c r="A39" s="137"/>
+      <c r="B39" s="127">
         <v>13</v>
       </c>
-      <c r="C39" s="118" t="s">
+      <c r="C39" s="130" t="s">
         <v>8</v>
       </c>
       <c r="D39" s="54">
@@ -13772,9 +13788,9 @@
       </c>
     </row>
     <row r="40" spans="1:41">
-      <c r="A40" s="121"/>
-      <c r="B40" s="116"/>
-      <c r="C40" s="118"/>
+      <c r="A40" s="137"/>
+      <c r="B40" s="128"/>
+      <c r="C40" s="130"/>
       <c r="D40" s="54">
         <v>2010</v>
       </c>
@@ -13840,9 +13856,9 @@
       </c>
     </row>
     <row r="41" spans="1:41">
-      <c r="A41" s="121"/>
-      <c r="B41" s="117"/>
-      <c r="C41" s="118"/>
+      <c r="A41" s="137"/>
+      <c r="B41" s="129"/>
+      <c r="C41" s="130"/>
       <c r="D41" s="25">
         <v>2014</v>
       </c>
@@ -13908,79 +13924,79 @@
       </c>
     </row>
     <row r="42" spans="1:41">
-      <c r="A42" s="121"/>
+      <c r="A42" s="137"/>
     </row>
     <row r="43" spans="1:41" s="75" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A43" s="121"/>
+      <c r="A43" s="137"/>
       <c r="B43" s="73"/>
-      <c r="C43" s="130" t="s">
+      <c r="C43" s="114" t="s">
         <v>50</v>
       </c>
-      <c r="D43" s="130"/>
-      <c r="E43" s="130"/>
-      <c r="F43" s="130" t="s">
+      <c r="D43" s="114"/>
+      <c r="E43" s="114"/>
+      <c r="F43" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="G43" s="130"/>
-      <c r="H43" s="130"/>
-      <c r="I43" s="130" t="s">
+      <c r="G43" s="114"/>
+      <c r="H43" s="114"/>
+      <c r="I43" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="J43" s="130"/>
-      <c r="K43" s="130"/>
-      <c r="L43" s="130" t="s">
+      <c r="J43" s="114"/>
+      <c r="K43" s="114"/>
+      <c r="L43" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="M43" s="130"/>
-      <c r="N43" s="130"/>
-      <c r="O43" s="130" t="s">
+      <c r="M43" s="114"/>
+      <c r="N43" s="114"/>
+      <c r="O43" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="P43" s="130"/>
-      <c r="Q43" s="130"/>
-      <c r="R43" s="127" t="s">
+      <c r="P43" s="114"/>
+      <c r="Q43" s="114"/>
+      <c r="R43" s="122" t="s">
         <v>87</v>
       </c>
-      <c r="S43" s="128"/>
-      <c r="T43" s="129"/>
-      <c r="U43" s="130" t="s">
+      <c r="S43" s="123"/>
+      <c r="T43" s="124"/>
+      <c r="U43" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="V43" s="130"/>
-      <c r="W43" s="130"/>
-      <c r="X43" s="127" t="s">
+      <c r="V43" s="114"/>
+      <c r="W43" s="114"/>
+      <c r="X43" s="122" t="s">
         <v>54</v>
       </c>
-      <c r="Y43" s="128"/>
-      <c r="Z43" s="129"/>
-      <c r="AA43" s="130" t="s">
+      <c r="Y43" s="123"/>
+      <c r="Z43" s="124"/>
+      <c r="AA43" s="114" t="s">
         <v>105</v>
       </c>
-      <c r="AB43" s="130"/>
-      <c r="AC43" s="130"/>
-      <c r="AD43" s="130" t="s">
+      <c r="AB43" s="114"/>
+      <c r="AC43" s="114"/>
+      <c r="AD43" s="114" t="s">
         <v>109</v>
       </c>
-      <c r="AE43" s="130"/>
-      <c r="AF43" s="130"/>
-      <c r="AG43" s="130" t="s">
+      <c r="AE43" s="114"/>
+      <c r="AF43" s="114"/>
+      <c r="AG43" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="AH43" s="130"/>
-      <c r="AI43" s="130"/>
-      <c r="AJ43" s="130" t="s">
+      <c r="AH43" s="114"/>
+      <c r="AI43" s="114"/>
+      <c r="AJ43" s="114" t="s">
         <v>13</v>
       </c>
-      <c r="AK43" s="130"/>
-      <c r="AL43" s="130"/>
-      <c r="AM43" s="130" t="s">
+      <c r="AK43" s="114"/>
+      <c r="AL43" s="114"/>
+      <c r="AM43" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="AN43" s="130"/>
-      <c r="AO43" s="130"/>
+      <c r="AN43" s="114"/>
+      <c r="AO43" s="114"/>
     </row>
     <row r="44" spans="1:41" s="75" customFormat="1" ht="70">
-      <c r="A44" s="122"/>
+      <c r="A44" s="138"/>
       <c r="B44" s="73"/>
       <c r="C44" s="73" t="s">
         <v>72</v>
@@ -14221,10 +14237,10 @@
       </c>
     </row>
     <row r="46" spans="1:41" s="79" customFormat="1" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A46" s="131" t="s">
+      <c r="A46" s="125" t="s">
         <v>129</v>
       </c>
-      <c r="B46" s="132"/>
+      <c r="B46" s="126"/>
       <c r="C46" s="79">
         <v>2006</v>
       </c>
@@ -14261,10 +14277,10 @@
       <c r="Y46" s="105"/>
     </row>
     <row r="47" spans="1:41" ht="16" thickTop="1">
-      <c r="A47" s="133" t="s">
+      <c r="A47" s="119" t="s">
         <v>125</v>
       </c>
-      <c r="B47" s="133"/>
+      <c r="B47" s="119"/>
       <c r="C47">
         <f xml:space="preserve"> C45/115</f>
         <v>3.4782608695652174E-2</v>
@@ -14423,10 +14439,10 @@
       </c>
     </row>
     <row r="48" spans="1:41">
-      <c r="A48" s="134" t="s">
+      <c r="A48" s="120" t="s">
         <v>124</v>
       </c>
-      <c r="B48" s="134"/>
+      <c r="B48" s="120"/>
       <c r="C48">
         <f xml:space="preserve"> C47*72</f>
         <v>2.5043478260869567</v>
@@ -14585,10 +14601,10 @@
       </c>
     </row>
     <row r="49" spans="1:41" s="80" customFormat="1">
-      <c r="A49" s="135" t="s">
+      <c r="A49" s="121" t="s">
         <v>126</v>
       </c>
-      <c r="B49" s="135"/>
+      <c r="B49" s="121"/>
       <c r="C49" s="80">
         <f xml:space="preserve"> 72-C48</f>
         <v>69.495652173913044</v>
@@ -14898,77 +14914,77 @@
       <c r="X54" s="85"/>
     </row>
     <row r="55" spans="1:41">
-      <c r="C55" s="130" t="s">
+      <c r="C55" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="D55" s="130"/>
-      <c r="E55" s="130"/>
-      <c r="F55" s="127" t="s">
+      <c r="D55" s="114"/>
+      <c r="E55" s="114"/>
+      <c r="F55" s="122" t="s">
         <v>54</v>
       </c>
-      <c r="G55" s="128"/>
-      <c r="H55" s="129"/>
-      <c r="I55" s="130" t="s">
+      <c r="G55" s="123"/>
+      <c r="H55" s="124"/>
+      <c r="I55" s="114" t="s">
         <v>105</v>
       </c>
-      <c r="J55" s="130"/>
-      <c r="K55" s="130"/>
-      <c r="L55" s="130" t="s">
+      <c r="J55" s="114"/>
+      <c r="K55" s="114"/>
+      <c r="L55" s="114" t="s">
         <v>50</v>
       </c>
-      <c r="M55" s="130"/>
-      <c r="N55" s="130"/>
-      <c r="O55" s="130" t="s">
+      <c r="M55" s="114"/>
+      <c r="N55" s="114"/>
+      <c r="O55" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="P55" s="130"/>
-      <c r="Q55" s="130"/>
-      <c r="R55" s="127" t="s">
+      <c r="P55" s="114"/>
+      <c r="Q55" s="114"/>
+      <c r="R55" s="122" t="s">
         <v>87</v>
       </c>
-      <c r="S55" s="128"/>
-      <c r="T55" s="129"/>
-      <c r="U55" s="130" t="s">
+      <c r="S55" s="123"/>
+      <c r="T55" s="124"/>
+      <c r="U55" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="V55" s="130"/>
-      <c r="W55" s="130"/>
-      <c r="X55" s="130" t="s">
+      <c r="V55" s="114"/>
+      <c r="W55" s="114"/>
+      <c r="X55" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="Y55" s="130"/>
-      <c r="Z55" s="130"/>
-      <c r="AA55" s="130" t="s">
+      <c r="Y55" s="114"/>
+      <c r="Z55" s="114"/>
+      <c r="AA55" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="AB55" s="130"/>
-      <c r="AC55" s="130"/>
-      <c r="AD55" s="130" t="s">
+      <c r="AB55" s="114"/>
+      <c r="AC55" s="114"/>
+      <c r="AD55" s="114" t="s">
         <v>109</v>
       </c>
-      <c r="AE55" s="130"/>
-      <c r="AF55" s="130"/>
-      <c r="AG55" s="130" t="s">
+      <c r="AE55" s="114"/>
+      <c r="AF55" s="114"/>
+      <c r="AG55" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="AH55" s="130"/>
-      <c r="AI55" s="130"/>
-      <c r="AJ55" s="130" t="s">
+      <c r="AH55" s="114"/>
+      <c r="AI55" s="114"/>
+      <c r="AJ55" s="114" t="s">
         <v>13</v>
       </c>
-      <c r="AK55" s="130"/>
-      <c r="AL55" s="130"/>
-      <c r="AM55" s="130" t="s">
+      <c r="AK55" s="114"/>
+      <c r="AL55" s="114"/>
+      <c r="AM55" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="AN55" s="130"/>
-      <c r="AO55" s="130"/>
+      <c r="AN55" s="114"/>
+      <c r="AO55" s="114"/>
     </row>
     <row r="56" spans="1:41" ht="70">
-      <c r="A56" s="136" t="s">
+      <c r="A56" s="115" t="s">
         <v>128</v>
       </c>
-      <c r="B56" s="137"/>
+      <c r="B56" s="116"/>
       <c r="C56" s="74" t="s">
         <v>99</v>
       </c>
@@ -15088,8 +15104,8 @@
       </c>
     </row>
     <row r="57" spans="1:41" ht="16" thickBot="1">
-      <c r="A57" s="138"/>
-      <c r="B57" s="139"/>
+      <c r="A57" s="117"/>
+      <c r="B57" s="118"/>
       <c r="C57" s="74">
         <v>23</v>
       </c>
@@ -15209,10 +15225,10 @@
       </c>
     </row>
     <row r="58" spans="1:41" ht="16" thickTop="1">
-      <c r="A58" s="133" t="s">
+      <c r="A58" s="119" t="s">
         <v>125</v>
       </c>
-      <c r="B58" s="133"/>
+      <c r="B58" s="119"/>
       <c r="C58">
         <f xml:space="preserve"> C57/115</f>
         <v>0.2</v>
@@ -15371,10 +15387,10 @@
       </c>
     </row>
     <row r="59" spans="1:41">
-      <c r="A59" s="134" t="s">
+      <c r="A59" s="120" t="s">
         <v>124</v>
       </c>
-      <c r="B59" s="134"/>
+      <c r="B59" s="120"/>
       <c r="C59">
         <f xml:space="preserve"> C58*65</f>
         <v>13</v>
@@ -15533,10 +15549,10 @@
       </c>
     </row>
     <row r="60" spans="1:41">
-      <c r="A60" s="135" t="s">
+      <c r="A60" s="121" t="s">
         <v>126</v>
       </c>
-      <c r="B60" s="135"/>
+      <c r="B60" s="121"/>
       <c r="C60" s="80">
         <f xml:space="preserve"> 65-C59</f>
         <v>52</v>
@@ -15701,6 +15717,59 @@
     </row>
   </sheetData>
   <mergeCells count="69">
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="L43:N43"/>
+    <mergeCell ref="O43:Q43"/>
+    <mergeCell ref="U43:W43"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="A3:A44"/>
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="AD43:AF43"/>
+    <mergeCell ref="AG43:AI43"/>
+    <mergeCell ref="AJ43:AL43"/>
+    <mergeCell ref="AM43:AO43"/>
+    <mergeCell ref="X43:Z43"/>
+    <mergeCell ref="AA43:AC43"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="AM55:AO55"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="AD55:AF55"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="B9:B11"/>
     <mergeCell ref="A60:B60"/>
     <mergeCell ref="A56:B57"/>
     <mergeCell ref="A46:B46"/>
@@ -15717,59 +15786,6 @@
     <mergeCell ref="I55:K55"/>
     <mergeCell ref="L55:N55"/>
     <mergeCell ref="R55:T55"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="AM55:AO55"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="AD55:AF55"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="AD43:AF43"/>
-    <mergeCell ref="AG43:AI43"/>
-    <mergeCell ref="AJ43:AL43"/>
-    <mergeCell ref="AM43:AO43"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="L43:N43"/>
-    <mergeCell ref="O43:Q43"/>
-    <mergeCell ref="U43:W43"/>
-    <mergeCell ref="X43:Z43"/>
-    <mergeCell ref="AA43:AC43"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="A3:A44"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -15799,44 +15815,44 @@
     <row r="1" spans="1:19">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="118" t="s">
+      <c r="C1" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="118" t="s">
+      <c r="D1" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="118" t="s">
+      <c r="E1" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="139" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="119" t="s">
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="134" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
-      <c r="N1" s="119"/>
-      <c r="O1" s="114" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="114"/>
-      <c r="Q1" s="119" t="s">
+      <c r="L1" s="134"/>
+      <c r="M1" s="134"/>
+      <c r="N1" s="134"/>
+      <c r="O1" s="135" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="135"/>
+      <c r="Q1" s="134" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="119"/>
-      <c r="S1" s="119"/>
+      <c r="R1" s="134"/>
+      <c r="S1" s="134"/>
     </row>
     <row r="2" spans="1:19" ht="84">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -15881,7 +15897,7 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="136" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="47" t="s">
@@ -15940,7 +15956,7 @@
       </c>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="121"/>
+      <c r="A4" s="137"/>
       <c r="B4" s="45" t="s">
         <v>55</v>
       </c>
@@ -15997,7 +16013,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A5" s="121"/>
+      <c r="A5" s="137"/>
       <c r="B5" s="45" t="s">
         <v>57</v>
       </c>
@@ -16054,7 +16070,7 @@
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="121"/>
+      <c r="A6" s="137"/>
       <c r="B6" s="45" t="s">
         <v>58</v>
       </c>
@@ -16111,7 +16127,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A7" s="121"/>
+      <c r="A7" s="137"/>
       <c r="B7" s="45" t="s">
         <v>59</v>
       </c>
@@ -16168,7 +16184,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A8" s="121"/>
+      <c r="A8" s="137"/>
       <c r="B8" s="45" t="s">
         <v>60</v>
       </c>
@@ -16225,7 +16241,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A9" s="121"/>
+      <c r="A9" s="137"/>
       <c r="B9" s="45" t="s">
         <v>61</v>
       </c>
@@ -16282,7 +16298,7 @@
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="121"/>
+      <c r="A10" s="137"/>
       <c r="B10" s="45" t="s">
         <v>62</v>
       </c>
@@ -16339,7 +16355,7 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="121"/>
+      <c r="A11" s="137"/>
       <c r="B11" s="45" t="s">
         <v>56</v>
       </c>
@@ -16396,7 +16412,7 @@
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="121"/>
+      <c r="A12" s="137"/>
       <c r="B12" s="45" t="s">
         <v>63</v>
       </c>
@@ -16453,7 +16469,7 @@
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="121"/>
+      <c r="A13" s="137"/>
       <c r="B13" s="45" t="s">
         <v>64</v>
       </c>
@@ -16510,7 +16526,7 @@
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="121"/>
+      <c r="A14" s="137"/>
       <c r="B14" s="45" t="s">
         <v>65</v>
       </c>
@@ -16567,7 +16583,7 @@
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="121"/>
+      <c r="A15" s="137"/>
       <c r="B15" s="45" t="s">
         <v>66</v>
       </c>
@@ -17329,44 +17345,44 @@
     <row r="1" spans="1:19">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="118" t="s">
+      <c r="C1" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="118" t="s">
+      <c r="D1" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="118" t="s">
+      <c r="E1" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="139" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="119" t="s">
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="134" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
-      <c r="N1" s="119"/>
-      <c r="O1" s="114" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="114"/>
-      <c r="Q1" s="119" t="s">
+      <c r="L1" s="134"/>
+      <c r="M1" s="134"/>
+      <c r="N1" s="134"/>
+      <c r="O1" s="135" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="135"/>
+      <c r="Q1" s="134" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="119"/>
-      <c r="S1" s="119"/>
+      <c r="R1" s="134"/>
+      <c r="S1" s="134"/>
     </row>
     <row r="2" spans="1:19" ht="84">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -17411,7 +17427,7 @@
       </c>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="136" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="44" t="s">
@@ -17470,7 +17486,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="24">
-      <c r="A4" s="121"/>
+      <c r="A4" s="137"/>
       <c r="B4" s="45" t="s">
         <v>55</v>
       </c>
@@ -17527,7 +17543,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="25.5" customHeight="1">
-      <c r="A5" s="121"/>
+      <c r="A5" s="137"/>
       <c r="B5" s="45" t="s">
         <v>57</v>
       </c>
@@ -17584,7 +17600,7 @@
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="121"/>
+      <c r="A6" s="137"/>
       <c r="B6" s="45" t="s">
         <v>58</v>
       </c>
@@ -17641,7 +17657,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="25.5" customHeight="1">
-      <c r="A7" s="121"/>
+      <c r="A7" s="137"/>
       <c r="B7" s="45" t="s">
         <v>59</v>
       </c>
@@ -17698,7 +17714,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="24">
-      <c r="A8" s="121"/>
+      <c r="A8" s="137"/>
       <c r="B8" s="45" t="s">
         <v>60</v>
       </c>
@@ -17755,7 +17771,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="25.5" customHeight="1">
-      <c r="A9" s="121"/>
+      <c r="A9" s="137"/>
       <c r="B9" s="45" t="s">
         <v>61</v>
       </c>
@@ -17812,7 +17828,7 @@
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="121"/>
+      <c r="A10" s="137"/>
       <c r="B10" s="45" t="s">
         <v>62</v>
       </c>
@@ -17869,7 +17885,7 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="121"/>
+      <c r="A11" s="137"/>
       <c r="B11" s="45" t="s">
         <v>56</v>
       </c>
@@ -17926,7 +17942,7 @@
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="121"/>
+      <c r="A12" s="137"/>
       <c r="B12" s="45" t="s">
         <v>63</v>
       </c>
@@ -17983,7 +17999,7 @@
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="121"/>
+      <c r="A13" s="137"/>
       <c r="B13" s="45" t="s">
         <v>64</v>
       </c>
@@ -18040,7 +18056,7 @@
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="121"/>
+      <c r="A14" s="137"/>
       <c r="B14" s="45" t="s">
         <v>65</v>
       </c>
@@ -18097,7 +18113,7 @@
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="121"/>
+      <c r="A15" s="137"/>
       <c r="B15" s="45" t="s">
         <v>66</v>
       </c>
@@ -18911,44 +18927,44 @@
     <row r="1" spans="1:19">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="118" t="s">
+      <c r="C1" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="118" t="s">
+      <c r="D1" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="118" t="s">
+      <c r="E1" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="139" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="119" t="s">
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="134" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
-      <c r="N1" s="119"/>
-      <c r="O1" s="114" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="114"/>
-      <c r="Q1" s="119" t="s">
+      <c r="L1" s="134"/>
+      <c r="M1" s="134"/>
+      <c r="N1" s="134"/>
+      <c r="O1" s="135" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="135"/>
+      <c r="Q1" s="134" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="119"/>
-      <c r="S1" s="119"/>
+      <c r="R1" s="134"/>
+      <c r="S1" s="134"/>
     </row>
     <row r="2" spans="1:19" ht="84">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -18993,7 +19009,7 @@
       </c>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="136" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="44" t="s">
@@ -19052,7 +19068,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="24">
-      <c r="A4" s="121"/>
+      <c r="A4" s="137"/>
       <c r="B4" s="45" t="s">
         <v>55</v>
       </c>
@@ -19109,7 +19125,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="24">
-      <c r="A5" s="121"/>
+      <c r="A5" s="137"/>
       <c r="B5" s="45" t="s">
         <v>57</v>
       </c>
@@ -19166,7 +19182,7 @@
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="121"/>
+      <c r="A6" s="137"/>
       <c r="B6" s="45" t="s">
         <v>58</v>
       </c>
@@ -19223,7 +19239,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="24">
-      <c r="A7" s="121"/>
+      <c r="A7" s="137"/>
       <c r="B7" s="45" t="s">
         <v>59</v>
       </c>
@@ -19280,7 +19296,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="24">
-      <c r="A8" s="121"/>
+      <c r="A8" s="137"/>
       <c r="B8" s="45" t="s">
         <v>60</v>
       </c>
@@ -19337,7 +19353,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="24">
-      <c r="A9" s="121"/>
+      <c r="A9" s="137"/>
       <c r="B9" s="45" t="s">
         <v>61</v>
       </c>
@@ -19394,7 +19410,7 @@
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="121"/>
+      <c r="A10" s="137"/>
       <c r="B10" s="45" t="s">
         <v>62</v>
       </c>
@@ -19451,7 +19467,7 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="121"/>
+      <c r="A11" s="137"/>
       <c r="B11" s="45" t="s">
         <v>56</v>
       </c>
@@ -19508,7 +19524,7 @@
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="121"/>
+      <c r="A12" s="137"/>
       <c r="B12" s="45" t="s">
         <v>63</v>
       </c>
@@ -19565,7 +19581,7 @@
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="121"/>
+      <c r="A13" s="137"/>
       <c r="B13" s="45" t="s">
         <v>64</v>
       </c>
@@ -19622,7 +19638,7 @@
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="121"/>
+      <c r="A14" s="137"/>
       <c r="B14" s="45" t="s">
         <v>65</v>
       </c>
@@ -19679,7 +19695,7 @@
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="121"/>
+      <c r="A15" s="137"/>
       <c r="B15" s="45" t="s">
         <v>66</v>
       </c>
@@ -19813,158 +19829,158 @@
       <c r="K1" s="140"/>
     </row>
     <row r="2" spans="1:44" ht="20" customHeight="1">
-      <c r="C2" s="115">
-        <v>1</v>
-      </c>
-      <c r="D2" s="116"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="115">
+      <c r="C2" s="127">
+        <v>1</v>
+      </c>
+      <c r="D2" s="128"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="127">
         <v>2</v>
       </c>
-      <c r="G2" s="116"/>
-      <c r="H2" s="117"/>
-      <c r="I2" s="115">
+      <c r="G2" s="128"/>
+      <c r="H2" s="129"/>
+      <c r="I2" s="127">
         <v>3</v>
       </c>
-      <c r="J2" s="116"/>
-      <c r="K2" s="117"/>
-      <c r="L2" s="115">
+      <c r="J2" s="128"/>
+      <c r="K2" s="129"/>
+      <c r="L2" s="127">
         <v>4</v>
       </c>
-      <c r="M2" s="116"/>
-      <c r="N2" s="117"/>
-      <c r="O2" s="115">
+      <c r="M2" s="128"/>
+      <c r="N2" s="129"/>
+      <c r="O2" s="127">
         <v>5</v>
       </c>
-      <c r="P2" s="116"/>
-      <c r="Q2" s="117"/>
-      <c r="R2" s="115">
+      <c r="P2" s="128"/>
+      <c r="Q2" s="129"/>
+      <c r="R2" s="127">
         <v>6</v>
       </c>
-      <c r="S2" s="116"/>
-      <c r="T2" s="117"/>
-      <c r="U2" s="115">
+      <c r="S2" s="128"/>
+      <c r="T2" s="129"/>
+      <c r="U2" s="127">
         <v>7</v>
       </c>
-      <c r="V2" s="116"/>
-      <c r="W2" s="117"/>
-      <c r="X2" s="115">
+      <c r="V2" s="128"/>
+      <c r="W2" s="129"/>
+      <c r="X2" s="127">
         <v>8</v>
       </c>
-      <c r="Y2" s="116"/>
-      <c r="Z2" s="117"/>
-      <c r="AA2" s="115">
+      <c r="Y2" s="128"/>
+      <c r="Z2" s="129"/>
+      <c r="AA2" s="127">
         <v>14</v>
       </c>
-      <c r="AB2" s="116"/>
-      <c r="AC2" s="117"/>
-      <c r="AD2" s="115">
+      <c r="AB2" s="128"/>
+      <c r="AC2" s="129"/>
+      <c r="AD2" s="127">
         <v>9</v>
       </c>
-      <c r="AE2" s="116"/>
-      <c r="AF2" s="117"/>
-      <c r="AG2" s="115">
+      <c r="AE2" s="128"/>
+      <c r="AF2" s="129"/>
+      <c r="AG2" s="127">
         <v>10</v>
       </c>
-      <c r="AH2" s="116"/>
-      <c r="AI2" s="117"/>
-      <c r="AJ2" s="115">
+      <c r="AH2" s="128"/>
+      <c r="AI2" s="129"/>
+      <c r="AJ2" s="127">
         <v>11</v>
       </c>
-      <c r="AK2" s="116"/>
-      <c r="AL2" s="117"/>
-      <c r="AM2" s="115">
+      <c r="AK2" s="128"/>
+      <c r="AL2" s="129"/>
+      <c r="AM2" s="127">
         <v>12</v>
       </c>
-      <c r="AN2" s="116"/>
-      <c r="AO2" s="117"/>
-      <c r="AP2" s="115">
+      <c r="AN2" s="128"/>
+      <c r="AO2" s="129"/>
+      <c r="AP2" s="127">
         <v>13</v>
       </c>
-      <c r="AQ2" s="116"/>
-      <c r="AR2" s="117"/>
+      <c r="AQ2" s="128"/>
+      <c r="AR2" s="129"/>
     </row>
     <row r="3" spans="1:44" s="14" customFormat="1" ht="20" customHeight="1">
-      <c r="A3" s="118" t="s">
+      <c r="A3" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="118"/>
-      <c r="C3" s="118" t="s">
+      <c r="B3" s="130"/>
+      <c r="C3" s="130" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="118"/>
-      <c r="E3" s="118"/>
-      <c r="F3" s="118" t="s">
+      <c r="D3" s="130"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="118"/>
-      <c r="H3" s="118"/>
-      <c r="I3" s="118" t="s">
+      <c r="G3" s="130"/>
+      <c r="H3" s="130"/>
+      <c r="I3" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="118"/>
-      <c r="K3" s="118"/>
-      <c r="L3" s="118" t="s">
+      <c r="J3" s="130"/>
+      <c r="K3" s="130"/>
+      <c r="L3" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="118"/>
-      <c r="N3" s="118"/>
-      <c r="O3" s="118" t="s">
+      <c r="M3" s="130"/>
+      <c r="N3" s="130"/>
+      <c r="O3" s="130" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="118"/>
-      <c r="Q3" s="118"/>
-      <c r="R3" s="118" t="s">
+      <c r="P3" s="130"/>
+      <c r="Q3" s="130"/>
+      <c r="R3" s="130" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="118"/>
-      <c r="T3" s="118"/>
-      <c r="U3" s="118" t="s">
+      <c r="S3" s="130"/>
+      <c r="T3" s="130"/>
+      <c r="U3" s="130" t="s">
         <v>15</v>
       </c>
-      <c r="V3" s="118"/>
-      <c r="W3" s="118"/>
-      <c r="X3" s="118" t="s">
+      <c r="V3" s="130"/>
+      <c r="W3" s="130"/>
+      <c r="X3" s="130" t="s">
         <v>6</v>
       </c>
-      <c r="Y3" s="118"/>
-      <c r="Z3" s="118"/>
-      <c r="AA3" s="124" t="s">
+      <c r="Y3" s="130"/>
+      <c r="Z3" s="130"/>
+      <c r="AA3" s="131" t="s">
         <v>54</v>
       </c>
-      <c r="AB3" s="125"/>
-      <c r="AC3" s="126"/>
-      <c r="AD3" s="118" t="s">
+      <c r="AB3" s="132"/>
+      <c r="AC3" s="133"/>
+      <c r="AD3" s="130" t="s">
         <v>30</v>
       </c>
-      <c r="AE3" s="118"/>
-      <c r="AF3" s="118"/>
-      <c r="AG3" s="118" t="s">
+      <c r="AE3" s="130"/>
+      <c r="AF3" s="130"/>
+      <c r="AG3" s="130" t="s">
         <v>31</v>
       </c>
-      <c r="AH3" s="118"/>
-      <c r="AI3" s="118"/>
-      <c r="AJ3" s="118" t="s">
+      <c r="AH3" s="130"/>
+      <c r="AI3" s="130"/>
+      <c r="AJ3" s="130" t="s">
         <v>21</v>
       </c>
-      <c r="AK3" s="118"/>
-      <c r="AL3" s="118"/>
-      <c r="AM3" s="118" t="s">
+      <c r="AK3" s="130"/>
+      <c r="AL3" s="130"/>
+      <c r="AM3" s="130" t="s">
         <v>13</v>
       </c>
-      <c r="AN3" s="118"/>
-      <c r="AO3" s="118"/>
-      <c r="AP3" s="118" t="s">
+      <c r="AN3" s="130"/>
+      <c r="AO3" s="130"/>
+      <c r="AP3" s="130" t="s">
         <v>8</v>
       </c>
-      <c r="AQ3" s="118"/>
-      <c r="AR3" s="118"/>
+      <c r="AQ3" s="130"/>
+      <c r="AR3" s="130"/>
     </row>
     <row r="4" spans="1:44" s="14" customFormat="1" ht="20" customHeight="1">
-      <c r="A4" s="118" t="s">
+      <c r="A4" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="118"/>
+      <c r="B4" s="130"/>
       <c r="C4" s="14">
         <v>2006</v>
       </c>
@@ -20093,10 +20109,10 @@
       </c>
     </row>
     <row r="5" spans="1:44" s="14" customFormat="1" ht="20" customHeight="1">
-      <c r="A5" s="118" t="s">
+      <c r="A5" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="118"/>
+      <c r="B5" s="130"/>
       <c r="C5" s="14">
         <v>4</v>
       </c>
@@ -20225,7 +20241,7 @@
       </c>
     </row>
     <row r="6" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A6" s="123" t="s">
+      <c r="A6" s="139" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -20359,7 +20375,7 @@
       </c>
     </row>
     <row r="7" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A7" s="123"/>
+      <c r="A7" s="139"/>
       <c r="B7" s="16" t="s">
         <v>34</v>
       </c>
@@ -20491,7 +20507,7 @@
       </c>
     </row>
     <row r="8" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A8" s="123"/>
+      <c r="A8" s="139"/>
       <c r="B8" s="16" t="s">
         <v>35</v>
       </c>
@@ -20623,7 +20639,7 @@
       </c>
     </row>
     <row r="9" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A9" s="123"/>
+      <c r="A9" s="139"/>
       <c r="B9" s="15" t="s">
         <v>51</v>
       </c>
@@ -20755,7 +20771,7 @@
       </c>
     </row>
     <row r="10" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A10" s="123"/>
+      <c r="A10" s="139"/>
       <c r="B10" s="16" t="s">
         <v>36</v>
       </c>
@@ -20887,7 +20903,7 @@
       </c>
     </row>
     <row r="11" spans="1:44" ht="20" customHeight="1">
-      <c r="A11" s="119" t="s">
+      <c r="A11" s="134" t="s">
         <v>37</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -21021,7 +21037,7 @@
       </c>
     </row>
     <row r="12" spans="1:44" ht="20" customHeight="1">
-      <c r="A12" s="119"/>
+      <c r="A12" s="134"/>
       <c r="B12" s="6" t="s">
         <v>39</v>
       </c>
@@ -21153,7 +21169,7 @@
       </c>
     </row>
     <row r="13" spans="1:44" ht="20" customHeight="1">
-      <c r="A13" s="119"/>
+      <c r="A13" s="134"/>
       <c r="B13" s="6" t="s">
         <v>40</v>
       </c>
@@ -21285,7 +21301,7 @@
       </c>
     </row>
     <row r="14" spans="1:44" ht="20" customHeight="1">
-      <c r="A14" s="119"/>
+      <c r="A14" s="134"/>
       <c r="B14" s="6" t="s">
         <v>41</v>
       </c>
@@ -21417,7 +21433,7 @@
       </c>
     </row>
     <row r="15" spans="1:44" s="11" customFormat="1" ht="20" customHeight="1">
-      <c r="A15" s="114" t="s">
+      <c r="A15" s="135" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="10" t="s">
@@ -21551,7 +21567,7 @@
       </c>
     </row>
     <row r="16" spans="1:44" s="11" customFormat="1" ht="20" customHeight="1">
-      <c r="A16" s="114"/>
+      <c r="A16" s="135"/>
       <c r="B16" s="10" t="s">
         <v>43</v>
       </c>
@@ -21683,7 +21699,7 @@
       </c>
     </row>
     <row r="17" spans="1:44" ht="20" customHeight="1">
-      <c r="A17" s="119" t="s">
+      <c r="A17" s="134" t="s">
         <v>44</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -21817,7 +21833,7 @@
       </c>
     </row>
     <row r="18" spans="1:44" ht="20" customHeight="1">
-      <c r="A18" s="119"/>
+      <c r="A18" s="134"/>
       <c r="B18" s="6" t="s">
         <v>46</v>
       </c>
@@ -21949,7 +21965,7 @@
       </c>
     </row>
     <row r="19" spans="1:44" ht="20" customHeight="1">
-      <c r="A19" s="119"/>
+      <c r="A19" s="134"/>
       <c r="B19" s="6" t="s">
         <v>47</v>
       </c>
@@ -22607,6 +22623,29 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="AP2:AR2"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="AJ2:AL2"/>
+    <mergeCell ref="AM2:AO2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="U2:W2"/>
+    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="AD2:AF2"/>
+    <mergeCell ref="AA2:AC2"/>
+    <mergeCell ref="AJ3:AL3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AM3:AO3"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="AG3:AI3"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="X3:Z3"/>
+    <mergeCell ref="AD3:AF3"/>
+    <mergeCell ref="AA3:AC3"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="O3:Q3"/>
     <mergeCell ref="R3:T3"/>
@@ -22620,29 +22659,6 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C2:E2"/>
-    <mergeCell ref="AJ3:AL3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AM3:AO3"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="AG3:AI3"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="X3:Z3"/>
-    <mergeCell ref="AD3:AF3"/>
-    <mergeCell ref="AA3:AC3"/>
-    <mergeCell ref="AP2:AR2"/>
-    <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="AJ2:AL2"/>
-    <mergeCell ref="AM2:AO2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="U2:W2"/>
-    <mergeCell ref="X2:Z2"/>
-    <mergeCell ref="AD2:AF2"/>
-    <mergeCell ref="AA2:AC2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -22854,44 +22870,44 @@
     <row r="1" spans="1:19">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="118" t="s">
+      <c r="C1" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="118" t="s">
+      <c r="D1" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="118" t="s">
+      <c r="E1" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="139" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="119" t="s">
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="134" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
-      <c r="N1" s="119"/>
-      <c r="O1" s="114" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="114"/>
-      <c r="Q1" s="119" t="s">
+      <c r="L1" s="134"/>
+      <c r="M1" s="134"/>
+      <c r="N1" s="134"/>
+      <c r="O1" s="135" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="135"/>
+      <c r="Q1" s="134" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="119"/>
-      <c r="S1" s="119"/>
+      <c r="R1" s="134"/>
+      <c r="S1" s="134"/>
     </row>
     <row r="2" spans="1:19" ht="84">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -22936,13 +22952,13 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="136" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="115">
-        <v>1</v>
-      </c>
-      <c r="C3" s="118" t="s">
+      <c r="B3" s="127">
+        <v>1</v>
+      </c>
+      <c r="C3" s="130" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="14">
@@ -22995,9 +23011,9 @@
       </c>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="121"/>
-      <c r="B4" s="116"/>
-      <c r="C4" s="118"/>
+      <c r="A4" s="137"/>
+      <c r="B4" s="128"/>
+      <c r="C4" s="130"/>
       <c r="D4" s="14">
         <v>2010</v>
       </c>
@@ -23048,9 +23064,9 @@
       </c>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="121"/>
-      <c r="B5" s="117"/>
-      <c r="C5" s="118"/>
+      <c r="A5" s="137"/>
+      <c r="B5" s="129"/>
+      <c r="C5" s="130"/>
       <c r="D5" s="25">
         <v>2014</v>
       </c>
@@ -23101,11 +23117,11 @@
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="121"/>
-      <c r="B6" s="115">
+      <c r="A6" s="137"/>
+      <c r="B6" s="127">
         <v>2</v>
       </c>
-      <c r="C6" s="118" t="s">
+      <c r="C6" s="130" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="14">
@@ -23158,9 +23174,9 @@
       </c>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="121"/>
-      <c r="B7" s="116"/>
-      <c r="C7" s="118"/>
+      <c r="A7" s="137"/>
+      <c r="B7" s="128"/>
+      <c r="C7" s="130"/>
       <c r="D7" s="14">
         <v>2010</v>
       </c>
@@ -23211,9 +23227,9 @@
       </c>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" s="121"/>
-      <c r="B8" s="117"/>
-      <c r="C8" s="118"/>
+      <c r="A8" s="137"/>
+      <c r="B8" s="129"/>
+      <c r="C8" s="130"/>
       <c r="D8" s="25">
         <v>2014</v>
       </c>
@@ -23264,11 +23280,11 @@
       </c>
     </row>
     <row r="9" spans="1:19">
-      <c r="A9" s="121"/>
-      <c r="B9" s="115">
+      <c r="A9" s="137"/>
+      <c r="B9" s="127">
         <v>3</v>
       </c>
-      <c r="C9" s="118" t="s">
+      <c r="C9" s="130" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="14">
@@ -23321,9 +23337,9 @@
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="121"/>
-      <c r="B10" s="116"/>
-      <c r="C10" s="118"/>
+      <c r="A10" s="137"/>
+      <c r="B10" s="128"/>
+      <c r="C10" s="130"/>
       <c r="D10" s="14">
         <v>2010</v>
       </c>
@@ -23374,9 +23390,9 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="121"/>
-      <c r="B11" s="117"/>
-      <c r="C11" s="118"/>
+      <c r="A11" s="137"/>
+      <c r="B11" s="129"/>
+      <c r="C11" s="130"/>
       <c r="D11" s="25">
         <v>2014</v>
       </c>
@@ -23427,11 +23443,11 @@
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="121"/>
-      <c r="B12" s="115">
+      <c r="A12" s="137"/>
+      <c r="B12" s="127">
         <v>4</v>
       </c>
-      <c r="C12" s="118" t="s">
+      <c r="C12" s="130" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="14">
@@ -23484,9 +23500,9 @@
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="121"/>
-      <c r="B13" s="116"/>
-      <c r="C13" s="118"/>
+      <c r="A13" s="137"/>
+      <c r="B13" s="128"/>
+      <c r="C13" s="130"/>
       <c r="D13" s="14">
         <v>2010</v>
       </c>
@@ -23537,9 +23553,9 @@
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="121"/>
-      <c r="B14" s="117"/>
-      <c r="C14" s="118"/>
+      <c r="A14" s="137"/>
+      <c r="B14" s="129"/>
+      <c r="C14" s="130"/>
       <c r="D14" s="25">
         <v>2014</v>
       </c>
@@ -23590,11 +23606,11 @@
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="121"/>
-      <c r="B15" s="115">
+      <c r="A15" s="137"/>
+      <c r="B15" s="127">
         <v>5</v>
       </c>
-      <c r="C15" s="118" t="s">
+      <c r="C15" s="130" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="14">
@@ -23647,9 +23663,9 @@
       </c>
     </row>
     <row r="16" spans="1:19">
-      <c r="A16" s="121"/>
-      <c r="B16" s="116"/>
-      <c r="C16" s="118"/>
+      <c r="A16" s="137"/>
+      <c r="B16" s="128"/>
+      <c r="C16" s="130"/>
       <c r="D16" s="14">
         <v>2010</v>
       </c>
@@ -23700,9 +23716,9 @@
       </c>
     </row>
     <row r="17" spans="1:19">
-      <c r="A17" s="121"/>
-      <c r="B17" s="117"/>
-      <c r="C17" s="118"/>
+      <c r="A17" s="137"/>
+      <c r="B17" s="129"/>
+      <c r="C17" s="130"/>
       <c r="D17" s="25">
         <v>2014</v>
       </c>
@@ -23753,11 +23769,11 @@
       </c>
     </row>
     <row r="18" spans="1:19">
-      <c r="A18" s="121"/>
-      <c r="B18" s="115">
+      <c r="A18" s="137"/>
+      <c r="B18" s="127">
         <v>6</v>
       </c>
-      <c r="C18" s="118" t="s">
+      <c r="C18" s="130" t="s">
         <v>25</v>
       </c>
       <c r="D18" s="14">
@@ -23810,9 +23826,9 @@
       </c>
     </row>
     <row r="19" spans="1:19">
-      <c r="A19" s="121"/>
-      <c r="B19" s="116"/>
-      <c r="C19" s="118"/>
+      <c r="A19" s="137"/>
+      <c r="B19" s="128"/>
+      <c r="C19" s="130"/>
       <c r="D19" s="14">
         <v>2010</v>
       </c>
@@ -23863,9 +23879,9 @@
       </c>
     </row>
     <row r="20" spans="1:19">
-      <c r="A20" s="121"/>
-      <c r="B20" s="117"/>
-      <c r="C20" s="118"/>
+      <c r="A20" s="137"/>
+      <c r="B20" s="129"/>
+      <c r="C20" s="130"/>
       <c r="D20" s="25">
         <v>2014</v>
       </c>
@@ -23916,11 +23932,11 @@
       </c>
     </row>
     <row r="21" spans="1:19">
-      <c r="A21" s="121"/>
-      <c r="B21" s="115">
+      <c r="A21" s="137"/>
+      <c r="B21" s="127">
         <v>7</v>
       </c>
-      <c r="C21" s="118" t="s">
+      <c r="C21" s="130" t="s">
         <v>15</v>
       </c>
       <c r="D21" s="14">
@@ -23973,9 +23989,9 @@
       </c>
     </row>
     <row r="22" spans="1:19">
-      <c r="A22" s="121"/>
-      <c r="B22" s="116"/>
-      <c r="C22" s="118"/>
+      <c r="A22" s="137"/>
+      <c r="B22" s="128"/>
+      <c r="C22" s="130"/>
       <c r="D22" s="14">
         <v>2010</v>
       </c>
@@ -24026,9 +24042,9 @@
       </c>
     </row>
     <row r="23" spans="1:19">
-      <c r="A23" s="121"/>
-      <c r="B23" s="117"/>
-      <c r="C23" s="118"/>
+      <c r="A23" s="137"/>
+      <c r="B23" s="129"/>
+      <c r="C23" s="130"/>
       <c r="D23" s="25">
         <v>2014</v>
       </c>
@@ -24079,11 +24095,11 @@
       </c>
     </row>
     <row r="24" spans="1:19">
-      <c r="A24" s="121"/>
-      <c r="B24" s="115">
+      <c r="A24" s="137"/>
+      <c r="B24" s="127">
         <v>8</v>
       </c>
-      <c r="C24" s="118" t="s">
+      <c r="C24" s="130" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="14">
@@ -24136,9 +24152,9 @@
       </c>
     </row>
     <row r="25" spans="1:19">
-      <c r="A25" s="121"/>
-      <c r="B25" s="116"/>
-      <c r="C25" s="118"/>
+      <c r="A25" s="137"/>
+      <c r="B25" s="128"/>
+      <c r="C25" s="130"/>
       <c r="D25" s="14">
         <v>2010</v>
       </c>
@@ -24189,9 +24205,9 @@
       </c>
     </row>
     <row r="26" spans="1:19">
-      <c r="A26" s="121"/>
-      <c r="B26" s="117"/>
-      <c r="C26" s="118"/>
+      <c r="A26" s="137"/>
+      <c r="B26" s="129"/>
+      <c r="C26" s="130"/>
       <c r="D26" s="25">
         <v>2014</v>
       </c>
@@ -24242,11 +24258,11 @@
       </c>
     </row>
     <row r="27" spans="1:19">
-      <c r="A27" s="121"/>
-      <c r="B27" s="115">
+      <c r="A27" s="137"/>
+      <c r="B27" s="127">
         <v>14</v>
       </c>
-      <c r="C27" s="124" t="s">
+      <c r="C27" s="131" t="s">
         <v>54</v>
       </c>
       <c r="D27" s="14">
@@ -24299,9 +24315,9 @@
       </c>
     </row>
     <row r="28" spans="1:19">
-      <c r="A28" s="121"/>
-      <c r="B28" s="116"/>
-      <c r="C28" s="125"/>
+      <c r="A28" s="137"/>
+      <c r="B28" s="128"/>
+      <c r="C28" s="132"/>
       <c r="D28" s="14">
         <v>2010</v>
       </c>
@@ -24352,9 +24368,9 @@
       </c>
     </row>
     <row r="29" spans="1:19">
-      <c r="A29" s="121"/>
-      <c r="B29" s="117"/>
-      <c r="C29" s="126"/>
+      <c r="A29" s="137"/>
+      <c r="B29" s="129"/>
+      <c r="C29" s="133"/>
       <c r="D29" s="25">
         <v>2014</v>
       </c>
@@ -24405,11 +24421,11 @@
       </c>
     </row>
     <row r="30" spans="1:19">
-      <c r="A30" s="121"/>
-      <c r="B30" s="115">
+      <c r="A30" s="137"/>
+      <c r="B30" s="127">
         <v>9</v>
       </c>
-      <c r="C30" s="118" t="s">
+      <c r="C30" s="130" t="s">
         <v>12</v>
       </c>
       <c r="D30" s="14">
@@ -24462,9 +24478,9 @@
       </c>
     </row>
     <row r="31" spans="1:19">
-      <c r="A31" s="121"/>
-      <c r="B31" s="116"/>
-      <c r="C31" s="118"/>
+      <c r="A31" s="137"/>
+      <c r="B31" s="128"/>
+      <c r="C31" s="130"/>
       <c r="D31" s="14">
         <v>2010</v>
       </c>
@@ -24515,9 +24531,9 @@
       </c>
     </row>
     <row r="32" spans="1:19">
-      <c r="A32" s="121"/>
-      <c r="B32" s="117"/>
-      <c r="C32" s="118"/>
+      <c r="A32" s="137"/>
+      <c r="B32" s="129"/>
+      <c r="C32" s="130"/>
       <c r="D32" s="25">
         <v>2014</v>
       </c>
@@ -24568,11 +24584,11 @@
       </c>
     </row>
     <row r="33" spans="1:41">
-      <c r="A33" s="121"/>
-      <c r="B33" s="115">
+      <c r="A33" s="137"/>
+      <c r="B33" s="127">
         <v>10</v>
       </c>
-      <c r="C33" s="118" t="s">
+      <c r="C33" s="130" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="14">
@@ -24625,9 +24641,9 @@
       </c>
     </row>
     <row r="34" spans="1:41">
-      <c r="A34" s="121"/>
-      <c r="B34" s="116"/>
-      <c r="C34" s="118"/>
+      <c r="A34" s="137"/>
+      <c r="B34" s="128"/>
+      <c r="C34" s="130"/>
       <c r="D34" s="14">
         <v>2010</v>
       </c>
@@ -24678,9 +24694,9 @@
       </c>
     </row>
     <row r="35" spans="1:41">
-      <c r="A35" s="121"/>
-      <c r="B35" s="117"/>
-      <c r="C35" s="118"/>
+      <c r="A35" s="137"/>
+      <c r="B35" s="129"/>
+      <c r="C35" s="130"/>
       <c r="D35" s="25">
         <v>2014</v>
       </c>
@@ -24731,11 +24747,11 @@
       </c>
     </row>
     <row r="36" spans="1:41">
-      <c r="A36" s="121"/>
-      <c r="B36" s="115">
+      <c r="A36" s="137"/>
+      <c r="B36" s="127">
         <v>11</v>
       </c>
-      <c r="C36" s="118" t="s">
+      <c r="C36" s="130" t="s">
         <v>21</v>
       </c>
       <c r="D36" s="14">
@@ -24788,9 +24804,9 @@
       </c>
     </row>
     <row r="37" spans="1:41">
-      <c r="A37" s="121"/>
-      <c r="B37" s="116"/>
-      <c r="C37" s="118"/>
+      <c r="A37" s="137"/>
+      <c r="B37" s="128"/>
+      <c r="C37" s="130"/>
       <c r="D37" s="14">
         <v>2010</v>
       </c>
@@ -24841,9 +24857,9 @@
       </c>
     </row>
     <row r="38" spans="1:41">
-      <c r="A38" s="121"/>
-      <c r="B38" s="117"/>
-      <c r="C38" s="118"/>
+      <c r="A38" s="137"/>
+      <c r="B38" s="129"/>
+      <c r="C38" s="130"/>
       <c r="D38" s="25">
         <v>2014</v>
       </c>
@@ -24894,11 +24910,11 @@
       </c>
     </row>
     <row r="39" spans="1:41">
-      <c r="A39" s="121"/>
-      <c r="B39" s="115">
+      <c r="A39" s="137"/>
+      <c r="B39" s="127">
         <v>12</v>
       </c>
-      <c r="C39" s="118" t="s">
+      <c r="C39" s="130" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="14">
@@ -24951,9 +24967,9 @@
       </c>
     </row>
     <row r="40" spans="1:41">
-      <c r="A40" s="121"/>
-      <c r="B40" s="116"/>
-      <c r="C40" s="118"/>
+      <c r="A40" s="137"/>
+      <c r="B40" s="128"/>
+      <c r="C40" s="130"/>
       <c r="D40" s="14">
         <v>2010</v>
       </c>
@@ -25004,9 +25020,9 @@
       </c>
     </row>
     <row r="41" spans="1:41">
-      <c r="A41" s="121"/>
-      <c r="B41" s="117"/>
-      <c r="C41" s="118"/>
+      <c r="A41" s="137"/>
+      <c r="B41" s="129"/>
+      <c r="C41" s="130"/>
       <c r="D41" s="25">
         <v>2014</v>
       </c>
@@ -25057,11 +25073,11 @@
       </c>
     </row>
     <row r="42" spans="1:41">
-      <c r="A42" s="121"/>
-      <c r="B42" s="115">
+      <c r="A42" s="137"/>
+      <c r="B42" s="127">
         <v>13</v>
       </c>
-      <c r="C42" s="118" t="s">
+      <c r="C42" s="130" t="s">
         <v>8</v>
       </c>
       <c r="D42" s="14">
@@ -25114,9 +25130,9 @@
       </c>
     </row>
     <row r="43" spans="1:41">
-      <c r="A43" s="121"/>
-      <c r="B43" s="116"/>
-      <c r="C43" s="118"/>
+      <c r="A43" s="137"/>
+      <c r="B43" s="128"/>
+      <c r="C43" s="130"/>
       <c r="D43" s="14">
         <v>2010</v>
       </c>
@@ -25167,9 +25183,9 @@
       </c>
     </row>
     <row r="44" spans="1:41">
-      <c r="A44" s="122"/>
-      <c r="B44" s="117"/>
-      <c r="C44" s="118"/>
+      <c r="A44" s="138"/>
+      <c r="B44" s="129"/>
+      <c r="C44" s="130"/>
       <c r="D44" s="25">
         <v>2014</v>
       </c>
@@ -25220,81 +25236,81 @@
       </c>
     </row>
     <row r="46" spans="1:41" ht="15.75" customHeight="1">
-      <c r="A46" s="118" t="s">
+      <c r="A46" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="118"/>
-      <c r="C46" s="118" t="s">
+      <c r="B46" s="130"/>
+      <c r="C46" s="130" t="s">
         <v>50</v>
       </c>
-      <c r="D46" s="118"/>
-      <c r="E46" s="118"/>
-      <c r="F46" s="118" t="s">
+      <c r="D46" s="130"/>
+      <c r="E46" s="130"/>
+      <c r="F46" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="G46" s="118"/>
-      <c r="H46" s="118"/>
-      <c r="I46" s="118" t="s">
+      <c r="G46" s="130"/>
+      <c r="H46" s="130"/>
+      <c r="I46" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="J46" s="118"/>
-      <c r="K46" s="118"/>
-      <c r="L46" s="118" t="s">
+      <c r="J46" s="130"/>
+      <c r="K46" s="130"/>
+      <c r="L46" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="M46" s="118"/>
-      <c r="N46" s="118"/>
-      <c r="O46" s="118" t="s">
+      <c r="M46" s="130"/>
+      <c r="N46" s="130"/>
+      <c r="O46" s="130" t="s">
         <v>23</v>
       </c>
-      <c r="P46" s="118"/>
-      <c r="Q46" s="118"/>
-      <c r="R46" s="118" t="s">
+      <c r="P46" s="130"/>
+      <c r="Q46" s="130"/>
+      <c r="R46" s="130" t="s">
         <v>87</v>
       </c>
-      <c r="S46" s="118"/>
-      <c r="T46" s="118"/>
-      <c r="U46" s="124" t="s">
+      <c r="S46" s="130"/>
+      <c r="T46" s="130"/>
+      <c r="U46" s="131" t="s">
         <v>70</v>
       </c>
-      <c r="V46" s="125"/>
-      <c r="W46" s="126"/>
-      <c r="X46" s="124" t="s">
+      <c r="V46" s="132"/>
+      <c r="W46" s="133"/>
+      <c r="X46" s="131" t="s">
         <v>54</v>
       </c>
-      <c r="Y46" s="125"/>
-      <c r="Z46" s="126"/>
-      <c r="AA46" s="118" t="s">
+      <c r="Y46" s="132"/>
+      <c r="Z46" s="133"/>
+      <c r="AA46" s="130" t="s">
         <v>12</v>
       </c>
-      <c r="AB46" s="118"/>
-      <c r="AC46" s="118"/>
-      <c r="AD46" s="118" t="s">
+      <c r="AB46" s="130"/>
+      <c r="AC46" s="130"/>
+      <c r="AD46" s="130" t="s">
         <v>28</v>
       </c>
-      <c r="AE46" s="118"/>
-      <c r="AF46" s="118"/>
-      <c r="AG46" s="118" t="s">
+      <c r="AE46" s="130"/>
+      <c r="AF46" s="130"/>
+      <c r="AG46" s="130" t="s">
         <v>21</v>
       </c>
-      <c r="AH46" s="118"/>
-      <c r="AI46" s="118"/>
-      <c r="AJ46" s="118" t="s">
+      <c r="AH46" s="130"/>
+      <c r="AI46" s="130"/>
+      <c r="AJ46" s="130" t="s">
         <v>13</v>
       </c>
-      <c r="AK46" s="118"/>
-      <c r="AL46" s="118"/>
-      <c r="AM46" s="118" t="s">
+      <c r="AK46" s="130"/>
+      <c r="AL46" s="130"/>
+      <c r="AM46" s="130" t="s">
         <v>8</v>
       </c>
-      <c r="AN46" s="118"/>
-      <c r="AO46" s="118"/>
+      <c r="AN46" s="130"/>
+      <c r="AO46" s="130"/>
     </row>
     <row r="47" spans="1:41" ht="42.75" customHeight="1">
-      <c r="A47" s="118" t="s">
+      <c r="A47" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="118"/>
+      <c r="B47" s="130"/>
       <c r="C47" s="54" t="s">
         <v>72</v>
       </c>
@@ -25414,10 +25430,10 @@
       </c>
     </row>
     <row r="48" spans="1:41" ht="33" customHeight="1">
-      <c r="A48" s="118" t="s">
+      <c r="A48" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="118"/>
+      <c r="B48" s="130"/>
       <c r="C48" s="54">
         <v>4</v>
       </c>
@@ -25548,7 +25564,7 @@
       </c>
     </row>
     <row r="50" spans="2:4">
-      <c r="B50" s="134"/>
+      <c r="B50" s="120"/>
       <c r="C50" s="63">
         <v>2010</v>
       </c>
@@ -25557,7 +25573,7 @@
       </c>
     </row>
     <row r="51" spans="2:4">
-      <c r="B51" s="134"/>
+      <c r="B51" s="120"/>
       <c r="C51" s="63">
         <v>2014</v>
       </c>
@@ -25567,26 +25583,23 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="AA46:AC46"/>
+    <mergeCell ref="AD46:AF46"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="L46:N46"/>
+    <mergeCell ref="AG46:AI46"/>
+    <mergeCell ref="AJ46:AL46"/>
+    <mergeCell ref="AM46:AO46"/>
+    <mergeCell ref="O46:Q46"/>
+    <mergeCell ref="R46:T46"/>
+    <mergeCell ref="U46:W46"/>
+    <mergeCell ref="X46:Z46"/>
     <mergeCell ref="B39:B41"/>
     <mergeCell ref="C39:C41"/>
     <mergeCell ref="B42:B44"/>
@@ -25603,23 +25616,26 @@
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="C24:C26"/>
     <mergeCell ref="B27:B29"/>
-    <mergeCell ref="AG46:AI46"/>
-    <mergeCell ref="AJ46:AL46"/>
-    <mergeCell ref="AM46:AO46"/>
-    <mergeCell ref="O46:Q46"/>
-    <mergeCell ref="R46:T46"/>
-    <mergeCell ref="U46:W46"/>
-    <mergeCell ref="X46:Z46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="AA46:AC46"/>
-    <mergeCell ref="AD46:AF46"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="I46:K46"/>
-    <mergeCell ref="L46:N46"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
transformXY for streamgraph_data - Don't look good
</commit_message>
<xml_diff>
--- a/GenderGap_Data/GenderGap_Find4Hourglass.xlsx
+++ b/GenderGap_Data/GenderGap_Find4Hourglass.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="200">
   <si>
     <t xml:space="preserve">Labour force participation                              </t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -767,6 +767,9 @@
   </si>
   <si>
     <t>size</t>
+  </si>
+  <si>
+    <t>ECONOMIC PARTICIPATION AND OPPORTUNITY</t>
   </si>
 </sst>
 </file>
@@ -1683,43 +1686,7 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="106" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="2" xfId="106" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="3" xfId="106" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="4" xfId="106" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" xfId="108" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="16" xfId="108" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1734,19 +1701,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1760,6 +1715,54 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="2" xfId="106" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="3" xfId="106" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="4" xfId="106" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="106" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" xfId="108" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="16" xfId="108" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2326,11 +2329,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="-2123193160"/>
-        <c:axId val="-2123196200"/>
+        <c:axId val="-2110959080"/>
+        <c:axId val="-2111540472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2123193160"/>
+        <c:axId val="-2110959080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2339,7 +2342,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123196200"/>
+        <c:crossAx val="-2111540472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2347,7 +2350,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2123196200"/>
+        <c:axId val="-2111540472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2363,14 +2366,13 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2123193160"/>
+        <c:crossAx val="-2110959080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2578,11 +2580,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2123271464"/>
-        <c:axId val="-2123274424"/>
+        <c:axId val="-2093535768"/>
+        <c:axId val="-2093532824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2123271464"/>
+        <c:axId val="-2093535768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2591,7 +2593,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123274424"/>
+        <c:crossAx val="-2093532824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2599,7 +2601,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2123274424"/>
+        <c:axId val="-2093532824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2610,7 +2612,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="-2123271464"/>
+        <c:crossAx val="-2093535768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6116,37 +6118,37 @@
     <row r="1" spans="1:27" ht="34" customHeight="1">
       <c r="A1" s="97"/>
       <c r="B1" s="97"/>
-      <c r="C1" s="130" t="s">
+      <c r="C1" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="130" t="s">
+      <c r="D1" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="130" t="s">
+      <c r="E1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="139" t="s">
+      <c r="F1" s="123" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="134" t="s">
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="123"/>
+      <c r="J1" s="123"/>
+      <c r="K1" s="119" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="134"/>
-      <c r="M1" s="134"/>
-      <c r="N1" s="134"/>
-      <c r="O1" s="135" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="135"/>
-      <c r="Q1" s="134" t="s">
+      <c r="L1" s="119"/>
+      <c r="M1" s="119"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="114" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="114"/>
+      <c r="Q1" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="134"/>
-      <c r="S1" s="134"/>
+      <c r="R1" s="119"/>
+      <c r="S1" s="119"/>
       <c r="T1" s="71" t="s">
         <v>92</v>
       </c>
@@ -6163,9 +6165,9 @@
     <row r="2" spans="1:27" ht="113" customHeight="1">
       <c r="A2" s="97"/>
       <c r="B2" s="97"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -6234,13 +6236,13 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="120" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="127">
-        <v>1</v>
-      </c>
-      <c r="C3" s="130" t="s">
+      <c r="B3" s="115">
+        <v>1</v>
+      </c>
+      <c r="C3" s="118" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="92">
@@ -6308,9 +6310,9 @@
       </c>
     </row>
     <row r="4" spans="1:27">
-      <c r="A4" s="137"/>
-      <c r="B4" s="128"/>
-      <c r="C4" s="130"/>
+      <c r="A4" s="121"/>
+      <c r="B4" s="116"/>
+      <c r="C4" s="118"/>
       <c r="D4" s="92">
         <v>2010</v>
       </c>
@@ -6376,9 +6378,9 @@
       </c>
     </row>
     <row r="5" spans="1:27">
-      <c r="A5" s="137"/>
-      <c r="B5" s="129"/>
-      <c r="C5" s="130"/>
+      <c r="A5" s="121"/>
+      <c r="B5" s="117"/>
+      <c r="C5" s="118"/>
       <c r="D5" s="25">
         <v>2014</v>
       </c>
@@ -6444,7 +6446,7 @@
       </c>
     </row>
     <row r="6" spans="1:27">
-      <c r="A6" s="137"/>
+      <c r="A6" s="121"/>
       <c r="B6" s="91"/>
       <c r="C6" s="92"/>
       <c r="D6" s="25"/>
@@ -6466,11 +6468,11 @@
       <c r="X6" s="106"/>
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1">
-      <c r="A7" s="137"/>
-      <c r="B7" s="127">
+      <c r="A7" s="121"/>
+      <c r="B7" s="115">
         <v>2</v>
       </c>
-      <c r="C7" s="130" t="s">
+      <c r="C7" s="118" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="92">
@@ -6538,9 +6540,9 @@
       </c>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="137"/>
-      <c r="B8" s="128"/>
-      <c r="C8" s="130"/>
+      <c r="A8" s="121"/>
+      <c r="B8" s="116"/>
+      <c r="C8" s="118"/>
       <c r="D8" s="92">
         <v>2010</v>
       </c>
@@ -6606,9 +6608,9 @@
       </c>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="137"/>
-      <c r="B9" s="129"/>
-      <c r="C9" s="130"/>
+      <c r="A9" s="121"/>
+      <c r="B9" s="117"/>
+      <c r="C9" s="118"/>
       <c r="D9" s="25">
         <v>2014</v>
       </c>
@@ -6674,7 +6676,7 @@
       </c>
     </row>
     <row r="10" spans="1:27">
-      <c r="A10" s="137"/>
+      <c r="A10" s="121"/>
       <c r="B10" s="91"/>
       <c r="C10" s="92"/>
       <c r="D10" s="25"/>
@@ -6696,11 +6698,11 @@
       <c r="X10" s="106"/>
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A11" s="137"/>
-      <c r="B11" s="127">
+      <c r="A11" s="121"/>
+      <c r="B11" s="115">
         <v>3</v>
       </c>
-      <c r="C11" s="130" t="s">
+      <c r="C11" s="118" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="92">
@@ -6768,9 +6770,9 @@
       </c>
     </row>
     <row r="12" spans="1:27">
-      <c r="A12" s="137"/>
-      <c r="B12" s="128"/>
-      <c r="C12" s="130"/>
+      <c r="A12" s="121"/>
+      <c r="B12" s="116"/>
+      <c r="C12" s="118"/>
       <c r="D12" s="92">
         <v>2010</v>
       </c>
@@ -6836,9 +6838,9 @@
       </c>
     </row>
     <row r="13" spans="1:27">
-      <c r="A13" s="137"/>
-      <c r="B13" s="129"/>
-      <c r="C13" s="130"/>
+      <c r="A13" s="121"/>
+      <c r="B13" s="117"/>
+      <c r="C13" s="118"/>
       <c r="D13" s="25">
         <v>2014</v>
       </c>
@@ -6904,7 +6906,7 @@
       </c>
     </row>
     <row r="14" spans="1:27">
-      <c r="A14" s="137"/>
+      <c r="A14" s="121"/>
       <c r="B14" s="91"/>
       <c r="C14" s="92"/>
       <c r="D14" s="25"/>
@@ -6926,11 +6928,11 @@
       <c r="X14" s="106"/>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="137"/>
-      <c r="B15" s="127">
+      <c r="A15" s="121"/>
+      <c r="B15" s="115">
         <v>4</v>
       </c>
-      <c r="C15" s="130" t="s">
+      <c r="C15" s="118" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="92">
@@ -6998,9 +7000,9 @@
       </c>
     </row>
     <row r="16" spans="1:27">
-      <c r="A16" s="137"/>
-      <c r="B16" s="128"/>
-      <c r="C16" s="130"/>
+      <c r="A16" s="121"/>
+      <c r="B16" s="116"/>
+      <c r="C16" s="118"/>
       <c r="D16" s="92">
         <v>2010</v>
       </c>
@@ -7066,9 +7068,9 @@
       </c>
     </row>
     <row r="17" spans="1:24">
-      <c r="A17" s="137"/>
-      <c r="B17" s="129"/>
-      <c r="C17" s="130"/>
+      <c r="A17" s="121"/>
+      <c r="B17" s="117"/>
+      <c r="C17" s="118"/>
       <c r="D17" s="25">
         <v>2014</v>
       </c>
@@ -7134,7 +7136,7 @@
       </c>
     </row>
     <row r="18" spans="1:24">
-      <c r="A18" s="137"/>
+      <c r="A18" s="121"/>
       <c r="B18" s="91"/>
       <c r="C18" s="92"/>
       <c r="D18" s="25"/>
@@ -7156,11 +7158,11 @@
       <c r="X18" s="106"/>
     </row>
     <row r="19" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A19" s="137"/>
-      <c r="B19" s="127">
+      <c r="A19" s="121"/>
+      <c r="B19" s="115">
         <v>5</v>
       </c>
-      <c r="C19" s="130" t="s">
+      <c r="C19" s="118" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="92">
@@ -7228,9 +7230,9 @@
       </c>
     </row>
     <row r="20" spans="1:24">
-      <c r="A20" s="137"/>
-      <c r="B20" s="128"/>
-      <c r="C20" s="130"/>
+      <c r="A20" s="121"/>
+      <c r="B20" s="116"/>
+      <c r="C20" s="118"/>
       <c r="D20" s="92">
         <v>2010</v>
       </c>
@@ -7296,9 +7298,9 @@
       </c>
     </row>
     <row r="21" spans="1:24">
-      <c r="A21" s="137"/>
-      <c r="B21" s="129"/>
-      <c r="C21" s="130"/>
+      <c r="A21" s="121"/>
+      <c r="B21" s="117"/>
+      <c r="C21" s="118"/>
       <c r="D21" s="25">
         <v>2014</v>
       </c>
@@ -7364,7 +7366,7 @@
       </c>
     </row>
     <row r="22" spans="1:24">
-      <c r="A22" s="137"/>
+      <c r="A22" s="121"/>
       <c r="B22" s="91"/>
       <c r="C22" s="92"/>
       <c r="D22" s="25"/>
@@ -7386,11 +7388,11 @@
       <c r="X22" s="106"/>
     </row>
     <row r="23" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A23" s="137"/>
-      <c r="B23" s="127">
+      <c r="A23" s="121"/>
+      <c r="B23" s="115">
         <v>6</v>
       </c>
-      <c r="C23" s="130" t="s">
+      <c r="C23" s="118" t="s">
         <v>25</v>
       </c>
       <c r="D23" s="92">
@@ -7458,9 +7460,9 @@
       </c>
     </row>
     <row r="24" spans="1:24">
-      <c r="A24" s="137"/>
-      <c r="B24" s="128"/>
-      <c r="C24" s="130"/>
+      <c r="A24" s="121"/>
+      <c r="B24" s="116"/>
+      <c r="C24" s="118"/>
       <c r="D24" s="92">
         <v>2010</v>
       </c>
@@ -7526,9 +7528,9 @@
       </c>
     </row>
     <row r="25" spans="1:24">
-      <c r="A25" s="137"/>
-      <c r="B25" s="129"/>
-      <c r="C25" s="130"/>
+      <c r="A25" s="121"/>
+      <c r="B25" s="117"/>
+      <c r="C25" s="118"/>
       <c r="D25" s="25">
         <v>2014</v>
       </c>
@@ -7594,7 +7596,7 @@
       </c>
     </row>
     <row r="26" spans="1:24">
-      <c r="A26" s="137"/>
+      <c r="A26" s="121"/>
       <c r="B26" s="91"/>
       <c r="C26" s="92"/>
       <c r="D26" s="25"/>
@@ -7616,11 +7618,11 @@
       <c r="X26" s="106"/>
     </row>
     <row r="27" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A27" s="137"/>
-      <c r="B27" s="127">
+      <c r="A27" s="121"/>
+      <c r="B27" s="115">
         <v>7</v>
       </c>
-      <c r="C27" s="130" t="s">
+      <c r="C27" s="118" t="s">
         <v>70</v>
       </c>
       <c r="D27" s="92">
@@ -7688,9 +7690,9 @@
       </c>
     </row>
     <row r="28" spans="1:24">
-      <c r="A28" s="137"/>
-      <c r="B28" s="128"/>
-      <c r="C28" s="130"/>
+      <c r="A28" s="121"/>
+      <c r="B28" s="116"/>
+      <c r="C28" s="118"/>
       <c r="D28" s="92">
         <v>2010</v>
       </c>
@@ -7756,9 +7758,9 @@
       </c>
     </row>
     <row r="29" spans="1:24">
-      <c r="A29" s="137"/>
-      <c r="B29" s="129"/>
-      <c r="C29" s="130"/>
+      <c r="A29" s="121"/>
+      <c r="B29" s="117"/>
+      <c r="C29" s="118"/>
       <c r="D29" s="25">
         <v>2014</v>
       </c>
@@ -7824,7 +7826,7 @@
       </c>
     </row>
     <row r="30" spans="1:24">
-      <c r="A30" s="137"/>
+      <c r="A30" s="121"/>
       <c r="B30" s="91"/>
       <c r="C30" s="95"/>
       <c r="D30" s="25"/>
@@ -7846,11 +7848,11 @@
       <c r="X30" s="106"/>
     </row>
     <row r="31" spans="1:24">
-      <c r="A31" s="137"/>
-      <c r="B31" s="127">
+      <c r="A31" s="121"/>
+      <c r="B31" s="115">
         <v>8</v>
       </c>
-      <c r="C31" s="131" t="s">
+      <c r="C31" s="124" t="s">
         <v>54</v>
       </c>
       <c r="D31" s="92">
@@ -7918,9 +7920,9 @@
       </c>
     </row>
     <row r="32" spans="1:24">
-      <c r="A32" s="137"/>
-      <c r="B32" s="128"/>
-      <c r="C32" s="132"/>
+      <c r="A32" s="121"/>
+      <c r="B32" s="116"/>
+      <c r="C32" s="125"/>
       <c r="D32" s="92">
         <v>2010</v>
       </c>
@@ -7986,9 +7988,9 @@
       </c>
     </row>
     <row r="33" spans="1:24">
-      <c r="A33" s="137"/>
-      <c r="B33" s="129"/>
-      <c r="C33" s="133"/>
+      <c r="A33" s="121"/>
+      <c r="B33" s="117"/>
+      <c r="C33" s="126"/>
       <c r="D33" s="25">
         <v>2014</v>
       </c>
@@ -8054,7 +8056,7 @@
       </c>
     </row>
     <row r="34" spans="1:24">
-      <c r="A34" s="137"/>
+      <c r="A34" s="121"/>
       <c r="B34" s="91"/>
       <c r="C34" s="96"/>
       <c r="D34" s="25"/>
@@ -8076,11 +8078,11 @@
       <c r="X34" s="106"/>
     </row>
     <row r="35" spans="1:24">
-      <c r="A35" s="137"/>
-      <c r="B35" s="127">
+      <c r="A35" s="121"/>
+      <c r="B35" s="115">
         <v>9</v>
       </c>
-      <c r="C35" s="130" t="s">
+      <c r="C35" s="118" t="s">
         <v>12</v>
       </c>
       <c r="D35" s="92">
@@ -8148,9 +8150,9 @@
       </c>
     </row>
     <row r="36" spans="1:24">
-      <c r="A36" s="137"/>
-      <c r="B36" s="128"/>
-      <c r="C36" s="130"/>
+      <c r="A36" s="121"/>
+      <c r="B36" s="116"/>
+      <c r="C36" s="118"/>
       <c r="D36" s="92">
         <v>2010</v>
       </c>
@@ -8216,9 +8218,9 @@
       </c>
     </row>
     <row r="37" spans="1:24">
-      <c r="A37" s="137"/>
-      <c r="B37" s="129"/>
-      <c r="C37" s="130"/>
+      <c r="A37" s="121"/>
+      <c r="B37" s="117"/>
+      <c r="C37" s="118"/>
       <c r="D37" s="25">
         <v>2014</v>
       </c>
@@ -8284,7 +8286,7 @@
       </c>
     </row>
     <row r="38" spans="1:24">
-      <c r="A38" s="137"/>
+      <c r="A38" s="121"/>
       <c r="B38" s="91"/>
       <c r="C38" s="92"/>
       <c r="D38" s="25"/>
@@ -8306,11 +8308,11 @@
       <c r="X38" s="106"/>
     </row>
     <row r="39" spans="1:24">
-      <c r="A39" s="137"/>
-      <c r="B39" s="127">
+      <c r="A39" s="121"/>
+      <c r="B39" s="115">
         <v>10</v>
       </c>
-      <c r="C39" s="130" t="s">
+      <c r="C39" s="118" t="s">
         <v>28</v>
       </c>
       <c r="D39" s="92">
@@ -8378,9 +8380,9 @@
       </c>
     </row>
     <row r="40" spans="1:24">
-      <c r="A40" s="137"/>
-      <c r="B40" s="128"/>
-      <c r="C40" s="130"/>
+      <c r="A40" s="121"/>
+      <c r="B40" s="116"/>
+      <c r="C40" s="118"/>
       <c r="D40" s="92">
         <v>2010</v>
       </c>
@@ -8446,9 +8448,9 @@
       </c>
     </row>
     <row r="41" spans="1:24">
-      <c r="A41" s="137"/>
-      <c r="B41" s="129"/>
-      <c r="C41" s="130"/>
+      <c r="A41" s="121"/>
+      <c r="B41" s="117"/>
+      <c r="C41" s="118"/>
       <c r="D41" s="25">
         <v>2014</v>
       </c>
@@ -8514,7 +8516,7 @@
       </c>
     </row>
     <row r="42" spans="1:24">
-      <c r="A42" s="137"/>
+      <c r="A42" s="121"/>
       <c r="B42" s="91"/>
       <c r="C42" s="92"/>
       <c r="D42" s="25"/>
@@ -8536,11 +8538,11 @@
       <c r="X42" s="106"/>
     </row>
     <row r="43" spans="1:24">
-      <c r="A43" s="137"/>
-      <c r="B43" s="127">
+      <c r="A43" s="121"/>
+      <c r="B43" s="115">
         <v>11</v>
       </c>
-      <c r="C43" s="130" t="s">
+      <c r="C43" s="118" t="s">
         <v>21</v>
       </c>
       <c r="D43" s="92">
@@ -8608,9 +8610,9 @@
       </c>
     </row>
     <row r="44" spans="1:24">
-      <c r="A44" s="137"/>
-      <c r="B44" s="128"/>
-      <c r="C44" s="130"/>
+      <c r="A44" s="121"/>
+      <c r="B44" s="116"/>
+      <c r="C44" s="118"/>
       <c r="D44" s="92">
         <v>2010</v>
       </c>
@@ -8676,9 +8678,9 @@
       </c>
     </row>
     <row r="45" spans="1:24">
-      <c r="A45" s="137"/>
-      <c r="B45" s="129"/>
-      <c r="C45" s="130"/>
+      <c r="A45" s="121"/>
+      <c r="B45" s="117"/>
+      <c r="C45" s="118"/>
       <c r="D45" s="25">
         <v>2014</v>
       </c>
@@ -8744,7 +8746,7 @@
       </c>
     </row>
     <row r="46" spans="1:24">
-      <c r="A46" s="137"/>
+      <c r="A46" s="121"/>
       <c r="B46" s="91"/>
       <c r="C46" s="92"/>
       <c r="D46" s="25"/>
@@ -8766,11 +8768,11 @@
       <c r="X46" s="106"/>
     </row>
     <row r="47" spans="1:24">
-      <c r="A47" s="137"/>
-      <c r="B47" s="127">
+      <c r="A47" s="121"/>
+      <c r="B47" s="115">
         <v>12</v>
       </c>
-      <c r="C47" s="130" t="s">
+      <c r="C47" s="118" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="92">
@@ -8838,9 +8840,9 @@
       </c>
     </row>
     <row r="48" spans="1:24">
-      <c r="A48" s="137"/>
-      <c r="B48" s="128"/>
-      <c r="C48" s="130"/>
+      <c r="A48" s="121"/>
+      <c r="B48" s="116"/>
+      <c r="C48" s="118"/>
       <c r="D48" s="92">
         <v>2010</v>
       </c>
@@ -8906,9 +8908,9 @@
       </c>
     </row>
     <row r="49" spans="1:41">
-      <c r="A49" s="137"/>
-      <c r="B49" s="129"/>
-      <c r="C49" s="130"/>
+      <c r="A49" s="121"/>
+      <c r="B49" s="117"/>
+      <c r="C49" s="118"/>
       <c r="D49" s="25">
         <v>2014</v>
       </c>
@@ -8974,7 +8976,7 @@
       </c>
     </row>
     <row r="50" spans="1:41">
-      <c r="A50" s="137"/>
+      <c r="A50" s="121"/>
       <c r="B50" s="91"/>
       <c r="C50" s="92"/>
       <c r="D50" s="25"/>
@@ -8996,11 +8998,11 @@
       <c r="X50" s="106"/>
     </row>
     <row r="51" spans="1:41">
-      <c r="A51" s="137"/>
-      <c r="B51" s="127">
+      <c r="A51" s="121"/>
+      <c r="B51" s="115">
         <v>13</v>
       </c>
-      <c r="C51" s="130" t="s">
+      <c r="C51" s="118" t="s">
         <v>8</v>
       </c>
       <c r="D51" s="92">
@@ -9068,9 +9070,9 @@
       </c>
     </row>
     <row r="52" spans="1:41">
-      <c r="A52" s="137"/>
-      <c r="B52" s="128"/>
-      <c r="C52" s="130"/>
+      <c r="A52" s="121"/>
+      <c r="B52" s="116"/>
+      <c r="C52" s="118"/>
       <c r="D52" s="92">
         <v>2010</v>
       </c>
@@ -9136,9 +9138,9 @@
       </c>
     </row>
     <row r="53" spans="1:41">
-      <c r="A53" s="137"/>
-      <c r="B53" s="129"/>
-      <c r="C53" s="130"/>
+      <c r="A53" s="121"/>
+      <c r="B53" s="117"/>
+      <c r="C53" s="118"/>
       <c r="D53" s="25">
         <v>2014</v>
       </c>
@@ -9204,79 +9206,79 @@
       </c>
     </row>
     <row r="54" spans="1:41">
-      <c r="A54" s="137"/>
+      <c r="A54" s="121"/>
     </row>
     <row r="55" spans="1:41" s="75" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A55" s="137"/>
+      <c r="A55" s="121"/>
       <c r="B55" s="86"/>
-      <c r="C55" s="114" t="s">
+      <c r="C55" s="130" t="s">
         <v>50</v>
       </c>
-      <c r="D55" s="114"/>
-      <c r="E55" s="114"/>
-      <c r="F55" s="114" t="s">
+      <c r="D55" s="130"/>
+      <c r="E55" s="130"/>
+      <c r="F55" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="G55" s="114"/>
-      <c r="H55" s="114"/>
-      <c r="I55" s="114" t="s">
+      <c r="G55" s="130"/>
+      <c r="H55" s="130"/>
+      <c r="I55" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="J55" s="114"/>
-      <c r="K55" s="114"/>
-      <c r="L55" s="114" t="s">
+      <c r="J55" s="130"/>
+      <c r="K55" s="130"/>
+      <c r="L55" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="M55" s="114"/>
-      <c r="N55" s="114"/>
-      <c r="O55" s="114" t="s">
+      <c r="M55" s="130"/>
+      <c r="N55" s="130"/>
+      <c r="O55" s="130" t="s">
         <v>23</v>
       </c>
-      <c r="P55" s="114"/>
-      <c r="Q55" s="114"/>
-      <c r="R55" s="122" t="s">
+      <c r="P55" s="130"/>
+      <c r="Q55" s="130"/>
+      <c r="R55" s="127" t="s">
         <v>87</v>
       </c>
-      <c r="S55" s="123"/>
-      <c r="T55" s="124"/>
-      <c r="U55" s="114" t="s">
+      <c r="S55" s="128"/>
+      <c r="T55" s="129"/>
+      <c r="U55" s="130" t="s">
         <v>70</v>
       </c>
-      <c r="V55" s="114"/>
-      <c r="W55" s="114"/>
-      <c r="X55" s="122" t="s">
+      <c r="V55" s="130"/>
+      <c r="W55" s="130"/>
+      <c r="X55" s="127" t="s">
         <v>54</v>
       </c>
-      <c r="Y55" s="123"/>
-      <c r="Z55" s="124"/>
-      <c r="AA55" s="114" t="s">
+      <c r="Y55" s="128"/>
+      <c r="Z55" s="129"/>
+      <c r="AA55" s="130" t="s">
         <v>105</v>
       </c>
-      <c r="AB55" s="114"/>
-      <c r="AC55" s="114"/>
-      <c r="AD55" s="114" t="s">
+      <c r="AB55" s="130"/>
+      <c r="AC55" s="130"/>
+      <c r="AD55" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="AE55" s="114"/>
-      <c r="AF55" s="114"/>
-      <c r="AG55" s="114" t="s">
+      <c r="AE55" s="130"/>
+      <c r="AF55" s="130"/>
+      <c r="AG55" s="130" t="s">
         <v>21</v>
       </c>
-      <c r="AH55" s="114"/>
-      <c r="AI55" s="114"/>
-      <c r="AJ55" s="114" t="s">
+      <c r="AH55" s="130"/>
+      <c r="AI55" s="130"/>
+      <c r="AJ55" s="130" t="s">
         <v>13</v>
       </c>
-      <c r="AK55" s="114"/>
-      <c r="AL55" s="114"/>
-      <c r="AM55" s="114" t="s">
+      <c r="AK55" s="130"/>
+      <c r="AL55" s="130"/>
+      <c r="AM55" s="130" t="s">
         <v>8</v>
       </c>
-      <c r="AN55" s="114"/>
-      <c r="AO55" s="114"/>
+      <c r="AN55" s="130"/>
+      <c r="AO55" s="130"/>
     </row>
     <row r="56" spans="1:41" s="75" customFormat="1" ht="70">
-      <c r="A56" s="138"/>
+      <c r="A56" s="122"/>
       <c r="B56" s="86"/>
       <c r="C56" s="86" t="s">
         <v>72</v>
@@ -9517,10 +9519,10 @@
       </c>
     </row>
     <row r="58" spans="1:41" s="79" customFormat="1" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A58" s="125" t="s">
+      <c r="A58" s="131" t="s">
         <v>129</v>
       </c>
-      <c r="B58" s="126"/>
+      <c r="B58" s="132"/>
       <c r="C58" s="79">
         <v>2006</v>
       </c>
@@ -9557,10 +9559,10 @@
       <c r="Y58" s="105"/>
     </row>
     <row r="59" spans="1:41" ht="16" thickTop="1">
-      <c r="A59" s="119" t="s">
+      <c r="A59" s="133" t="s">
         <v>125</v>
       </c>
-      <c r="B59" s="119"/>
+      <c r="B59" s="133"/>
       <c r="C59">
         <f xml:space="preserve"> C57/115</f>
         <v>3.4782608695652174E-2</v>
@@ -9719,10 +9721,10 @@
       </c>
     </row>
     <row r="60" spans="1:41">
-      <c r="A60" s="120" t="s">
+      <c r="A60" s="134" t="s">
         <v>124</v>
       </c>
-      <c r="B60" s="120"/>
+      <c r="B60" s="134"/>
       <c r="C60">
         <f xml:space="preserve"> C59*72</f>
         <v>2.5043478260869567</v>
@@ -9881,10 +9883,10 @@
       </c>
     </row>
     <row r="61" spans="1:41" s="80" customFormat="1">
-      <c r="A61" s="121" t="s">
+      <c r="A61" s="135" t="s">
         <v>126</v>
       </c>
-      <c r="B61" s="121"/>
+      <c r="B61" s="135"/>
       <c r="C61" s="80">
         <f xml:space="preserve"> 72-C60</f>
         <v>69.495652173913044</v>
@@ -10194,77 +10196,77 @@
       <c r="X66" s="85"/>
     </row>
     <row r="67" spans="1:41">
-      <c r="C67" s="114" t="s">
+      <c r="C67" s="130" t="s">
         <v>70</v>
       </c>
-      <c r="D67" s="114"/>
-      <c r="E67" s="114"/>
-      <c r="F67" s="122" t="s">
+      <c r="D67" s="130"/>
+      <c r="E67" s="130"/>
+      <c r="F67" s="127" t="s">
         <v>54</v>
       </c>
-      <c r="G67" s="123"/>
-      <c r="H67" s="124"/>
-      <c r="I67" s="114" t="s">
+      <c r="G67" s="128"/>
+      <c r="H67" s="129"/>
+      <c r="I67" s="130" t="s">
         <v>105</v>
       </c>
-      <c r="J67" s="114"/>
-      <c r="K67" s="114"/>
-      <c r="L67" s="114" t="s">
+      <c r="J67" s="130"/>
+      <c r="K67" s="130"/>
+      <c r="L67" s="130" t="s">
         <v>50</v>
       </c>
-      <c r="M67" s="114"/>
-      <c r="N67" s="114"/>
-      <c r="O67" s="114" t="s">
+      <c r="M67" s="130"/>
+      <c r="N67" s="130"/>
+      <c r="O67" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="P67" s="114"/>
-      <c r="Q67" s="114"/>
-      <c r="R67" s="122" t="s">
+      <c r="P67" s="130"/>
+      <c r="Q67" s="130"/>
+      <c r="R67" s="127" t="s">
         <v>87</v>
       </c>
-      <c r="S67" s="123"/>
-      <c r="T67" s="124"/>
-      <c r="U67" s="114" t="s">
+      <c r="S67" s="128"/>
+      <c r="T67" s="129"/>
+      <c r="U67" s="130" t="s">
         <v>23</v>
       </c>
-      <c r="V67" s="114"/>
-      <c r="W67" s="114"/>
-      <c r="X67" s="114" t="s">
+      <c r="V67" s="130"/>
+      <c r="W67" s="130"/>
+      <c r="X67" s="130" t="s">
         <v>21</v>
       </c>
-      <c r="Y67" s="114"/>
-      <c r="Z67" s="114"/>
-      <c r="AA67" s="114" t="s">
+      <c r="Y67" s="130"/>
+      <c r="Z67" s="130"/>
+      <c r="AA67" s="130" t="s">
         <v>8</v>
       </c>
-      <c r="AB67" s="114"/>
-      <c r="AC67" s="114"/>
-      <c r="AD67" s="114" t="s">
+      <c r="AB67" s="130"/>
+      <c r="AC67" s="130"/>
+      <c r="AD67" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="AE67" s="114"/>
-      <c r="AF67" s="114"/>
-      <c r="AG67" s="114" t="s">
+      <c r="AE67" s="130"/>
+      <c r="AF67" s="130"/>
+      <c r="AG67" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="AH67" s="114"/>
-      <c r="AI67" s="114"/>
-      <c r="AJ67" s="114" t="s">
+      <c r="AH67" s="130"/>
+      <c r="AI67" s="130"/>
+      <c r="AJ67" s="130" t="s">
         <v>13</v>
       </c>
-      <c r="AK67" s="114"/>
-      <c r="AL67" s="114"/>
-      <c r="AM67" s="114" t="s">
+      <c r="AK67" s="130"/>
+      <c r="AL67" s="130"/>
+      <c r="AM67" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="AN67" s="114"/>
-      <c r="AO67" s="114"/>
+      <c r="AN67" s="130"/>
+      <c r="AO67" s="130"/>
     </row>
     <row r="68" spans="1:41" ht="70">
-      <c r="A68" s="115" t="s">
+      <c r="A68" s="136" t="s">
         <v>128</v>
       </c>
-      <c r="B68" s="116"/>
+      <c r="B68" s="137"/>
       <c r="C68" s="86" t="s">
         <v>99</v>
       </c>
@@ -10384,8 +10386,8 @@
       </c>
     </row>
     <row r="69" spans="1:41" ht="16" thickBot="1">
-      <c r="A69" s="117"/>
-      <c r="B69" s="118"/>
+      <c r="A69" s="138"/>
+      <c r="B69" s="139"/>
       <c r="C69" s="86">
         <v>23</v>
       </c>
@@ -10505,10 +10507,10 @@
       </c>
     </row>
     <row r="70" spans="1:41" ht="16" thickTop="1">
-      <c r="A70" s="119" t="s">
+      <c r="A70" s="133" t="s">
         <v>125</v>
       </c>
-      <c r="B70" s="119"/>
+      <c r="B70" s="133"/>
       <c r="C70">
         <f xml:space="preserve"> C69/115</f>
         <v>0.2</v>
@@ -10667,10 +10669,10 @@
       </c>
     </row>
     <row r="71" spans="1:41">
-      <c r="A71" s="120" t="s">
+      <c r="A71" s="134" t="s">
         <v>124</v>
       </c>
-      <c r="B71" s="120"/>
+      <c r="B71" s="134"/>
       <c r="C71">
         <f xml:space="preserve"> C70*65</f>
         <v>13</v>
@@ -10829,10 +10831,10 @@
       </c>
     </row>
     <row r="72" spans="1:41">
-      <c r="A72" s="121" t="s">
+      <c r="A72" s="135" t="s">
         <v>126</v>
       </c>
-      <c r="B72" s="121"/>
+      <c r="B72" s="135"/>
       <c r="C72" s="80">
         <f xml:space="preserve"> 65-C71</f>
         <v>52</v>
@@ -10997,6 +10999,58 @@
     </row>
   </sheetData>
   <mergeCells count="68">
+    <mergeCell ref="AJ67:AL67"/>
+    <mergeCell ref="AM67:AO67"/>
+    <mergeCell ref="A68:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="AD67:AF67"/>
+    <mergeCell ref="AG67:AI67"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="R67:T67"/>
+    <mergeCell ref="U67:W67"/>
+    <mergeCell ref="X67:Z67"/>
+    <mergeCell ref="AA67:AC67"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="I67:K67"/>
+    <mergeCell ref="L67:N67"/>
+    <mergeCell ref="O67:Q67"/>
+    <mergeCell ref="AM55:AO55"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="U55:W55"/>
+    <mergeCell ref="X55:Z55"/>
+    <mergeCell ref="AA55:AC55"/>
+    <mergeCell ref="AD55:AF55"/>
+    <mergeCell ref="AG55:AI55"/>
+    <mergeCell ref="AJ55:AL55"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="I55:K55"/>
+    <mergeCell ref="L55:N55"/>
+    <mergeCell ref="O55:Q55"/>
+    <mergeCell ref="R55:T55"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="C27:C29"/>
@@ -11013,58 +11067,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="R55:T55"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="B51:B53"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="AM55:AO55"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="U55:W55"/>
-    <mergeCell ref="X55:Z55"/>
-    <mergeCell ref="AA55:AC55"/>
-    <mergeCell ref="AD55:AF55"/>
-    <mergeCell ref="AG55:AI55"/>
-    <mergeCell ref="AJ55:AL55"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="I55:K55"/>
-    <mergeCell ref="L55:N55"/>
-    <mergeCell ref="O55:Q55"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="R67:T67"/>
-    <mergeCell ref="U67:W67"/>
-    <mergeCell ref="X67:Z67"/>
-    <mergeCell ref="AA67:AC67"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="I67:K67"/>
-    <mergeCell ref="L67:N67"/>
-    <mergeCell ref="O67:Q67"/>
-    <mergeCell ref="AJ67:AL67"/>
-    <mergeCell ref="AM67:AO67"/>
-    <mergeCell ref="A68:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="AD67:AF67"/>
-    <mergeCell ref="AG67:AI67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -11081,8 +11083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="T21" sqref="T21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11108,37 +11110,37 @@
     <row r="1" spans="1:24" ht="34" customHeight="1">
       <c r="A1" s="57"/>
       <c r="B1" s="57"/>
-      <c r="C1" s="130" t="s">
+      <c r="C1" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="130" t="s">
+      <c r="D1" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="130" t="s">
+      <c r="E1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="139" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="134" t="s">
+      <c r="F1" s="123" t="s">
+        <v>199</v>
+      </c>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="123"/>
+      <c r="J1" s="123"/>
+      <c r="K1" s="119" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="134"/>
-      <c r="M1" s="134"/>
-      <c r="N1" s="134"/>
-      <c r="O1" s="135" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="135"/>
-      <c r="Q1" s="134" t="s">
+      <c r="L1" s="119"/>
+      <c r="M1" s="119"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="114" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="114"/>
+      <c r="Q1" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="134"/>
-      <c r="S1" s="134"/>
+      <c r="R1" s="119"/>
+      <c r="S1" s="119"/>
       <c r="T1" s="71" t="s">
         <v>92</v>
       </c>
@@ -11151,16 +11153,16 @@
       <c r="W1" s="71" t="s">
         <v>133</v>
       </c>
-      <c r="X1" s="130" t="s">
+      <c r="X1" s="118" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="144">
       <c r="A2" s="57"/>
       <c r="B2" s="57"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -11215,16 +11217,16 @@
       <c r="W2" s="72" t="s">
         <v>98</v>
       </c>
-      <c r="X2" s="130"/>
+      <c r="X2" s="118"/>
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="120" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="127">
-        <v>1</v>
-      </c>
-      <c r="C3" s="130" t="s">
+      <c r="B3" s="115">
+        <v>1</v>
+      </c>
+      <c r="C3" s="118" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="54">
@@ -11292,9 +11294,9 @@
       </c>
     </row>
     <row r="4" spans="1:24">
-      <c r="A4" s="137"/>
-      <c r="B4" s="128"/>
-      <c r="C4" s="130"/>
+      <c r="A4" s="121"/>
+      <c r="B4" s="116"/>
+      <c r="C4" s="118"/>
       <c r="D4" s="54">
         <v>2010</v>
       </c>
@@ -11360,9 +11362,9 @@
       </c>
     </row>
     <row r="5" spans="1:24">
-      <c r="A5" s="137"/>
-      <c r="B5" s="129"/>
-      <c r="C5" s="130"/>
+      <c r="A5" s="121"/>
+      <c r="B5" s="117"/>
+      <c r="C5" s="118"/>
       <c r="D5" s="25">
         <v>2014</v>
       </c>
@@ -11428,11 +11430,11 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="15" customHeight="1">
-      <c r="A6" s="137"/>
-      <c r="B6" s="127">
+      <c r="A6" s="121"/>
+      <c r="B6" s="115">
         <v>2</v>
       </c>
-      <c r="C6" s="130" t="s">
+      <c r="C6" s="118" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="54">
@@ -11500,9 +11502,9 @@
       </c>
     </row>
     <row r="7" spans="1:24">
-      <c r="A7" s="137"/>
-      <c r="B7" s="128"/>
-      <c r="C7" s="130"/>
+      <c r="A7" s="121"/>
+      <c r="B7" s="116"/>
+      <c r="C7" s="118"/>
       <c r="D7" s="54">
         <v>2010</v>
       </c>
@@ -11568,9 +11570,9 @@
       </c>
     </row>
     <row r="8" spans="1:24">
-      <c r="A8" s="137"/>
-      <c r="B8" s="129"/>
-      <c r="C8" s="130"/>
+      <c r="A8" s="121"/>
+      <c r="B8" s="117"/>
+      <c r="C8" s="118"/>
       <c r="D8" s="25">
         <v>2014</v>
       </c>
@@ -11636,11 +11638,11 @@
       </c>
     </row>
     <row r="9" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A9" s="137"/>
-      <c r="B9" s="127">
+      <c r="A9" s="121"/>
+      <c r="B9" s="115">
         <v>3</v>
       </c>
-      <c r="C9" s="130" t="s">
+      <c r="C9" s="118" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="54">
@@ -11708,9 +11710,9 @@
       </c>
     </row>
     <row r="10" spans="1:24">
-      <c r="A10" s="137"/>
-      <c r="B10" s="128"/>
-      <c r="C10" s="130"/>
+      <c r="A10" s="121"/>
+      <c r="B10" s="116"/>
+      <c r="C10" s="118"/>
       <c r="D10" s="54">
         <v>2010</v>
       </c>
@@ -11776,9 +11778,9 @@
       </c>
     </row>
     <row r="11" spans="1:24">
-      <c r="A11" s="137"/>
-      <c r="B11" s="129"/>
-      <c r="C11" s="130"/>
+      <c r="A11" s="121"/>
+      <c r="B11" s="117"/>
+      <c r="C11" s="118"/>
       <c r="D11" s="25">
         <v>2014</v>
       </c>
@@ -11844,11 +11846,11 @@
       </c>
     </row>
     <row r="12" spans="1:24">
-      <c r="A12" s="137"/>
-      <c r="B12" s="127">
+      <c r="A12" s="121"/>
+      <c r="B12" s="115">
         <v>4</v>
       </c>
-      <c r="C12" s="130" t="s">
+      <c r="C12" s="118" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="54">
@@ -11916,9 +11918,9 @@
       </c>
     </row>
     <row r="13" spans="1:24">
-      <c r="A13" s="137"/>
-      <c r="B13" s="128"/>
-      <c r="C13" s="130"/>
+      <c r="A13" s="121"/>
+      <c r="B13" s="116"/>
+      <c r="C13" s="118"/>
       <c r="D13" s="54">
         <v>2010</v>
       </c>
@@ -11984,9 +11986,9 @@
       </c>
     </row>
     <row r="14" spans="1:24">
-      <c r="A14" s="137"/>
-      <c r="B14" s="129"/>
-      <c r="C14" s="130"/>
+      <c r="A14" s="121"/>
+      <c r="B14" s="117"/>
+      <c r="C14" s="118"/>
       <c r="D14" s="25">
         <v>2014</v>
       </c>
@@ -12052,11 +12054,11 @@
       </c>
     </row>
     <row r="15" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A15" s="137"/>
-      <c r="B15" s="127">
+      <c r="A15" s="121"/>
+      <c r="B15" s="115">
         <v>5</v>
       </c>
-      <c r="C15" s="130" t="s">
+      <c r="C15" s="118" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="54">
@@ -12124,9 +12126,9 @@
       </c>
     </row>
     <row r="16" spans="1:24">
-      <c r="A16" s="137"/>
-      <c r="B16" s="128"/>
-      <c r="C16" s="130"/>
+      <c r="A16" s="121"/>
+      <c r="B16" s="116"/>
+      <c r="C16" s="118"/>
       <c r="D16" s="54">
         <v>2010</v>
       </c>
@@ -12192,9 +12194,9 @@
       </c>
     </row>
     <row r="17" spans="1:24">
-      <c r="A17" s="137"/>
-      <c r="B17" s="129"/>
-      <c r="C17" s="130"/>
+      <c r="A17" s="121"/>
+      <c r="B17" s="117"/>
+      <c r="C17" s="118"/>
       <c r="D17" s="25">
         <v>2014</v>
       </c>
@@ -12260,11 +12262,11 @@
       </c>
     </row>
     <row r="18" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A18" s="137"/>
-      <c r="B18" s="127">
+      <c r="A18" s="121"/>
+      <c r="B18" s="115">
         <v>6</v>
       </c>
-      <c r="C18" s="130" t="s">
+      <c r="C18" s="118" t="s">
         <v>25</v>
       </c>
       <c r="D18" s="54">
@@ -12332,9 +12334,9 @@
       </c>
     </row>
     <row r="19" spans="1:24">
-      <c r="A19" s="137"/>
-      <c r="B19" s="128"/>
-      <c r="C19" s="130"/>
+      <c r="A19" s="121"/>
+      <c r="B19" s="116"/>
+      <c r="C19" s="118"/>
       <c r="D19" s="54">
         <v>2010</v>
       </c>
@@ -12400,9 +12402,9 @@
       </c>
     </row>
     <row r="20" spans="1:24">
-      <c r="A20" s="137"/>
-      <c r="B20" s="129"/>
-      <c r="C20" s="130"/>
+      <c r="A20" s="121"/>
+      <c r="B20" s="117"/>
+      <c r="C20" s="118"/>
       <c r="D20" s="25">
         <v>2014</v>
       </c>
@@ -12468,11 +12470,11 @@
       </c>
     </row>
     <row r="21" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A21" s="137"/>
-      <c r="B21" s="127">
+      <c r="A21" s="121"/>
+      <c r="B21" s="115">
         <v>7</v>
       </c>
-      <c r="C21" s="130" t="s">
+      <c r="C21" s="118" t="s">
         <v>70</v>
       </c>
       <c r="D21" s="54">
@@ -12540,9 +12542,9 @@
       </c>
     </row>
     <row r="22" spans="1:24">
-      <c r="A22" s="137"/>
-      <c r="B22" s="128"/>
-      <c r="C22" s="130"/>
+      <c r="A22" s="121"/>
+      <c r="B22" s="116"/>
+      <c r="C22" s="118"/>
       <c r="D22" s="54">
         <v>2010</v>
       </c>
@@ -12608,9 +12610,9 @@
       </c>
     </row>
     <row r="23" spans="1:24">
-      <c r="A23" s="137"/>
-      <c r="B23" s="129"/>
-      <c r="C23" s="130"/>
+      <c r="A23" s="121"/>
+      <c r="B23" s="117"/>
+      <c r="C23" s="118"/>
       <c r="D23" s="25">
         <v>2014</v>
       </c>
@@ -12676,11 +12678,11 @@
       </c>
     </row>
     <row r="24" spans="1:24">
-      <c r="A24" s="137"/>
-      <c r="B24" s="127">
+      <c r="A24" s="121"/>
+      <c r="B24" s="115">
         <v>8</v>
       </c>
-      <c r="C24" s="131" t="s">
+      <c r="C24" s="124" t="s">
         <v>54</v>
       </c>
       <c r="D24" s="54">
@@ -12748,9 +12750,9 @@
       </c>
     </row>
     <row r="25" spans="1:24">
-      <c r="A25" s="137"/>
-      <c r="B25" s="128"/>
-      <c r="C25" s="132"/>
+      <c r="A25" s="121"/>
+      <c r="B25" s="116"/>
+      <c r="C25" s="125"/>
       <c r="D25" s="54">
         <v>2010</v>
       </c>
@@ -12816,9 +12818,9 @@
       </c>
     </row>
     <row r="26" spans="1:24">
-      <c r="A26" s="137"/>
-      <c r="B26" s="129"/>
-      <c r="C26" s="133"/>
+      <c r="A26" s="121"/>
+      <c r="B26" s="117"/>
+      <c r="C26" s="126"/>
       <c r="D26" s="25">
         <v>2014</v>
       </c>
@@ -12884,11 +12886,11 @@
       </c>
     </row>
     <row r="27" spans="1:24">
-      <c r="A27" s="137"/>
-      <c r="B27" s="127">
+      <c r="A27" s="121"/>
+      <c r="B27" s="115">
         <v>9</v>
       </c>
-      <c r="C27" s="130" t="s">
+      <c r="C27" s="118" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="54">
@@ -12956,9 +12958,9 @@
       </c>
     </row>
     <row r="28" spans="1:24">
-      <c r="A28" s="137"/>
-      <c r="B28" s="128"/>
-      <c r="C28" s="130"/>
+      <c r="A28" s="121"/>
+      <c r="B28" s="116"/>
+      <c r="C28" s="118"/>
       <c r="D28" s="54">
         <v>2010</v>
       </c>
@@ -13024,9 +13026,9 @@
       </c>
     </row>
     <row r="29" spans="1:24">
-      <c r="A29" s="137"/>
-      <c r="B29" s="129"/>
-      <c r="C29" s="130"/>
+      <c r="A29" s="121"/>
+      <c r="B29" s="117"/>
+      <c r="C29" s="118"/>
       <c r="D29" s="25">
         <v>2014</v>
       </c>
@@ -13092,11 +13094,11 @@
       </c>
     </row>
     <row r="30" spans="1:24">
-      <c r="A30" s="137"/>
-      <c r="B30" s="127">
+      <c r="A30" s="121"/>
+      <c r="B30" s="115">
         <v>10</v>
       </c>
-      <c r="C30" s="130" t="s">
+      <c r="C30" s="118" t="s">
         <v>28</v>
       </c>
       <c r="D30" s="54">
@@ -13164,9 +13166,9 @@
       </c>
     </row>
     <row r="31" spans="1:24">
-      <c r="A31" s="137"/>
-      <c r="B31" s="128"/>
-      <c r="C31" s="130"/>
+      <c r="A31" s="121"/>
+      <c r="B31" s="116"/>
+      <c r="C31" s="118"/>
       <c r="D31" s="54">
         <v>2010</v>
       </c>
@@ -13232,9 +13234,9 @@
       </c>
     </row>
     <row r="32" spans="1:24">
-      <c r="A32" s="137"/>
-      <c r="B32" s="129"/>
-      <c r="C32" s="130"/>
+      <c r="A32" s="121"/>
+      <c r="B32" s="117"/>
+      <c r="C32" s="118"/>
       <c r="D32" s="25">
         <v>2014</v>
       </c>
@@ -13300,11 +13302,11 @@
       </c>
     </row>
     <row r="33" spans="1:41">
-      <c r="A33" s="137"/>
-      <c r="B33" s="127">
+      <c r="A33" s="121"/>
+      <c r="B33" s="115">
         <v>11</v>
       </c>
-      <c r="C33" s="130" t="s">
+      <c r="C33" s="118" t="s">
         <v>21</v>
       </c>
       <c r="D33" s="54">
@@ -13372,9 +13374,9 @@
       </c>
     </row>
     <row r="34" spans="1:41">
-      <c r="A34" s="137"/>
-      <c r="B34" s="128"/>
-      <c r="C34" s="130"/>
+      <c r="A34" s="121"/>
+      <c r="B34" s="116"/>
+      <c r="C34" s="118"/>
       <c r="D34" s="54">
         <v>2010</v>
       </c>
@@ -13440,9 +13442,9 @@
       </c>
     </row>
     <row r="35" spans="1:41">
-      <c r="A35" s="137"/>
-      <c r="B35" s="129"/>
-      <c r="C35" s="130"/>
+      <c r="A35" s="121"/>
+      <c r="B35" s="117"/>
+      <c r="C35" s="118"/>
       <c r="D35" s="25">
         <v>2014</v>
       </c>
@@ -13508,11 +13510,11 @@
       </c>
     </row>
     <row r="36" spans="1:41">
-      <c r="A36" s="137"/>
-      <c r="B36" s="127">
+      <c r="A36" s="121"/>
+      <c r="B36" s="115">
         <v>12</v>
       </c>
-      <c r="C36" s="130" t="s">
+      <c r="C36" s="118" t="s">
         <v>13</v>
       </c>
       <c r="D36" s="54">
@@ -13580,9 +13582,9 @@
       </c>
     </row>
     <row r="37" spans="1:41">
-      <c r="A37" s="137"/>
-      <c r="B37" s="128"/>
-      <c r="C37" s="130"/>
+      <c r="A37" s="121"/>
+      <c r="B37" s="116"/>
+      <c r="C37" s="118"/>
       <c r="D37" s="54">
         <v>2010</v>
       </c>
@@ -13648,9 +13650,9 @@
       </c>
     </row>
     <row r="38" spans="1:41">
-      <c r="A38" s="137"/>
-      <c r="B38" s="129"/>
-      <c r="C38" s="130"/>
+      <c r="A38" s="121"/>
+      <c r="B38" s="117"/>
+      <c r="C38" s="118"/>
       <c r="D38" s="25">
         <v>2014</v>
       </c>
@@ -13716,11 +13718,11 @@
       </c>
     </row>
     <row r="39" spans="1:41">
-      <c r="A39" s="137"/>
-      <c r="B39" s="127">
+      <c r="A39" s="121"/>
+      <c r="B39" s="115">
         <v>13</v>
       </c>
-      <c r="C39" s="130" t="s">
+      <c r="C39" s="118" t="s">
         <v>8</v>
       </c>
       <c r="D39" s="54">
@@ -13788,9 +13790,9 @@
       </c>
     </row>
     <row r="40" spans="1:41">
-      <c r="A40" s="137"/>
-      <c r="B40" s="128"/>
-      <c r="C40" s="130"/>
+      <c r="A40" s="121"/>
+      <c r="B40" s="116"/>
+      <c r="C40" s="118"/>
       <c r="D40" s="54">
         <v>2010</v>
       </c>
@@ -13856,9 +13858,9 @@
       </c>
     </row>
     <row r="41" spans="1:41">
-      <c r="A41" s="137"/>
-      <c r="B41" s="129"/>
-      <c r="C41" s="130"/>
+      <c r="A41" s="121"/>
+      <c r="B41" s="117"/>
+      <c r="C41" s="118"/>
       <c r="D41" s="25">
         <v>2014</v>
       </c>
@@ -13924,79 +13926,79 @@
       </c>
     </row>
     <row r="42" spans="1:41">
-      <c r="A42" s="137"/>
+      <c r="A42" s="121"/>
     </row>
     <row r="43" spans="1:41" s="75" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A43" s="137"/>
+      <c r="A43" s="121"/>
       <c r="B43" s="73"/>
-      <c r="C43" s="114" t="s">
+      <c r="C43" s="130" t="s">
         <v>50</v>
       </c>
-      <c r="D43" s="114"/>
-      <c r="E43" s="114"/>
-      <c r="F43" s="114" t="s">
+      <c r="D43" s="130"/>
+      <c r="E43" s="130"/>
+      <c r="F43" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="G43" s="114"/>
-      <c r="H43" s="114"/>
-      <c r="I43" s="114" t="s">
+      <c r="G43" s="130"/>
+      <c r="H43" s="130"/>
+      <c r="I43" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="J43" s="114"/>
-      <c r="K43" s="114"/>
-      <c r="L43" s="114" t="s">
+      <c r="J43" s="130"/>
+      <c r="K43" s="130"/>
+      <c r="L43" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="M43" s="114"/>
-      <c r="N43" s="114"/>
-      <c r="O43" s="114" t="s">
+      <c r="M43" s="130"/>
+      <c r="N43" s="130"/>
+      <c r="O43" s="130" t="s">
         <v>23</v>
       </c>
-      <c r="P43" s="114"/>
-      <c r="Q43" s="114"/>
-      <c r="R43" s="122" t="s">
+      <c r="P43" s="130"/>
+      <c r="Q43" s="130"/>
+      <c r="R43" s="127" t="s">
         <v>87</v>
       </c>
-      <c r="S43" s="123"/>
-      <c r="T43" s="124"/>
-      <c r="U43" s="114" t="s">
+      <c r="S43" s="128"/>
+      <c r="T43" s="129"/>
+      <c r="U43" s="130" t="s">
         <v>70</v>
       </c>
-      <c r="V43" s="114"/>
-      <c r="W43" s="114"/>
-      <c r="X43" s="122" t="s">
+      <c r="V43" s="130"/>
+      <c r="W43" s="130"/>
+      <c r="X43" s="127" t="s">
         <v>54</v>
       </c>
-      <c r="Y43" s="123"/>
-      <c r="Z43" s="124"/>
-      <c r="AA43" s="114" t="s">
+      <c r="Y43" s="128"/>
+      <c r="Z43" s="129"/>
+      <c r="AA43" s="130" t="s">
         <v>105</v>
       </c>
-      <c r="AB43" s="114"/>
-      <c r="AC43" s="114"/>
-      <c r="AD43" s="114" t="s">
+      <c r="AB43" s="130"/>
+      <c r="AC43" s="130"/>
+      <c r="AD43" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="AE43" s="114"/>
-      <c r="AF43" s="114"/>
-      <c r="AG43" s="114" t="s">
+      <c r="AE43" s="130"/>
+      <c r="AF43" s="130"/>
+      <c r="AG43" s="130" t="s">
         <v>21</v>
       </c>
-      <c r="AH43" s="114"/>
-      <c r="AI43" s="114"/>
-      <c r="AJ43" s="114" t="s">
+      <c r="AH43" s="130"/>
+      <c r="AI43" s="130"/>
+      <c r="AJ43" s="130" t="s">
         <v>13</v>
       </c>
-      <c r="AK43" s="114"/>
-      <c r="AL43" s="114"/>
-      <c r="AM43" s="114" t="s">
+      <c r="AK43" s="130"/>
+      <c r="AL43" s="130"/>
+      <c r="AM43" s="130" t="s">
         <v>8</v>
       </c>
-      <c r="AN43" s="114"/>
-      <c r="AO43" s="114"/>
+      <c r="AN43" s="130"/>
+      <c r="AO43" s="130"/>
     </row>
     <row r="44" spans="1:41" s="75" customFormat="1" ht="70">
-      <c r="A44" s="138"/>
+      <c r="A44" s="122"/>
       <c r="B44" s="73"/>
       <c r="C44" s="73" t="s">
         <v>72</v>
@@ -14237,10 +14239,10 @@
       </c>
     </row>
     <row r="46" spans="1:41" s="79" customFormat="1" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A46" s="125" t="s">
+      <c r="A46" s="131" t="s">
         <v>129</v>
       </c>
-      <c r="B46" s="126"/>
+      <c r="B46" s="132"/>
       <c r="C46" s="79">
         <v>2006</v>
       </c>
@@ -14277,10 +14279,10 @@
       <c r="Y46" s="105"/>
     </row>
     <row r="47" spans="1:41" ht="16" thickTop="1">
-      <c r="A47" s="119" t="s">
+      <c r="A47" s="133" t="s">
         <v>125</v>
       </c>
-      <c r="B47" s="119"/>
+      <c r="B47" s="133"/>
       <c r="C47">
         <f xml:space="preserve"> C45/115</f>
         <v>3.4782608695652174E-2</v>
@@ -14439,10 +14441,10 @@
       </c>
     </row>
     <row r="48" spans="1:41">
-      <c r="A48" s="120" t="s">
+      <c r="A48" s="134" t="s">
         <v>124</v>
       </c>
-      <c r="B48" s="120"/>
+      <c r="B48" s="134"/>
       <c r="C48">
         <f xml:space="preserve"> C47*72</f>
         <v>2.5043478260869567</v>
@@ -14601,10 +14603,10 @@
       </c>
     </row>
     <row r="49" spans="1:41" s="80" customFormat="1">
-      <c r="A49" s="121" t="s">
+      <c r="A49" s="135" t="s">
         <v>126</v>
       </c>
-      <c r="B49" s="121"/>
+      <c r="B49" s="135"/>
       <c r="C49" s="80">
         <f xml:space="preserve"> 72-C48</f>
         <v>69.495652173913044</v>
@@ -14914,77 +14916,77 @@
       <c r="X54" s="85"/>
     </row>
     <row r="55" spans="1:41">
-      <c r="C55" s="114" t="s">
+      <c r="C55" s="130" t="s">
         <v>70</v>
       </c>
-      <c r="D55" s="114"/>
-      <c r="E55" s="114"/>
-      <c r="F55" s="122" t="s">
+      <c r="D55" s="130"/>
+      <c r="E55" s="130"/>
+      <c r="F55" s="127" t="s">
         <v>54</v>
       </c>
-      <c r="G55" s="123"/>
-      <c r="H55" s="124"/>
-      <c r="I55" s="114" t="s">
+      <c r="G55" s="128"/>
+      <c r="H55" s="129"/>
+      <c r="I55" s="130" t="s">
         <v>105</v>
       </c>
-      <c r="J55" s="114"/>
-      <c r="K55" s="114"/>
-      <c r="L55" s="114" t="s">
+      <c r="J55" s="130"/>
+      <c r="K55" s="130"/>
+      <c r="L55" s="130" t="s">
         <v>50</v>
       </c>
-      <c r="M55" s="114"/>
-      <c r="N55" s="114"/>
-      <c r="O55" s="114" t="s">
+      <c r="M55" s="130"/>
+      <c r="N55" s="130"/>
+      <c r="O55" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="P55" s="114"/>
-      <c r="Q55" s="114"/>
-      <c r="R55" s="122" t="s">
+      <c r="P55" s="130"/>
+      <c r="Q55" s="130"/>
+      <c r="R55" s="127" t="s">
         <v>87</v>
       </c>
-      <c r="S55" s="123"/>
-      <c r="T55" s="124"/>
-      <c r="U55" s="114" t="s">
+      <c r="S55" s="128"/>
+      <c r="T55" s="129"/>
+      <c r="U55" s="130" t="s">
         <v>23</v>
       </c>
-      <c r="V55" s="114"/>
-      <c r="W55" s="114"/>
-      <c r="X55" s="114" t="s">
+      <c r="V55" s="130"/>
+      <c r="W55" s="130"/>
+      <c r="X55" s="130" t="s">
         <v>21</v>
       </c>
-      <c r="Y55" s="114"/>
-      <c r="Z55" s="114"/>
-      <c r="AA55" s="114" t="s">
+      <c r="Y55" s="130"/>
+      <c r="Z55" s="130"/>
+      <c r="AA55" s="130" t="s">
         <v>8</v>
       </c>
-      <c r="AB55" s="114"/>
-      <c r="AC55" s="114"/>
-      <c r="AD55" s="114" t="s">
+      <c r="AB55" s="130"/>
+      <c r="AC55" s="130"/>
+      <c r="AD55" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="AE55" s="114"/>
-      <c r="AF55" s="114"/>
-      <c r="AG55" s="114" t="s">
+      <c r="AE55" s="130"/>
+      <c r="AF55" s="130"/>
+      <c r="AG55" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="AH55" s="114"/>
-      <c r="AI55" s="114"/>
-      <c r="AJ55" s="114" t="s">
+      <c r="AH55" s="130"/>
+      <c r="AI55" s="130"/>
+      <c r="AJ55" s="130" t="s">
         <v>13</v>
       </c>
-      <c r="AK55" s="114"/>
-      <c r="AL55" s="114"/>
-      <c r="AM55" s="114" t="s">
+      <c r="AK55" s="130"/>
+      <c r="AL55" s="130"/>
+      <c r="AM55" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="AN55" s="114"/>
-      <c r="AO55" s="114"/>
+      <c r="AN55" s="130"/>
+      <c r="AO55" s="130"/>
     </row>
     <row r="56" spans="1:41" ht="70">
-      <c r="A56" s="115" t="s">
+      <c r="A56" s="136" t="s">
         <v>128</v>
       </c>
-      <c r="B56" s="116"/>
+      <c r="B56" s="137"/>
       <c r="C56" s="74" t="s">
         <v>99</v>
       </c>
@@ -15104,8 +15106,8 @@
       </c>
     </row>
     <row r="57" spans="1:41" ht="16" thickBot="1">
-      <c r="A57" s="117"/>
-      <c r="B57" s="118"/>
+      <c r="A57" s="138"/>
+      <c r="B57" s="139"/>
       <c r="C57" s="74">
         <v>23</v>
       </c>
@@ -15225,10 +15227,10 @@
       </c>
     </row>
     <row r="58" spans="1:41" ht="16" thickTop="1">
-      <c r="A58" s="119" t="s">
+      <c r="A58" s="133" t="s">
         <v>125</v>
       </c>
-      <c r="B58" s="119"/>
+      <c r="B58" s="133"/>
       <c r="C58">
         <f xml:space="preserve"> C57/115</f>
         <v>0.2</v>
@@ -15387,10 +15389,10 @@
       </c>
     </row>
     <row r="59" spans="1:41">
-      <c r="A59" s="120" t="s">
+      <c r="A59" s="134" t="s">
         <v>124</v>
       </c>
-      <c r="B59" s="120"/>
+      <c r="B59" s="134"/>
       <c r="C59">
         <f xml:space="preserve"> C58*65</f>
         <v>13</v>
@@ -15549,10 +15551,10 @@
       </c>
     </row>
     <row r="60" spans="1:41">
-      <c r="A60" s="121" t="s">
+      <c r="A60" s="135" t="s">
         <v>126</v>
       </c>
-      <c r="B60" s="121"/>
+      <c r="B60" s="135"/>
       <c r="C60" s="80">
         <f xml:space="preserve"> 65-C59</f>
         <v>52</v>
@@ -15717,14 +15719,51 @@
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A56:B57"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="AG55:AI55"/>
+    <mergeCell ref="AJ55:AL55"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="O55:Q55"/>
+    <mergeCell ref="U55:W55"/>
+    <mergeCell ref="X55:Z55"/>
+    <mergeCell ref="AA55:AC55"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="I55:K55"/>
+    <mergeCell ref="L55:N55"/>
+    <mergeCell ref="R55:T55"/>
+    <mergeCell ref="AM55:AO55"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="AD55:AF55"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="AD43:AF43"/>
+    <mergeCell ref="AG43:AI43"/>
+    <mergeCell ref="AJ43:AL43"/>
+    <mergeCell ref="AM43:AO43"/>
+    <mergeCell ref="X43:Z43"/>
+    <mergeCell ref="AA43:AC43"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:S1"/>
     <mergeCell ref="A48:B48"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="L43:N43"/>
@@ -15741,51 +15780,14 @@
     <mergeCell ref="C30:C32"/>
     <mergeCell ref="B33:B35"/>
     <mergeCell ref="C33:C35"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="AD43:AF43"/>
-    <mergeCell ref="AG43:AI43"/>
-    <mergeCell ref="AJ43:AL43"/>
-    <mergeCell ref="AM43:AO43"/>
-    <mergeCell ref="X43:Z43"/>
-    <mergeCell ref="AA43:AC43"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="AM55:AO55"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="AD55:AF55"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A56:B57"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="AG55:AI55"/>
-    <mergeCell ref="AJ55:AL55"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="O55:Q55"/>
-    <mergeCell ref="U55:W55"/>
-    <mergeCell ref="X55:Z55"/>
-    <mergeCell ref="AA55:AC55"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="I55:K55"/>
-    <mergeCell ref="L55:N55"/>
-    <mergeCell ref="R55:T55"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -15815,44 +15817,44 @@
     <row r="1" spans="1:19">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="130" t="s">
+      <c r="C1" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="130" t="s">
+      <c r="D1" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="130" t="s">
+      <c r="E1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="139" t="s">
+      <c r="F1" s="123" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="134" t="s">
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="123"/>
+      <c r="J1" s="123"/>
+      <c r="K1" s="119" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="134"/>
-      <c r="M1" s="134"/>
-      <c r="N1" s="134"/>
-      <c r="O1" s="135" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="135"/>
-      <c r="Q1" s="134" t="s">
+      <c r="L1" s="119"/>
+      <c r="M1" s="119"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="114" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="114"/>
+      <c r="Q1" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="134"/>
-      <c r="S1" s="134"/>
+      <c r="R1" s="119"/>
+      <c r="S1" s="119"/>
     </row>
     <row r="2" spans="1:19" ht="84">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -15897,7 +15899,7 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="120" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="47" t="s">
@@ -15956,7 +15958,7 @@
       </c>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="137"/>
+      <c r="A4" s="121"/>
       <c r="B4" s="45" t="s">
         <v>55</v>
       </c>
@@ -16013,7 +16015,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A5" s="137"/>
+      <c r="A5" s="121"/>
       <c r="B5" s="45" t="s">
         <v>57</v>
       </c>
@@ -16070,7 +16072,7 @@
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="137"/>
+      <c r="A6" s="121"/>
       <c r="B6" s="45" t="s">
         <v>58</v>
       </c>
@@ -16127,7 +16129,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A7" s="137"/>
+      <c r="A7" s="121"/>
       <c r="B7" s="45" t="s">
         <v>59</v>
       </c>
@@ -16184,7 +16186,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A8" s="137"/>
+      <c r="A8" s="121"/>
       <c r="B8" s="45" t="s">
         <v>60</v>
       </c>
@@ -16241,7 +16243,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A9" s="137"/>
+      <c r="A9" s="121"/>
       <c r="B9" s="45" t="s">
         <v>61</v>
       </c>
@@ -16298,7 +16300,7 @@
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="137"/>
+      <c r="A10" s="121"/>
       <c r="B10" s="45" t="s">
         <v>62</v>
       </c>
@@ -16355,7 +16357,7 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="137"/>
+      <c r="A11" s="121"/>
       <c r="B11" s="45" t="s">
         <v>56</v>
       </c>
@@ -16412,7 +16414,7 @@
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="137"/>
+      <c r="A12" s="121"/>
       <c r="B12" s="45" t="s">
         <v>63</v>
       </c>
@@ -16469,7 +16471,7 @@
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="137"/>
+      <c r="A13" s="121"/>
       <c r="B13" s="45" t="s">
         <v>64</v>
       </c>
@@ -16526,7 +16528,7 @@
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="137"/>
+      <c r="A14" s="121"/>
       <c r="B14" s="45" t="s">
         <v>65</v>
       </c>
@@ -16583,7 +16585,7 @@
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="137"/>
+      <c r="A15" s="121"/>
       <c r="B15" s="45" t="s">
         <v>66</v>
       </c>
@@ -17345,44 +17347,44 @@
     <row r="1" spans="1:19">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="130" t="s">
+      <c r="C1" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="130" t="s">
+      <c r="D1" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="130" t="s">
+      <c r="E1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="139" t="s">
+      <c r="F1" s="123" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="134" t="s">
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="123"/>
+      <c r="J1" s="123"/>
+      <c r="K1" s="119" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="134"/>
-      <c r="M1" s="134"/>
-      <c r="N1" s="134"/>
-      <c r="O1" s="135" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="135"/>
-      <c r="Q1" s="134" t="s">
+      <c r="L1" s="119"/>
+      <c r="M1" s="119"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="114" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="114"/>
+      <c r="Q1" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="134"/>
-      <c r="S1" s="134"/>
+      <c r="R1" s="119"/>
+      <c r="S1" s="119"/>
     </row>
     <row r="2" spans="1:19" ht="84">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -17427,7 +17429,7 @@
       </c>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="120" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="44" t="s">
@@ -17486,7 +17488,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="24">
-      <c r="A4" s="137"/>
+      <c r="A4" s="121"/>
       <c r="B4" s="45" t="s">
         <v>55</v>
       </c>
@@ -17543,7 +17545,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="25.5" customHeight="1">
-      <c r="A5" s="137"/>
+      <c r="A5" s="121"/>
       <c r="B5" s="45" t="s">
         <v>57</v>
       </c>
@@ -17600,7 +17602,7 @@
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="137"/>
+      <c r="A6" s="121"/>
       <c r="B6" s="45" t="s">
         <v>58</v>
       </c>
@@ -17657,7 +17659,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="25.5" customHeight="1">
-      <c r="A7" s="137"/>
+      <c r="A7" s="121"/>
       <c r="B7" s="45" t="s">
         <v>59</v>
       </c>
@@ -17714,7 +17716,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="24">
-      <c r="A8" s="137"/>
+      <c r="A8" s="121"/>
       <c r="B8" s="45" t="s">
         <v>60</v>
       </c>
@@ -17771,7 +17773,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="25.5" customHeight="1">
-      <c r="A9" s="137"/>
+      <c r="A9" s="121"/>
       <c r="B9" s="45" t="s">
         <v>61</v>
       </c>
@@ -17828,7 +17830,7 @@
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="137"/>
+      <c r="A10" s="121"/>
       <c r="B10" s="45" t="s">
         <v>62</v>
       </c>
@@ -17885,7 +17887,7 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="137"/>
+      <c r="A11" s="121"/>
       <c r="B11" s="45" t="s">
         <v>56</v>
       </c>
@@ -17942,7 +17944,7 @@
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="137"/>
+      <c r="A12" s="121"/>
       <c r="B12" s="45" t="s">
         <v>63</v>
       </c>
@@ -17999,7 +18001,7 @@
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="137"/>
+      <c r="A13" s="121"/>
       <c r="B13" s="45" t="s">
         <v>64</v>
       </c>
@@ -18056,7 +18058,7 @@
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="137"/>
+      <c r="A14" s="121"/>
       <c r="B14" s="45" t="s">
         <v>65</v>
       </c>
@@ -18113,7 +18115,7 @@
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="137"/>
+      <c r="A15" s="121"/>
       <c r="B15" s="45" t="s">
         <v>66</v>
       </c>
@@ -18927,44 +18929,44 @@
     <row r="1" spans="1:19">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="130" t="s">
+      <c r="C1" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="130" t="s">
+      <c r="D1" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="130" t="s">
+      <c r="E1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="139" t="s">
+      <c r="F1" s="123" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="134" t="s">
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="123"/>
+      <c r="J1" s="123"/>
+      <c r="K1" s="119" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="134"/>
-      <c r="M1" s="134"/>
-      <c r="N1" s="134"/>
-      <c r="O1" s="135" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="135"/>
-      <c r="Q1" s="134" t="s">
+      <c r="L1" s="119"/>
+      <c r="M1" s="119"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="114" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="114"/>
+      <c r="Q1" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="134"/>
-      <c r="S1" s="134"/>
+      <c r="R1" s="119"/>
+      <c r="S1" s="119"/>
     </row>
     <row r="2" spans="1:19" ht="84">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -19009,7 +19011,7 @@
       </c>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="120" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="44" t="s">
@@ -19068,7 +19070,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="24">
-      <c r="A4" s="137"/>
+      <c r="A4" s="121"/>
       <c r="B4" s="45" t="s">
         <v>55</v>
       </c>
@@ -19125,7 +19127,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="24">
-      <c r="A5" s="137"/>
+      <c r="A5" s="121"/>
       <c r="B5" s="45" t="s">
         <v>57</v>
       </c>
@@ -19182,7 +19184,7 @@
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="137"/>
+      <c r="A6" s="121"/>
       <c r="B6" s="45" t="s">
         <v>58</v>
       </c>
@@ -19239,7 +19241,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="24">
-      <c r="A7" s="137"/>
+      <c r="A7" s="121"/>
       <c r="B7" s="45" t="s">
         <v>59</v>
       </c>
@@ -19296,7 +19298,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="24">
-      <c r="A8" s="137"/>
+      <c r="A8" s="121"/>
       <c r="B8" s="45" t="s">
         <v>60</v>
       </c>
@@ -19353,7 +19355,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="24">
-      <c r="A9" s="137"/>
+      <c r="A9" s="121"/>
       <c r="B9" s="45" t="s">
         <v>61</v>
       </c>
@@ -19410,7 +19412,7 @@
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="137"/>
+      <c r="A10" s="121"/>
       <c r="B10" s="45" t="s">
         <v>62</v>
       </c>
@@ -19467,7 +19469,7 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="137"/>
+      <c r="A11" s="121"/>
       <c r="B11" s="45" t="s">
         <v>56</v>
       </c>
@@ -19524,7 +19526,7 @@
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="137"/>
+      <c r="A12" s="121"/>
       <c r="B12" s="45" t="s">
         <v>63</v>
       </c>
@@ -19581,7 +19583,7 @@
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="137"/>
+      <c r="A13" s="121"/>
       <c r="B13" s="45" t="s">
         <v>64</v>
       </c>
@@ -19638,7 +19640,7 @@
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="137"/>
+      <c r="A14" s="121"/>
       <c r="B14" s="45" t="s">
         <v>65</v>
       </c>
@@ -19695,7 +19697,7 @@
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="137"/>
+      <c r="A15" s="121"/>
       <c r="B15" s="45" t="s">
         <v>66</v>
       </c>
@@ -19829,158 +19831,158 @@
       <c r="K1" s="140"/>
     </row>
     <row r="2" spans="1:44" ht="20" customHeight="1">
-      <c r="C2" s="127">
-        <v>1</v>
-      </c>
-      <c r="D2" s="128"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="127">
+      <c r="C2" s="115">
+        <v>1</v>
+      </c>
+      <c r="D2" s="116"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="115">
         <v>2</v>
       </c>
-      <c r="G2" s="128"/>
-      <c r="H2" s="129"/>
-      <c r="I2" s="127">
+      <c r="G2" s="116"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="115">
         <v>3</v>
       </c>
-      <c r="J2" s="128"/>
-      <c r="K2" s="129"/>
-      <c r="L2" s="127">
+      <c r="J2" s="116"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="115">
         <v>4</v>
       </c>
-      <c r="M2" s="128"/>
-      <c r="N2" s="129"/>
-      <c r="O2" s="127">
+      <c r="M2" s="116"/>
+      <c r="N2" s="117"/>
+      <c r="O2" s="115">
         <v>5</v>
       </c>
-      <c r="P2" s="128"/>
-      <c r="Q2" s="129"/>
-      <c r="R2" s="127">
+      <c r="P2" s="116"/>
+      <c r="Q2" s="117"/>
+      <c r="R2" s="115">
         <v>6</v>
       </c>
-      <c r="S2" s="128"/>
-      <c r="T2" s="129"/>
-      <c r="U2" s="127">
+      <c r="S2" s="116"/>
+      <c r="T2" s="117"/>
+      <c r="U2" s="115">
         <v>7</v>
       </c>
-      <c r="V2" s="128"/>
-      <c r="W2" s="129"/>
-      <c r="X2" s="127">
+      <c r="V2" s="116"/>
+      <c r="W2" s="117"/>
+      <c r="X2" s="115">
         <v>8</v>
       </c>
-      <c r="Y2" s="128"/>
-      <c r="Z2" s="129"/>
-      <c r="AA2" s="127">
+      <c r="Y2" s="116"/>
+      <c r="Z2" s="117"/>
+      <c r="AA2" s="115">
         <v>14</v>
       </c>
-      <c r="AB2" s="128"/>
-      <c r="AC2" s="129"/>
-      <c r="AD2" s="127">
+      <c r="AB2" s="116"/>
+      <c r="AC2" s="117"/>
+      <c r="AD2" s="115">
         <v>9</v>
       </c>
-      <c r="AE2" s="128"/>
-      <c r="AF2" s="129"/>
-      <c r="AG2" s="127">
+      <c r="AE2" s="116"/>
+      <c r="AF2" s="117"/>
+      <c r="AG2" s="115">
         <v>10</v>
       </c>
-      <c r="AH2" s="128"/>
-      <c r="AI2" s="129"/>
-      <c r="AJ2" s="127">
+      <c r="AH2" s="116"/>
+      <c r="AI2" s="117"/>
+      <c r="AJ2" s="115">
         <v>11</v>
       </c>
-      <c r="AK2" s="128"/>
-      <c r="AL2" s="129"/>
-      <c r="AM2" s="127">
+      <c r="AK2" s="116"/>
+      <c r="AL2" s="117"/>
+      <c r="AM2" s="115">
         <v>12</v>
       </c>
-      <c r="AN2" s="128"/>
-      <c r="AO2" s="129"/>
-      <c r="AP2" s="127">
+      <c r="AN2" s="116"/>
+      <c r="AO2" s="117"/>
+      <c r="AP2" s="115">
         <v>13</v>
       </c>
-      <c r="AQ2" s="128"/>
-      <c r="AR2" s="129"/>
+      <c r="AQ2" s="116"/>
+      <c r="AR2" s="117"/>
     </row>
     <row r="3" spans="1:44" s="14" customFormat="1" ht="20" customHeight="1">
-      <c r="A3" s="130" t="s">
+      <c r="A3" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="130"/>
-      <c r="C3" s="130" t="s">
+      <c r="B3" s="118"/>
+      <c r="C3" s="118" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="130"/>
-      <c r="E3" s="130"/>
-      <c r="F3" s="130" t="s">
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="130"/>
-      <c r="H3" s="130"/>
-      <c r="I3" s="130" t="s">
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="130"/>
-      <c r="K3" s="130"/>
-      <c r="L3" s="130" t="s">
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="130"/>
-      <c r="N3" s="130"/>
-      <c r="O3" s="130" t="s">
+      <c r="M3" s="118"/>
+      <c r="N3" s="118"/>
+      <c r="O3" s="118" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="130"/>
-      <c r="Q3" s="130"/>
-      <c r="R3" s="130" t="s">
+      <c r="P3" s="118"/>
+      <c r="Q3" s="118"/>
+      <c r="R3" s="118" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="130"/>
-      <c r="T3" s="130"/>
-      <c r="U3" s="130" t="s">
+      <c r="S3" s="118"/>
+      <c r="T3" s="118"/>
+      <c r="U3" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="V3" s="130"/>
-      <c r="W3" s="130"/>
-      <c r="X3" s="130" t="s">
+      <c r="V3" s="118"/>
+      <c r="W3" s="118"/>
+      <c r="X3" s="118" t="s">
         <v>6</v>
       </c>
-      <c r="Y3" s="130"/>
-      <c r="Z3" s="130"/>
-      <c r="AA3" s="131" t="s">
+      <c r="Y3" s="118"/>
+      <c r="Z3" s="118"/>
+      <c r="AA3" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="AB3" s="132"/>
-      <c r="AC3" s="133"/>
-      <c r="AD3" s="130" t="s">
+      <c r="AB3" s="125"/>
+      <c r="AC3" s="126"/>
+      <c r="AD3" s="118" t="s">
         <v>30</v>
       </c>
-      <c r="AE3" s="130"/>
-      <c r="AF3" s="130"/>
-      <c r="AG3" s="130" t="s">
+      <c r="AE3" s="118"/>
+      <c r="AF3" s="118"/>
+      <c r="AG3" s="118" t="s">
         <v>31</v>
       </c>
-      <c r="AH3" s="130"/>
-      <c r="AI3" s="130"/>
-      <c r="AJ3" s="130" t="s">
+      <c r="AH3" s="118"/>
+      <c r="AI3" s="118"/>
+      <c r="AJ3" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="AK3" s="130"/>
-      <c r="AL3" s="130"/>
-      <c r="AM3" s="130" t="s">
+      <c r="AK3" s="118"/>
+      <c r="AL3" s="118"/>
+      <c r="AM3" s="118" t="s">
         <v>13</v>
       </c>
-      <c r="AN3" s="130"/>
-      <c r="AO3" s="130"/>
-      <c r="AP3" s="130" t="s">
+      <c r="AN3" s="118"/>
+      <c r="AO3" s="118"/>
+      <c r="AP3" s="118" t="s">
         <v>8</v>
       </c>
-      <c r="AQ3" s="130"/>
-      <c r="AR3" s="130"/>
+      <c r="AQ3" s="118"/>
+      <c r="AR3" s="118"/>
     </row>
     <row r="4" spans="1:44" s="14" customFormat="1" ht="20" customHeight="1">
-      <c r="A4" s="130" t="s">
+      <c r="A4" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="130"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="14">
         <v>2006</v>
       </c>
@@ -20109,10 +20111,10 @@
       </c>
     </row>
     <row r="5" spans="1:44" s="14" customFormat="1" ht="20" customHeight="1">
-      <c r="A5" s="130" t="s">
+      <c r="A5" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="130"/>
+      <c r="B5" s="118"/>
       <c r="C5" s="14">
         <v>4</v>
       </c>
@@ -20241,7 +20243,7 @@
       </c>
     </row>
     <row r="6" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A6" s="139" t="s">
+      <c r="A6" s="123" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -20375,7 +20377,7 @@
       </c>
     </row>
     <row r="7" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A7" s="139"/>
+      <c r="A7" s="123"/>
       <c r="B7" s="16" t="s">
         <v>34</v>
       </c>
@@ -20507,7 +20509,7 @@
       </c>
     </row>
     <row r="8" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A8" s="139"/>
+      <c r="A8" s="123"/>
       <c r="B8" s="16" t="s">
         <v>35</v>
       </c>
@@ -20639,7 +20641,7 @@
       </c>
     </row>
     <row r="9" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A9" s="139"/>
+      <c r="A9" s="123"/>
       <c r="B9" s="15" t="s">
         <v>51</v>
       </c>
@@ -20771,7 +20773,7 @@
       </c>
     </row>
     <row r="10" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A10" s="139"/>
+      <c r="A10" s="123"/>
       <c r="B10" s="16" t="s">
         <v>36</v>
       </c>
@@ -20903,7 +20905,7 @@
       </c>
     </row>
     <row r="11" spans="1:44" ht="20" customHeight="1">
-      <c r="A11" s="134" t="s">
+      <c r="A11" s="119" t="s">
         <v>37</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -21037,7 +21039,7 @@
       </c>
     </row>
     <row r="12" spans="1:44" ht="20" customHeight="1">
-      <c r="A12" s="134"/>
+      <c r="A12" s="119"/>
       <c r="B12" s="6" t="s">
         <v>39</v>
       </c>
@@ -21169,7 +21171,7 @@
       </c>
     </row>
     <row r="13" spans="1:44" ht="20" customHeight="1">
-      <c r="A13" s="134"/>
+      <c r="A13" s="119"/>
       <c r="B13" s="6" t="s">
         <v>40</v>
       </c>
@@ -21301,7 +21303,7 @@
       </c>
     </row>
     <row r="14" spans="1:44" ht="20" customHeight="1">
-      <c r="A14" s="134"/>
+      <c r="A14" s="119"/>
       <c r="B14" s="6" t="s">
         <v>41</v>
       </c>
@@ -21433,7 +21435,7 @@
       </c>
     </row>
     <row r="15" spans="1:44" s="11" customFormat="1" ht="20" customHeight="1">
-      <c r="A15" s="135" t="s">
+      <c r="A15" s="114" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="10" t="s">
@@ -21567,7 +21569,7 @@
       </c>
     </row>
     <row r="16" spans="1:44" s="11" customFormat="1" ht="20" customHeight="1">
-      <c r="A16" s="135"/>
+      <c r="A16" s="114"/>
       <c r="B16" s="10" t="s">
         <v>43</v>
       </c>
@@ -21699,7 +21701,7 @@
       </c>
     </row>
     <row r="17" spans="1:44" ht="20" customHeight="1">
-      <c r="A17" s="134" t="s">
+      <c r="A17" s="119" t="s">
         <v>44</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -21833,7 +21835,7 @@
       </c>
     </row>
     <row r="18" spans="1:44" ht="20" customHeight="1">
-      <c r="A18" s="134"/>
+      <c r="A18" s="119"/>
       <c r="B18" s="6" t="s">
         <v>46</v>
       </c>
@@ -21965,7 +21967,7 @@
       </c>
     </row>
     <row r="19" spans="1:44" ht="20" customHeight="1">
-      <c r="A19" s="134"/>
+      <c r="A19" s="119"/>
       <c r="B19" s="6" t="s">
         <v>47</v>
       </c>
@@ -22623,6 +22625,29 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="AJ3:AL3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AM3:AO3"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="AG3:AI3"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="X3:Z3"/>
+    <mergeCell ref="AD3:AF3"/>
+    <mergeCell ref="AA3:AC3"/>
     <mergeCell ref="AP2:AR2"/>
     <mergeCell ref="AG2:AI2"/>
     <mergeCell ref="AJ2:AL2"/>
@@ -22636,29 +22661,6 @@
     <mergeCell ref="X2:Z2"/>
     <mergeCell ref="AD2:AF2"/>
     <mergeCell ref="AA2:AC2"/>
-    <mergeCell ref="AJ3:AL3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AM3:AO3"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="AG3:AI3"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="X3:Z3"/>
-    <mergeCell ref="AD3:AF3"/>
-    <mergeCell ref="AA3:AC3"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C2:E2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -22870,44 +22872,44 @@
     <row r="1" spans="1:19">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="130" t="s">
+      <c r="C1" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="130" t="s">
+      <c r="D1" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="130" t="s">
+      <c r="E1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="139" t="s">
+      <c r="F1" s="123" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="134" t="s">
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="123"/>
+      <c r="J1" s="123"/>
+      <c r="K1" s="119" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="134"/>
-      <c r="M1" s="134"/>
-      <c r="N1" s="134"/>
-      <c r="O1" s="135" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="135"/>
-      <c r="Q1" s="134" t="s">
+      <c r="L1" s="119"/>
+      <c r="M1" s="119"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="114" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="114"/>
+      <c r="Q1" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="134"/>
-      <c r="S1" s="134"/>
+      <c r="R1" s="119"/>
+      <c r="S1" s="119"/>
     </row>
     <row r="2" spans="1:19" ht="84">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -22952,13 +22954,13 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="120" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="127">
-        <v>1</v>
-      </c>
-      <c r="C3" s="130" t="s">
+      <c r="B3" s="115">
+        <v>1</v>
+      </c>
+      <c r="C3" s="118" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="14">
@@ -23011,9 +23013,9 @@
       </c>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="137"/>
-      <c r="B4" s="128"/>
-      <c r="C4" s="130"/>
+      <c r="A4" s="121"/>
+      <c r="B4" s="116"/>
+      <c r="C4" s="118"/>
       <c r="D4" s="14">
         <v>2010</v>
       </c>
@@ -23064,9 +23066,9 @@
       </c>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="137"/>
-      <c r="B5" s="129"/>
-      <c r="C5" s="130"/>
+      <c r="A5" s="121"/>
+      <c r="B5" s="117"/>
+      <c r="C5" s="118"/>
       <c r="D5" s="25">
         <v>2014</v>
       </c>
@@ -23117,11 +23119,11 @@
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="137"/>
-      <c r="B6" s="127">
+      <c r="A6" s="121"/>
+      <c r="B6" s="115">
         <v>2</v>
       </c>
-      <c r="C6" s="130" t="s">
+      <c r="C6" s="118" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="14">
@@ -23174,9 +23176,9 @@
       </c>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="137"/>
-      <c r="B7" s="128"/>
-      <c r="C7" s="130"/>
+      <c r="A7" s="121"/>
+      <c r="B7" s="116"/>
+      <c r="C7" s="118"/>
       <c r="D7" s="14">
         <v>2010</v>
       </c>
@@ -23227,9 +23229,9 @@
       </c>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" s="137"/>
-      <c r="B8" s="129"/>
-      <c r="C8" s="130"/>
+      <c r="A8" s="121"/>
+      <c r="B8" s="117"/>
+      <c r="C8" s="118"/>
       <c r="D8" s="25">
         <v>2014</v>
       </c>
@@ -23280,11 +23282,11 @@
       </c>
     </row>
     <row r="9" spans="1:19">
-      <c r="A9" s="137"/>
-      <c r="B9" s="127">
+      <c r="A9" s="121"/>
+      <c r="B9" s="115">
         <v>3</v>
       </c>
-      <c r="C9" s="130" t="s">
+      <c r="C9" s="118" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="14">
@@ -23337,9 +23339,9 @@
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="137"/>
-      <c r="B10" s="128"/>
-      <c r="C10" s="130"/>
+      <c r="A10" s="121"/>
+      <c r="B10" s="116"/>
+      <c r="C10" s="118"/>
       <c r="D10" s="14">
         <v>2010</v>
       </c>
@@ -23390,9 +23392,9 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="137"/>
-      <c r="B11" s="129"/>
-      <c r="C11" s="130"/>
+      <c r="A11" s="121"/>
+      <c r="B11" s="117"/>
+      <c r="C11" s="118"/>
       <c r="D11" s="25">
         <v>2014</v>
       </c>
@@ -23443,11 +23445,11 @@
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="137"/>
-      <c r="B12" s="127">
+      <c r="A12" s="121"/>
+      <c r="B12" s="115">
         <v>4</v>
       </c>
-      <c r="C12" s="130" t="s">
+      <c r="C12" s="118" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="14">
@@ -23500,9 +23502,9 @@
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="137"/>
-      <c r="B13" s="128"/>
-      <c r="C13" s="130"/>
+      <c r="A13" s="121"/>
+      <c r="B13" s="116"/>
+      <c r="C13" s="118"/>
       <c r="D13" s="14">
         <v>2010</v>
       </c>
@@ -23553,9 +23555,9 @@
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="137"/>
-      <c r="B14" s="129"/>
-      <c r="C14" s="130"/>
+      <c r="A14" s="121"/>
+      <c r="B14" s="117"/>
+      <c r="C14" s="118"/>
       <c r="D14" s="25">
         <v>2014</v>
       </c>
@@ -23606,11 +23608,11 @@
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="137"/>
-      <c r="B15" s="127">
+      <c r="A15" s="121"/>
+      <c r="B15" s="115">
         <v>5</v>
       </c>
-      <c r="C15" s="130" t="s">
+      <c r="C15" s="118" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="14">
@@ -23663,9 +23665,9 @@
       </c>
     </row>
     <row r="16" spans="1:19">
-      <c r="A16" s="137"/>
-      <c r="B16" s="128"/>
-      <c r="C16" s="130"/>
+      <c r="A16" s="121"/>
+      <c r="B16" s="116"/>
+      <c r="C16" s="118"/>
       <c r="D16" s="14">
         <v>2010</v>
       </c>
@@ -23716,9 +23718,9 @@
       </c>
     </row>
     <row r="17" spans="1:19">
-      <c r="A17" s="137"/>
-      <c r="B17" s="129"/>
-      <c r="C17" s="130"/>
+      <c r="A17" s="121"/>
+      <c r="B17" s="117"/>
+      <c r="C17" s="118"/>
       <c r="D17" s="25">
         <v>2014</v>
       </c>
@@ -23769,11 +23771,11 @@
       </c>
     </row>
     <row r="18" spans="1:19">
-      <c r="A18" s="137"/>
-      <c r="B18" s="127">
+      <c r="A18" s="121"/>
+      <c r="B18" s="115">
         <v>6</v>
       </c>
-      <c r="C18" s="130" t="s">
+      <c r="C18" s="118" t="s">
         <v>25</v>
       </c>
       <c r="D18" s="14">
@@ -23826,9 +23828,9 @@
       </c>
     </row>
     <row r="19" spans="1:19">
-      <c r="A19" s="137"/>
-      <c r="B19" s="128"/>
-      <c r="C19" s="130"/>
+      <c r="A19" s="121"/>
+      <c r="B19" s="116"/>
+      <c r="C19" s="118"/>
       <c r="D19" s="14">
         <v>2010</v>
       </c>
@@ -23879,9 +23881,9 @@
       </c>
     </row>
     <row r="20" spans="1:19">
-      <c r="A20" s="137"/>
-      <c r="B20" s="129"/>
-      <c r="C20" s="130"/>
+      <c r="A20" s="121"/>
+      <c r="B20" s="117"/>
+      <c r="C20" s="118"/>
       <c r="D20" s="25">
         <v>2014</v>
       </c>
@@ -23932,11 +23934,11 @@
       </c>
     </row>
     <row r="21" spans="1:19">
-      <c r="A21" s="137"/>
-      <c r="B21" s="127">
+      <c r="A21" s="121"/>
+      <c r="B21" s="115">
         <v>7</v>
       </c>
-      <c r="C21" s="130" t="s">
+      <c r="C21" s="118" t="s">
         <v>15</v>
       </c>
       <c r="D21" s="14">
@@ -23989,9 +23991,9 @@
       </c>
     </row>
     <row r="22" spans="1:19">
-      <c r="A22" s="137"/>
-      <c r="B22" s="128"/>
-      <c r="C22" s="130"/>
+      <c r="A22" s="121"/>
+      <c r="B22" s="116"/>
+      <c r="C22" s="118"/>
       <c r="D22" s="14">
         <v>2010</v>
       </c>
@@ -24042,9 +24044,9 @@
       </c>
     </row>
     <row r="23" spans="1:19">
-      <c r="A23" s="137"/>
-      <c r="B23" s="129"/>
-      <c r="C23" s="130"/>
+      <c r="A23" s="121"/>
+      <c r="B23" s="117"/>
+      <c r="C23" s="118"/>
       <c r="D23" s="25">
         <v>2014</v>
       </c>
@@ -24095,11 +24097,11 @@
       </c>
     </row>
     <row r="24" spans="1:19">
-      <c r="A24" s="137"/>
-      <c r="B24" s="127">
+      <c r="A24" s="121"/>
+      <c r="B24" s="115">
         <v>8</v>
       </c>
-      <c r="C24" s="130" t="s">
+      <c r="C24" s="118" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="14">
@@ -24152,9 +24154,9 @@
       </c>
     </row>
     <row r="25" spans="1:19">
-      <c r="A25" s="137"/>
-      <c r="B25" s="128"/>
-      <c r="C25" s="130"/>
+      <c r="A25" s="121"/>
+      <c r="B25" s="116"/>
+      <c r="C25" s="118"/>
       <c r="D25" s="14">
         <v>2010</v>
       </c>
@@ -24205,9 +24207,9 @@
       </c>
     </row>
     <row r="26" spans="1:19">
-      <c r="A26" s="137"/>
-      <c r="B26" s="129"/>
-      <c r="C26" s="130"/>
+      <c r="A26" s="121"/>
+      <c r="B26" s="117"/>
+      <c r="C26" s="118"/>
       <c r="D26" s="25">
         <v>2014</v>
       </c>
@@ -24258,11 +24260,11 @@
       </c>
     </row>
     <row r="27" spans="1:19">
-      <c r="A27" s="137"/>
-      <c r="B27" s="127">
+      <c r="A27" s="121"/>
+      <c r="B27" s="115">
         <v>14</v>
       </c>
-      <c r="C27" s="131" t="s">
+      <c r="C27" s="124" t="s">
         <v>54</v>
       </c>
       <c r="D27" s="14">
@@ -24315,9 +24317,9 @@
       </c>
     </row>
     <row r="28" spans="1:19">
-      <c r="A28" s="137"/>
-      <c r="B28" s="128"/>
-      <c r="C28" s="132"/>
+      <c r="A28" s="121"/>
+      <c r="B28" s="116"/>
+      <c r="C28" s="125"/>
       <c r="D28" s="14">
         <v>2010</v>
       </c>
@@ -24368,9 +24370,9 @@
       </c>
     </row>
     <row r="29" spans="1:19">
-      <c r="A29" s="137"/>
-      <c r="B29" s="129"/>
-      <c r="C29" s="133"/>
+      <c r="A29" s="121"/>
+      <c r="B29" s="117"/>
+      <c r="C29" s="126"/>
       <c r="D29" s="25">
         <v>2014</v>
       </c>
@@ -24421,11 +24423,11 @@
       </c>
     </row>
     <row r="30" spans="1:19">
-      <c r="A30" s="137"/>
-      <c r="B30" s="127">
+      <c r="A30" s="121"/>
+      <c r="B30" s="115">
         <v>9</v>
       </c>
-      <c r="C30" s="130" t="s">
+      <c r="C30" s="118" t="s">
         <v>12</v>
       </c>
       <c r="D30" s="14">
@@ -24478,9 +24480,9 @@
       </c>
     </row>
     <row r="31" spans="1:19">
-      <c r="A31" s="137"/>
-      <c r="B31" s="128"/>
-      <c r="C31" s="130"/>
+      <c r="A31" s="121"/>
+      <c r="B31" s="116"/>
+      <c r="C31" s="118"/>
       <c r="D31" s="14">
         <v>2010</v>
       </c>
@@ -24531,9 +24533,9 @@
       </c>
     </row>
     <row r="32" spans="1:19">
-      <c r="A32" s="137"/>
-      <c r="B32" s="129"/>
-      <c r="C32" s="130"/>
+      <c r="A32" s="121"/>
+      <c r="B32" s="117"/>
+      <c r="C32" s="118"/>
       <c r="D32" s="25">
         <v>2014</v>
       </c>
@@ -24584,11 +24586,11 @@
       </c>
     </row>
     <row r="33" spans="1:41">
-      <c r="A33" s="137"/>
-      <c r="B33" s="127">
+      <c r="A33" s="121"/>
+      <c r="B33" s="115">
         <v>10</v>
       </c>
-      <c r="C33" s="130" t="s">
+      <c r="C33" s="118" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="14">
@@ -24641,9 +24643,9 @@
       </c>
     </row>
     <row r="34" spans="1:41">
-      <c r="A34" s="137"/>
-      <c r="B34" s="128"/>
-      <c r="C34" s="130"/>
+      <c r="A34" s="121"/>
+      <c r="B34" s="116"/>
+      <c r="C34" s="118"/>
       <c r="D34" s="14">
         <v>2010</v>
       </c>
@@ -24694,9 +24696,9 @@
       </c>
     </row>
     <row r="35" spans="1:41">
-      <c r="A35" s="137"/>
-      <c r="B35" s="129"/>
-      <c r="C35" s="130"/>
+      <c r="A35" s="121"/>
+      <c r="B35" s="117"/>
+      <c r="C35" s="118"/>
       <c r="D35" s="25">
         <v>2014</v>
       </c>
@@ -24747,11 +24749,11 @@
       </c>
     </row>
     <row r="36" spans="1:41">
-      <c r="A36" s="137"/>
-      <c r="B36" s="127">
+      <c r="A36" s="121"/>
+      <c r="B36" s="115">
         <v>11</v>
       </c>
-      <c r="C36" s="130" t="s">
+      <c r="C36" s="118" t="s">
         <v>21</v>
       </c>
       <c r="D36" s="14">
@@ -24804,9 +24806,9 @@
       </c>
     </row>
     <row r="37" spans="1:41">
-      <c r="A37" s="137"/>
-      <c r="B37" s="128"/>
-      <c r="C37" s="130"/>
+      <c r="A37" s="121"/>
+      <c r="B37" s="116"/>
+      <c r="C37" s="118"/>
       <c r="D37" s="14">
         <v>2010</v>
       </c>
@@ -24857,9 +24859,9 @@
       </c>
     </row>
     <row r="38" spans="1:41">
-      <c r="A38" s="137"/>
-      <c r="B38" s="129"/>
-      <c r="C38" s="130"/>
+      <c r="A38" s="121"/>
+      <c r="B38" s="117"/>
+      <c r="C38" s="118"/>
       <c r="D38" s="25">
         <v>2014</v>
       </c>
@@ -24910,11 +24912,11 @@
       </c>
     </row>
     <row r="39" spans="1:41">
-      <c r="A39" s="137"/>
-      <c r="B39" s="127">
+      <c r="A39" s="121"/>
+      <c r="B39" s="115">
         <v>12</v>
       </c>
-      <c r="C39" s="130" t="s">
+      <c r="C39" s="118" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="14">
@@ -24967,9 +24969,9 @@
       </c>
     </row>
     <row r="40" spans="1:41">
-      <c r="A40" s="137"/>
-      <c r="B40" s="128"/>
-      <c r="C40" s="130"/>
+      <c r="A40" s="121"/>
+      <c r="B40" s="116"/>
+      <c r="C40" s="118"/>
       <c r="D40" s="14">
         <v>2010</v>
       </c>
@@ -25020,9 +25022,9 @@
       </c>
     </row>
     <row r="41" spans="1:41">
-      <c r="A41" s="137"/>
-      <c r="B41" s="129"/>
-      <c r="C41" s="130"/>
+      <c r="A41" s="121"/>
+      <c r="B41" s="117"/>
+      <c r="C41" s="118"/>
       <c r="D41" s="25">
         <v>2014</v>
       </c>
@@ -25073,11 +25075,11 @@
       </c>
     </row>
     <row r="42" spans="1:41">
-      <c r="A42" s="137"/>
-      <c r="B42" s="127">
+      <c r="A42" s="121"/>
+      <c r="B42" s="115">
         <v>13</v>
       </c>
-      <c r="C42" s="130" t="s">
+      <c r="C42" s="118" t="s">
         <v>8</v>
       </c>
       <c r="D42" s="14">
@@ -25130,9 +25132,9 @@
       </c>
     </row>
     <row r="43" spans="1:41">
-      <c r="A43" s="137"/>
-      <c r="B43" s="128"/>
-      <c r="C43" s="130"/>
+      <c r="A43" s="121"/>
+      <c r="B43" s="116"/>
+      <c r="C43" s="118"/>
       <c r="D43" s="14">
         <v>2010</v>
       </c>
@@ -25183,9 +25185,9 @@
       </c>
     </row>
     <row r="44" spans="1:41">
-      <c r="A44" s="138"/>
-      <c r="B44" s="129"/>
-      <c r="C44" s="130"/>
+      <c r="A44" s="122"/>
+      <c r="B44" s="117"/>
+      <c r="C44" s="118"/>
       <c r="D44" s="25">
         <v>2014</v>
       </c>
@@ -25236,81 +25238,81 @@
       </c>
     </row>
     <row r="46" spans="1:41" ht="15.75" customHeight="1">
-      <c r="A46" s="130" t="s">
+      <c r="A46" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="130"/>
-      <c r="C46" s="130" t="s">
+      <c r="B46" s="118"/>
+      <c r="C46" s="118" t="s">
         <v>50</v>
       </c>
-      <c r="D46" s="130"/>
-      <c r="E46" s="130"/>
-      <c r="F46" s="130" t="s">
+      <c r="D46" s="118"/>
+      <c r="E46" s="118"/>
+      <c r="F46" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="G46" s="130"/>
-      <c r="H46" s="130"/>
-      <c r="I46" s="130" t="s">
+      <c r="G46" s="118"/>
+      <c r="H46" s="118"/>
+      <c r="I46" s="118" t="s">
         <v>17</v>
       </c>
-      <c r="J46" s="130"/>
-      <c r="K46" s="130"/>
-      <c r="L46" s="130" t="s">
+      <c r="J46" s="118"/>
+      <c r="K46" s="118"/>
+      <c r="L46" s="118" t="s">
         <v>10</v>
       </c>
-      <c r="M46" s="130"/>
-      <c r="N46" s="130"/>
-      <c r="O46" s="130" t="s">
+      <c r="M46" s="118"/>
+      <c r="N46" s="118"/>
+      <c r="O46" s="118" t="s">
         <v>23</v>
       </c>
-      <c r="P46" s="130"/>
-      <c r="Q46" s="130"/>
-      <c r="R46" s="130" t="s">
+      <c r="P46" s="118"/>
+      <c r="Q46" s="118"/>
+      <c r="R46" s="118" t="s">
         <v>87</v>
       </c>
-      <c r="S46" s="130"/>
-      <c r="T46" s="130"/>
-      <c r="U46" s="131" t="s">
+      <c r="S46" s="118"/>
+      <c r="T46" s="118"/>
+      <c r="U46" s="124" t="s">
         <v>70</v>
       </c>
-      <c r="V46" s="132"/>
-      <c r="W46" s="133"/>
-      <c r="X46" s="131" t="s">
+      <c r="V46" s="125"/>
+      <c r="W46" s="126"/>
+      <c r="X46" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="Y46" s="132"/>
-      <c r="Z46" s="133"/>
-      <c r="AA46" s="130" t="s">
+      <c r="Y46" s="125"/>
+      <c r="Z46" s="126"/>
+      <c r="AA46" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="AB46" s="130"/>
-      <c r="AC46" s="130"/>
-      <c r="AD46" s="130" t="s">
+      <c r="AB46" s="118"/>
+      <c r="AC46" s="118"/>
+      <c r="AD46" s="118" t="s">
         <v>28</v>
       </c>
-      <c r="AE46" s="130"/>
-      <c r="AF46" s="130"/>
-      <c r="AG46" s="130" t="s">
+      <c r="AE46" s="118"/>
+      <c r="AF46" s="118"/>
+      <c r="AG46" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="AH46" s="130"/>
-      <c r="AI46" s="130"/>
-      <c r="AJ46" s="130" t="s">
+      <c r="AH46" s="118"/>
+      <c r="AI46" s="118"/>
+      <c r="AJ46" s="118" t="s">
         <v>13</v>
       </c>
-      <c r="AK46" s="130"/>
-      <c r="AL46" s="130"/>
-      <c r="AM46" s="130" t="s">
+      <c r="AK46" s="118"/>
+      <c r="AL46" s="118"/>
+      <c r="AM46" s="118" t="s">
         <v>8</v>
       </c>
-      <c r="AN46" s="130"/>
-      <c r="AO46" s="130"/>
+      <c r="AN46" s="118"/>
+      <c r="AO46" s="118"/>
     </row>
     <row r="47" spans="1:41" ht="42.75" customHeight="1">
-      <c r="A47" s="130" t="s">
+      <c r="A47" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="130"/>
+      <c r="B47" s="118"/>
       <c r="C47" s="54" t="s">
         <v>72</v>
       </c>
@@ -25430,10 +25432,10 @@
       </c>
     </row>
     <row r="48" spans="1:41" ht="33" customHeight="1">
-      <c r="A48" s="130" t="s">
+      <c r="A48" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="130"/>
+      <c r="B48" s="118"/>
       <c r="C48" s="54">
         <v>4</v>
       </c>
@@ -25564,7 +25566,7 @@
       </c>
     </row>
     <row r="50" spans="2:4">
-      <c r="B50" s="120"/>
+      <c r="B50" s="134"/>
       <c r="C50" s="63">
         <v>2010</v>
       </c>
@@ -25573,7 +25575,7 @@
       </c>
     </row>
     <row r="51" spans="2:4">
-      <c r="B51" s="120"/>
+      <c r="B51" s="134"/>
       <c r="C51" s="63">
         <v>2014</v>
       </c>
@@ -25583,23 +25585,26 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="AA46:AC46"/>
-    <mergeCell ref="AD46:AF46"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="I46:K46"/>
-    <mergeCell ref="L46:N46"/>
-    <mergeCell ref="AG46:AI46"/>
-    <mergeCell ref="AJ46:AL46"/>
-    <mergeCell ref="AM46:AO46"/>
-    <mergeCell ref="O46:Q46"/>
-    <mergeCell ref="R46:T46"/>
-    <mergeCell ref="U46:W46"/>
-    <mergeCell ref="X46:Z46"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
     <mergeCell ref="B39:B41"/>
     <mergeCell ref="C39:C41"/>
     <mergeCell ref="B42:B44"/>
@@ -25616,26 +25621,23 @@
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="C24:C26"/>
     <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="AG46:AI46"/>
+    <mergeCell ref="AJ46:AL46"/>
+    <mergeCell ref="AM46:AO46"/>
+    <mergeCell ref="O46:Q46"/>
+    <mergeCell ref="R46:T46"/>
+    <mergeCell ref="U46:W46"/>
+    <mergeCell ref="X46:Z46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="AA46:AC46"/>
+    <mergeCell ref="AD46:AF46"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="L46:N46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Call(wrap, width) function to help wrap GenderGap Titles
</commit_message>
<xml_diff>
--- a/GenderGap_Data/GenderGap_Find4Hourglass.xlsx
+++ b/GenderGap_Data/GenderGap_Find4Hourglass.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22860" windowHeight="12480" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="24840" yWindow="5320" windowWidth="22500" windowHeight="13620" tabRatio="624" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="13C_csv" sheetId="10" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="工作表1" sheetId="1" r:id="rId7"/>
     <sheet name="工作表2" sheetId="2" r:id="rId8"/>
     <sheet name="convert_row" sheetId="3" r:id="rId9"/>
+    <sheet name="Title_json" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="221">
   <si>
     <t xml:space="preserve">Labour force participation                              </t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -771,6 +772,69 @@
   <si>
     <t>ECONOMIC PARTICIPATION AND OPPORTUNITY</t>
   </si>
+  <si>
+    <t xml:space="preserve">Labour force participation </t>
+  </si>
+  <si>
+    <t>Economic Participation and Opportunity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDUCATIONAL ATTAINMENT                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">POLITICAL EMPOWERMENT                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wage equality for similar work (survey)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Professional and technical workers               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Literacy rate                                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enrolment in primary education                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enrolment in secondary education                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enrolment in tertiary education                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sex ratio at birth (female/male)                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Healthy life expectancy                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Women in parliament                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Women in ministerial positions        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Years with female head of state (last 50)     </t>
+  </si>
+  <si>
+    <t>Educational Attainment</t>
+  </si>
+  <si>
+    <t>Health and Survival</t>
+  </si>
+  <si>
+    <t>Political Empowerment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enrollment in primary education                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enrollment in secondary education                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enrollment in tertiary education                         </t>
+  </si>
 </sst>
 </file>
 
@@ -780,7 +844,7 @@
     <numFmt numFmtId="164" formatCode="###0.00;###0.00"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -929,6 +993,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1180,7 +1250,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="183">
+  <cellStyleXfs count="239">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1364,8 +1434,64 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1686,7 +1812,43 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="106" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="2" xfId="106" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="3" xfId="106" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="4" xfId="106" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" xfId="108" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="16" xfId="108" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1701,7 +1863,19 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1716,62 +1890,17 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="2" xfId="106" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="3" xfId="106" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="4" xfId="106" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="106" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" xfId="108" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="16" xfId="108" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="105" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="105" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="183">
+  <cellStyles count="239">
     <cellStyle name="Bad" xfId="107" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="108" builtinId="23"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1863,6 +1992,34 @@
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="106" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1953,6 +2110,34 @@
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="105"/>
   </cellStyles>
@@ -2329,11 +2514,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="-2110959080"/>
-        <c:axId val="-2111540472"/>
+        <c:axId val="2133376968"/>
+        <c:axId val="2133379992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2110959080"/>
+        <c:axId val="2133376968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2342,7 +2527,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111540472"/>
+        <c:crossAx val="2133379992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2350,7 +2535,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2111540472"/>
+        <c:axId val="2133379992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2366,13 +2551,14 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2110959080"/>
+        <c:crossAx val="2133376968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2580,11 +2766,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2093535768"/>
-        <c:axId val="-2093532824"/>
+        <c:axId val="2133457464"/>
+        <c:axId val="2133460408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2093535768"/>
+        <c:axId val="2133457464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2593,7 +2779,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093532824"/>
+        <c:crossAx val="2133460408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2601,7 +2787,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2093532824"/>
+        <c:axId val="2133460408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2612,7 +2798,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="-2093535768"/>
+        <c:crossAx val="2133457464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3038,8 +3224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31:R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6084,12 +6270,262 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="49.33203125" style="143" customWidth="1"/>
+    <col min="2" max="2" width="26" style="143" customWidth="1"/>
+    <col min="3" max="3" width="40.5" style="143" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="143" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="143"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15" customHeight="1">
+      <c r="A1" s="142" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="142"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
+      <c r="J1" s="142" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="142"/>
+      <c r="L1" s="142" t="s">
+        <v>203</v>
+      </c>
+      <c r="M1" s="142"/>
+      <c r="N1" s="142"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="143" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" s="143" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="143" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="143" t="s">
+        <v>205</v>
+      </c>
+      <c r="F2" s="143" t="s">
+        <v>206</v>
+      </c>
+      <c r="G2" s="143" t="s">
+        <v>207</v>
+      </c>
+      <c r="H2" s="143" t="s">
+        <v>208</v>
+      </c>
+      <c r="I2" s="143" t="s">
+        <v>209</v>
+      </c>
+      <c r="J2" s="143" t="s">
+        <v>210</v>
+      </c>
+      <c r="K2" s="143" t="s">
+        <v>211</v>
+      </c>
+      <c r="L2" s="143" t="s">
+        <v>212</v>
+      </c>
+      <c r="M2" s="143" t="s">
+        <v>213</v>
+      </c>
+      <c r="N2" s="143" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="142" t="s">
+        <v>201</v>
+      </c>
+      <c r="B3" s="142"/>
+      <c r="C3" s="142"/>
+      <c r="D3" s="142"/>
+      <c r="E3" s="142"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="143" t="s">
+        <v>197</v>
+      </c>
+      <c r="B7" s="143" t="s">
+        <v>198</v>
+      </c>
+      <c r="C7" s="143" t="s">
+        <v>197</v>
+      </c>
+      <c r="D7" s="143" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="143" t="s">
+        <v>200</v>
+      </c>
+      <c r="B8" s="26">
+        <v>0.84</v>
+      </c>
+      <c r="C8" s="143" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="143" t="s">
+        <v>204</v>
+      </c>
+      <c r="B9" s="26">
+        <v>0.63</v>
+      </c>
+      <c r="C9" s="144" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="26">
+        <v>0.64</v>
+      </c>
+      <c r="C10" s="143" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="143" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="26">
+        <v>0.2</v>
+      </c>
+      <c r="C11" s="143" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="143" t="s">
+        <v>205</v>
+      </c>
+      <c r="B12" s="26">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="143" t="s">
+        <v>206</v>
+      </c>
+      <c r="B13" s="34">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="143" t="s">
+        <v>218</v>
+      </c>
+      <c r="B14" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="143" t="s">
+        <v>219</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="143" t="s">
+        <v>220</v>
+      </c>
+      <c r="B16" s="34">
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="143" t="s">
+        <v>210</v>
+      </c>
+      <c r="B17" s="28">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="143" t="s">
+        <v>211</v>
+      </c>
+      <c r="B18" s="28">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="143" t="s">
+        <v>212</v>
+      </c>
+      <c r="B19" s="34">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="143" t="s">
+        <v>213</v>
+      </c>
+      <c r="B20" s="34">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="143" t="s">
+        <v>214</v>
+      </c>
+      <c r="B21" s="34">
+        <v>0.08</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="A3:E3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO82"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W2" sqref="T1:W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6118,37 +6554,37 @@
     <row r="1" spans="1:27" ht="34" customHeight="1">
       <c r="A1" s="97"/>
       <c r="B1" s="97"/>
-      <c r="C1" s="118" t="s">
+      <c r="C1" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="118" t="s">
+      <c r="D1" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="118" t="s">
+      <c r="E1" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="139" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="119" t="s">
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="134" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
-      <c r="N1" s="119"/>
-      <c r="O1" s="114" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="114"/>
-      <c r="Q1" s="119" t="s">
+      <c r="L1" s="134"/>
+      <c r="M1" s="134"/>
+      <c r="N1" s="134"/>
+      <c r="O1" s="135" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="135"/>
+      <c r="Q1" s="134" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="119"/>
-      <c r="S1" s="119"/>
+      <c r="R1" s="134"/>
+      <c r="S1" s="134"/>
       <c r="T1" s="71" t="s">
         <v>92</v>
       </c>
@@ -6165,9 +6601,9 @@
     <row r="2" spans="1:27" ht="113" customHeight="1">
       <c r="A2" s="97"/>
       <c r="B2" s="97"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -6236,13 +6672,13 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="136" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="115">
-        <v>1</v>
-      </c>
-      <c r="C3" s="118" t="s">
+      <c r="B3" s="127">
+        <v>1</v>
+      </c>
+      <c r="C3" s="130" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="92">
@@ -6310,9 +6746,9 @@
       </c>
     </row>
     <row r="4" spans="1:27">
-      <c r="A4" s="121"/>
-      <c r="B4" s="116"/>
-      <c r="C4" s="118"/>
+      <c r="A4" s="137"/>
+      <c r="B4" s="128"/>
+      <c r="C4" s="130"/>
       <c r="D4" s="92">
         <v>2010</v>
       </c>
@@ -6378,9 +6814,9 @@
       </c>
     </row>
     <row r="5" spans="1:27">
-      <c r="A5" s="121"/>
-      <c r="B5" s="117"/>
-      <c r="C5" s="118"/>
+      <c r="A5" s="137"/>
+      <c r="B5" s="129"/>
+      <c r="C5" s="130"/>
       <c r="D5" s="25">
         <v>2014</v>
       </c>
@@ -6446,7 +6882,7 @@
       </c>
     </row>
     <row r="6" spans="1:27">
-      <c r="A6" s="121"/>
+      <c r="A6" s="137"/>
       <c r="B6" s="91"/>
       <c r="C6" s="92"/>
       <c r="D6" s="25"/>
@@ -6468,11 +6904,11 @@
       <c r="X6" s="106"/>
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1">
-      <c r="A7" s="121"/>
-      <c r="B7" s="115">
+      <c r="A7" s="137"/>
+      <c r="B7" s="127">
         <v>2</v>
       </c>
-      <c r="C7" s="118" t="s">
+      <c r="C7" s="130" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="92">
@@ -6540,9 +6976,9 @@
       </c>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="121"/>
-      <c r="B8" s="116"/>
-      <c r="C8" s="118"/>
+      <c r="A8" s="137"/>
+      <c r="B8" s="128"/>
+      <c r="C8" s="130"/>
       <c r="D8" s="92">
         <v>2010</v>
       </c>
@@ -6608,9 +7044,9 @@
       </c>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="121"/>
-      <c r="B9" s="117"/>
-      <c r="C9" s="118"/>
+      <c r="A9" s="137"/>
+      <c r="B9" s="129"/>
+      <c r="C9" s="130"/>
       <c r="D9" s="25">
         <v>2014</v>
       </c>
@@ -6676,7 +7112,7 @@
       </c>
     </row>
     <row r="10" spans="1:27">
-      <c r="A10" s="121"/>
+      <c r="A10" s="137"/>
       <c r="B10" s="91"/>
       <c r="C10" s="92"/>
       <c r="D10" s="25"/>
@@ -6698,11 +7134,11 @@
       <c r="X10" s="106"/>
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A11" s="121"/>
-      <c r="B11" s="115">
+      <c r="A11" s="137"/>
+      <c r="B11" s="127">
         <v>3</v>
       </c>
-      <c r="C11" s="118" t="s">
+      <c r="C11" s="130" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="92">
@@ -6770,9 +7206,9 @@
       </c>
     </row>
     <row r="12" spans="1:27">
-      <c r="A12" s="121"/>
-      <c r="B12" s="116"/>
-      <c r="C12" s="118"/>
+      <c r="A12" s="137"/>
+      <c r="B12" s="128"/>
+      <c r="C12" s="130"/>
       <c r="D12" s="92">
         <v>2010</v>
       </c>
@@ -6838,9 +7274,9 @@
       </c>
     </row>
     <row r="13" spans="1:27">
-      <c r="A13" s="121"/>
-      <c r="B13" s="117"/>
-      <c r="C13" s="118"/>
+      <c r="A13" s="137"/>
+      <c r="B13" s="129"/>
+      <c r="C13" s="130"/>
       <c r="D13" s="25">
         <v>2014</v>
       </c>
@@ -6906,7 +7342,7 @@
       </c>
     </row>
     <row r="14" spans="1:27">
-      <c r="A14" s="121"/>
+      <c r="A14" s="137"/>
       <c r="B14" s="91"/>
       <c r="C14" s="92"/>
       <c r="D14" s="25"/>
@@ -6928,11 +7364,11 @@
       <c r="X14" s="106"/>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="121"/>
-      <c r="B15" s="115">
+      <c r="A15" s="137"/>
+      <c r="B15" s="127">
         <v>4</v>
       </c>
-      <c r="C15" s="118" t="s">
+      <c r="C15" s="130" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="92">
@@ -7000,9 +7436,9 @@
       </c>
     </row>
     <row r="16" spans="1:27">
-      <c r="A16" s="121"/>
-      <c r="B16" s="116"/>
-      <c r="C16" s="118"/>
+      <c r="A16" s="137"/>
+      <c r="B16" s="128"/>
+      <c r="C16" s="130"/>
       <c r="D16" s="92">
         <v>2010</v>
       </c>
@@ -7068,9 +7504,9 @@
       </c>
     </row>
     <row r="17" spans="1:24">
-      <c r="A17" s="121"/>
-      <c r="B17" s="117"/>
-      <c r="C17" s="118"/>
+      <c r="A17" s="137"/>
+      <c r="B17" s="129"/>
+      <c r="C17" s="130"/>
       <c r="D17" s="25">
         <v>2014</v>
       </c>
@@ -7136,7 +7572,7 @@
       </c>
     </row>
     <row r="18" spans="1:24">
-      <c r="A18" s="121"/>
+      <c r="A18" s="137"/>
       <c r="B18" s="91"/>
       <c r="C18" s="92"/>
       <c r="D18" s="25"/>
@@ -7158,11 +7594,11 @@
       <c r="X18" s="106"/>
     </row>
     <row r="19" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A19" s="121"/>
-      <c r="B19" s="115">
+      <c r="A19" s="137"/>
+      <c r="B19" s="127">
         <v>5</v>
       </c>
-      <c r="C19" s="118" t="s">
+      <c r="C19" s="130" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="92">
@@ -7230,9 +7666,9 @@
       </c>
     </row>
     <row r="20" spans="1:24">
-      <c r="A20" s="121"/>
-      <c r="B20" s="116"/>
-      <c r="C20" s="118"/>
+      <c r="A20" s="137"/>
+      <c r="B20" s="128"/>
+      <c r="C20" s="130"/>
       <c r="D20" s="92">
         <v>2010</v>
       </c>
@@ -7298,9 +7734,9 @@
       </c>
     </row>
     <row r="21" spans="1:24">
-      <c r="A21" s="121"/>
-      <c r="B21" s="117"/>
-      <c r="C21" s="118"/>
+      <c r="A21" s="137"/>
+      <c r="B21" s="129"/>
+      <c r="C21" s="130"/>
       <c r="D21" s="25">
         <v>2014</v>
       </c>
@@ -7366,7 +7802,7 @@
       </c>
     </row>
     <row r="22" spans="1:24">
-      <c r="A22" s="121"/>
+      <c r="A22" s="137"/>
       <c r="B22" s="91"/>
       <c r="C22" s="92"/>
       <c r="D22" s="25"/>
@@ -7388,11 +7824,11 @@
       <c r="X22" s="106"/>
     </row>
     <row r="23" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A23" s="121"/>
-      <c r="B23" s="115">
+      <c r="A23" s="137"/>
+      <c r="B23" s="127">
         <v>6</v>
       </c>
-      <c r="C23" s="118" t="s">
+      <c r="C23" s="130" t="s">
         <v>25</v>
       </c>
       <c r="D23" s="92">
@@ -7460,9 +7896,9 @@
       </c>
     </row>
     <row r="24" spans="1:24">
-      <c r="A24" s="121"/>
-      <c r="B24" s="116"/>
-      <c r="C24" s="118"/>
+      <c r="A24" s="137"/>
+      <c r="B24" s="128"/>
+      <c r="C24" s="130"/>
       <c r="D24" s="92">
         <v>2010</v>
       </c>
@@ -7528,9 +7964,9 @@
       </c>
     </row>
     <row r="25" spans="1:24">
-      <c r="A25" s="121"/>
-      <c r="B25" s="117"/>
-      <c r="C25" s="118"/>
+      <c r="A25" s="137"/>
+      <c r="B25" s="129"/>
+      <c r="C25" s="130"/>
       <c r="D25" s="25">
         <v>2014</v>
       </c>
@@ -7596,7 +8032,7 @@
       </c>
     </row>
     <row r="26" spans="1:24">
-      <c r="A26" s="121"/>
+      <c r="A26" s="137"/>
       <c r="B26" s="91"/>
       <c r="C26" s="92"/>
       <c r="D26" s="25"/>
@@ -7618,11 +8054,11 @@
       <c r="X26" s="106"/>
     </row>
     <row r="27" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A27" s="121"/>
-      <c r="B27" s="115">
+      <c r="A27" s="137"/>
+      <c r="B27" s="127">
         <v>7</v>
       </c>
-      <c r="C27" s="118" t="s">
+      <c r="C27" s="130" t="s">
         <v>70</v>
       </c>
       <c r="D27" s="92">
@@ -7690,9 +8126,9 @@
       </c>
     </row>
     <row r="28" spans="1:24">
-      <c r="A28" s="121"/>
-      <c r="B28" s="116"/>
-      <c r="C28" s="118"/>
+      <c r="A28" s="137"/>
+      <c r="B28" s="128"/>
+      <c r="C28" s="130"/>
       <c r="D28" s="92">
         <v>2010</v>
       </c>
@@ -7758,9 +8194,9 @@
       </c>
     </row>
     <row r="29" spans="1:24">
-      <c r="A29" s="121"/>
-      <c r="B29" s="117"/>
-      <c r="C29" s="118"/>
+      <c r="A29" s="137"/>
+      <c r="B29" s="129"/>
+      <c r="C29" s="130"/>
       <c r="D29" s="25">
         <v>2014</v>
       </c>
@@ -7826,7 +8262,7 @@
       </c>
     </row>
     <row r="30" spans="1:24">
-      <c r="A30" s="121"/>
+      <c r="A30" s="137"/>
       <c r="B30" s="91"/>
       <c r="C30" s="95"/>
       <c r="D30" s="25"/>
@@ -7848,11 +8284,11 @@
       <c r="X30" s="106"/>
     </row>
     <row r="31" spans="1:24">
-      <c r="A31" s="121"/>
-      <c r="B31" s="115">
+      <c r="A31" s="137"/>
+      <c r="B31" s="127">
         <v>8</v>
       </c>
-      <c r="C31" s="124" t="s">
+      <c r="C31" s="131" t="s">
         <v>54</v>
       </c>
       <c r="D31" s="92">
@@ -7920,9 +8356,9 @@
       </c>
     </row>
     <row r="32" spans="1:24">
-      <c r="A32" s="121"/>
-      <c r="B32" s="116"/>
-      <c r="C32" s="125"/>
+      <c r="A32" s="137"/>
+      <c r="B32" s="128"/>
+      <c r="C32" s="132"/>
       <c r="D32" s="92">
         <v>2010</v>
       </c>
@@ -7988,9 +8424,9 @@
       </c>
     </row>
     <row r="33" spans="1:24">
-      <c r="A33" s="121"/>
-      <c r="B33" s="117"/>
-      <c r="C33" s="126"/>
+      <c r="A33" s="137"/>
+      <c r="B33" s="129"/>
+      <c r="C33" s="133"/>
       <c r="D33" s="25">
         <v>2014</v>
       </c>
@@ -8056,7 +8492,7 @@
       </c>
     </row>
     <row r="34" spans="1:24">
-      <c r="A34" s="121"/>
+      <c r="A34" s="137"/>
       <c r="B34" s="91"/>
       <c r="C34" s="96"/>
       <c r="D34" s="25"/>
@@ -8078,11 +8514,11 @@
       <c r="X34" s="106"/>
     </row>
     <row r="35" spans="1:24">
-      <c r="A35" s="121"/>
-      <c r="B35" s="115">
+      <c r="A35" s="137"/>
+      <c r="B35" s="127">
         <v>9</v>
       </c>
-      <c r="C35" s="118" t="s">
+      <c r="C35" s="130" t="s">
         <v>12</v>
       </c>
       <c r="D35" s="92">
@@ -8150,9 +8586,9 @@
       </c>
     </row>
     <row r="36" spans="1:24">
-      <c r="A36" s="121"/>
-      <c r="B36" s="116"/>
-      <c r="C36" s="118"/>
+      <c r="A36" s="137"/>
+      <c r="B36" s="128"/>
+      <c r="C36" s="130"/>
       <c r="D36" s="92">
         <v>2010</v>
       </c>
@@ -8218,9 +8654,9 @@
       </c>
     </row>
     <row r="37" spans="1:24">
-      <c r="A37" s="121"/>
-      <c r="B37" s="117"/>
-      <c r="C37" s="118"/>
+      <c r="A37" s="137"/>
+      <c r="B37" s="129"/>
+      <c r="C37" s="130"/>
       <c r="D37" s="25">
         <v>2014</v>
       </c>
@@ -8286,7 +8722,7 @@
       </c>
     </row>
     <row r="38" spans="1:24">
-      <c r="A38" s="121"/>
+      <c r="A38" s="137"/>
       <c r="B38" s="91"/>
       <c r="C38" s="92"/>
       <c r="D38" s="25"/>
@@ -8308,11 +8744,11 @@
       <c r="X38" s="106"/>
     </row>
     <row r="39" spans="1:24">
-      <c r="A39" s="121"/>
-      <c r="B39" s="115">
+      <c r="A39" s="137"/>
+      <c r="B39" s="127">
         <v>10</v>
       </c>
-      <c r="C39" s="118" t="s">
+      <c r="C39" s="130" t="s">
         <v>28</v>
       </c>
       <c r="D39" s="92">
@@ -8380,9 +8816,9 @@
       </c>
     </row>
     <row r="40" spans="1:24">
-      <c r="A40" s="121"/>
-      <c r="B40" s="116"/>
-      <c r="C40" s="118"/>
+      <c r="A40" s="137"/>
+      <c r="B40" s="128"/>
+      <c r="C40" s="130"/>
       <c r="D40" s="92">
         <v>2010</v>
       </c>
@@ -8448,9 +8884,9 @@
       </c>
     </row>
     <row r="41" spans="1:24">
-      <c r="A41" s="121"/>
-      <c r="B41" s="117"/>
-      <c r="C41" s="118"/>
+      <c r="A41" s="137"/>
+      <c r="B41" s="129"/>
+      <c r="C41" s="130"/>
       <c r="D41" s="25">
         <v>2014</v>
       </c>
@@ -8516,7 +8952,7 @@
       </c>
     </row>
     <row r="42" spans="1:24">
-      <c r="A42" s="121"/>
+      <c r="A42" s="137"/>
       <c r="B42" s="91"/>
       <c r="C42" s="92"/>
       <c r="D42" s="25"/>
@@ -8538,11 +8974,11 @@
       <c r="X42" s="106"/>
     </row>
     <row r="43" spans="1:24">
-      <c r="A43" s="121"/>
-      <c r="B43" s="115">
+      <c r="A43" s="137"/>
+      <c r="B43" s="127">
         <v>11</v>
       </c>
-      <c r="C43" s="118" t="s">
+      <c r="C43" s="130" t="s">
         <v>21</v>
       </c>
       <c r="D43" s="92">
@@ -8610,9 +9046,9 @@
       </c>
     </row>
     <row r="44" spans="1:24">
-      <c r="A44" s="121"/>
-      <c r="B44" s="116"/>
-      <c r="C44" s="118"/>
+      <c r="A44" s="137"/>
+      <c r="B44" s="128"/>
+      <c r="C44" s="130"/>
       <c r="D44" s="92">
         <v>2010</v>
       </c>
@@ -8678,9 +9114,9 @@
       </c>
     </row>
     <row r="45" spans="1:24">
-      <c r="A45" s="121"/>
-      <c r="B45" s="117"/>
-      <c r="C45" s="118"/>
+      <c r="A45" s="137"/>
+      <c r="B45" s="129"/>
+      <c r="C45" s="130"/>
       <c r="D45" s="25">
         <v>2014</v>
       </c>
@@ -8746,7 +9182,7 @@
       </c>
     </row>
     <row r="46" spans="1:24">
-      <c r="A46" s="121"/>
+      <c r="A46" s="137"/>
       <c r="B46" s="91"/>
       <c r="C46" s="92"/>
       <c r="D46" s="25"/>
@@ -8768,11 +9204,11 @@
       <c r="X46" s="106"/>
     </row>
     <row r="47" spans="1:24">
-      <c r="A47" s="121"/>
-      <c r="B47" s="115">
+      <c r="A47" s="137"/>
+      <c r="B47" s="127">
         <v>12</v>
       </c>
-      <c r="C47" s="118" t="s">
+      <c r="C47" s="130" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="92">
@@ -8840,9 +9276,9 @@
       </c>
     </row>
     <row r="48" spans="1:24">
-      <c r="A48" s="121"/>
-      <c r="B48" s="116"/>
-      <c r="C48" s="118"/>
+      <c r="A48" s="137"/>
+      <c r="B48" s="128"/>
+      <c r="C48" s="130"/>
       <c r="D48" s="92">
         <v>2010</v>
       </c>
@@ -8908,9 +9344,9 @@
       </c>
     </row>
     <row r="49" spans="1:41">
-      <c r="A49" s="121"/>
-      <c r="B49" s="117"/>
-      <c r="C49" s="118"/>
+      <c r="A49" s="137"/>
+      <c r="B49" s="129"/>
+      <c r="C49" s="130"/>
       <c r="D49" s="25">
         <v>2014</v>
       </c>
@@ -8976,7 +9412,7 @@
       </c>
     </row>
     <row r="50" spans="1:41">
-      <c r="A50" s="121"/>
+      <c r="A50" s="137"/>
       <c r="B50" s="91"/>
       <c r="C50" s="92"/>
       <c r="D50" s="25"/>
@@ -8998,11 +9434,11 @@
       <c r="X50" s="106"/>
     </row>
     <row r="51" spans="1:41">
-      <c r="A51" s="121"/>
-      <c r="B51" s="115">
+      <c r="A51" s="137"/>
+      <c r="B51" s="127">
         <v>13</v>
       </c>
-      <c r="C51" s="118" t="s">
+      <c r="C51" s="130" t="s">
         <v>8</v>
       </c>
       <c r="D51" s="92">
@@ -9070,9 +9506,9 @@
       </c>
     </row>
     <row r="52" spans="1:41">
-      <c r="A52" s="121"/>
-      <c r="B52" s="116"/>
-      <c r="C52" s="118"/>
+      <c r="A52" s="137"/>
+      <c r="B52" s="128"/>
+      <c r="C52" s="130"/>
       <c r="D52" s="92">
         <v>2010</v>
       </c>
@@ -9138,9 +9574,9 @@
       </c>
     </row>
     <row r="53" spans="1:41">
-      <c r="A53" s="121"/>
-      <c r="B53" s="117"/>
-      <c r="C53" s="118"/>
+      <c r="A53" s="137"/>
+      <c r="B53" s="129"/>
+      <c r="C53" s="130"/>
       <c r="D53" s="25">
         <v>2014</v>
       </c>
@@ -9206,79 +9642,79 @@
       </c>
     </row>
     <row r="54" spans="1:41">
-      <c r="A54" s="121"/>
+      <c r="A54" s="137"/>
     </row>
     <row r="55" spans="1:41" s="75" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A55" s="121"/>
+      <c r="A55" s="137"/>
       <c r="B55" s="86"/>
-      <c r="C55" s="130" t="s">
+      <c r="C55" s="114" t="s">
         <v>50</v>
       </c>
-      <c r="D55" s="130"/>
-      <c r="E55" s="130"/>
-      <c r="F55" s="130" t="s">
+      <c r="D55" s="114"/>
+      <c r="E55" s="114"/>
+      <c r="F55" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="G55" s="130"/>
-      <c r="H55" s="130"/>
-      <c r="I55" s="130" t="s">
+      <c r="G55" s="114"/>
+      <c r="H55" s="114"/>
+      <c r="I55" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="J55" s="130"/>
-      <c r="K55" s="130"/>
-      <c r="L55" s="130" t="s">
+      <c r="J55" s="114"/>
+      <c r="K55" s="114"/>
+      <c r="L55" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="M55" s="130"/>
-      <c r="N55" s="130"/>
-      <c r="O55" s="130" t="s">
+      <c r="M55" s="114"/>
+      <c r="N55" s="114"/>
+      <c r="O55" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="P55" s="130"/>
-      <c r="Q55" s="130"/>
-      <c r="R55" s="127" t="s">
+      <c r="P55" s="114"/>
+      <c r="Q55" s="114"/>
+      <c r="R55" s="122" t="s">
         <v>87</v>
       </c>
-      <c r="S55" s="128"/>
-      <c r="T55" s="129"/>
-      <c r="U55" s="130" t="s">
+      <c r="S55" s="123"/>
+      <c r="T55" s="124"/>
+      <c r="U55" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="V55" s="130"/>
-      <c r="W55" s="130"/>
-      <c r="X55" s="127" t="s">
+      <c r="V55" s="114"/>
+      <c r="W55" s="114"/>
+      <c r="X55" s="122" t="s">
         <v>54</v>
       </c>
-      <c r="Y55" s="128"/>
-      <c r="Z55" s="129"/>
-      <c r="AA55" s="130" t="s">
+      <c r="Y55" s="123"/>
+      <c r="Z55" s="124"/>
+      <c r="AA55" s="114" t="s">
         <v>105</v>
       </c>
-      <c r="AB55" s="130"/>
-      <c r="AC55" s="130"/>
-      <c r="AD55" s="130" t="s">
+      <c r="AB55" s="114"/>
+      <c r="AC55" s="114"/>
+      <c r="AD55" s="114" t="s">
         <v>109</v>
       </c>
-      <c r="AE55" s="130"/>
-      <c r="AF55" s="130"/>
-      <c r="AG55" s="130" t="s">
+      <c r="AE55" s="114"/>
+      <c r="AF55" s="114"/>
+      <c r="AG55" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="AH55" s="130"/>
-      <c r="AI55" s="130"/>
-      <c r="AJ55" s="130" t="s">
+      <c r="AH55" s="114"/>
+      <c r="AI55" s="114"/>
+      <c r="AJ55" s="114" t="s">
         <v>13</v>
       </c>
-      <c r="AK55" s="130"/>
-      <c r="AL55" s="130"/>
-      <c r="AM55" s="130" t="s">
+      <c r="AK55" s="114"/>
+      <c r="AL55" s="114"/>
+      <c r="AM55" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="AN55" s="130"/>
-      <c r="AO55" s="130"/>
+      <c r="AN55" s="114"/>
+      <c r="AO55" s="114"/>
     </row>
     <row r="56" spans="1:41" s="75" customFormat="1" ht="70">
-      <c r="A56" s="122"/>
+      <c r="A56" s="138"/>
       <c r="B56" s="86"/>
       <c r="C56" s="86" t="s">
         <v>72</v>
@@ -9519,10 +9955,10 @@
       </c>
     </row>
     <row r="58" spans="1:41" s="79" customFormat="1" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A58" s="131" t="s">
+      <c r="A58" s="125" t="s">
         <v>129</v>
       </c>
-      <c r="B58" s="132"/>
+      <c r="B58" s="126"/>
       <c r="C58" s="79">
         <v>2006</v>
       </c>
@@ -9559,10 +9995,10 @@
       <c r="Y58" s="105"/>
     </row>
     <row r="59" spans="1:41" ht="16" thickTop="1">
-      <c r="A59" s="133" t="s">
+      <c r="A59" s="119" t="s">
         <v>125</v>
       </c>
-      <c r="B59" s="133"/>
+      <c r="B59" s="119"/>
       <c r="C59">
         <f xml:space="preserve"> C57/115</f>
         <v>3.4782608695652174E-2</v>
@@ -9721,10 +10157,10 @@
       </c>
     </row>
     <row r="60" spans="1:41">
-      <c r="A60" s="134" t="s">
+      <c r="A60" s="120" t="s">
         <v>124</v>
       </c>
-      <c r="B60" s="134"/>
+      <c r="B60" s="120"/>
       <c r="C60">
         <f xml:space="preserve"> C59*72</f>
         <v>2.5043478260869567</v>
@@ -9883,10 +10319,10 @@
       </c>
     </row>
     <row r="61" spans="1:41" s="80" customFormat="1">
-      <c r="A61" s="135" t="s">
+      <c r="A61" s="121" t="s">
         <v>126</v>
       </c>
-      <c r="B61" s="135"/>
+      <c r="B61" s="121"/>
       <c r="C61" s="80">
         <f xml:space="preserve"> 72-C60</f>
         <v>69.495652173913044</v>
@@ -10196,77 +10632,77 @@
       <c r="X66" s="85"/>
     </row>
     <row r="67" spans="1:41">
-      <c r="C67" s="130" t="s">
+      <c r="C67" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="D67" s="130"/>
-      <c r="E67" s="130"/>
-      <c r="F67" s="127" t="s">
+      <c r="D67" s="114"/>
+      <c r="E67" s="114"/>
+      <c r="F67" s="122" t="s">
         <v>54</v>
       </c>
-      <c r="G67" s="128"/>
-      <c r="H67" s="129"/>
-      <c r="I67" s="130" t="s">
+      <c r="G67" s="123"/>
+      <c r="H67" s="124"/>
+      <c r="I67" s="114" t="s">
         <v>105</v>
       </c>
-      <c r="J67" s="130"/>
-      <c r="K67" s="130"/>
-      <c r="L67" s="130" t="s">
+      <c r="J67" s="114"/>
+      <c r="K67" s="114"/>
+      <c r="L67" s="114" t="s">
         <v>50</v>
       </c>
-      <c r="M67" s="130"/>
-      <c r="N67" s="130"/>
-      <c r="O67" s="130" t="s">
+      <c r="M67" s="114"/>
+      <c r="N67" s="114"/>
+      <c r="O67" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="P67" s="130"/>
-      <c r="Q67" s="130"/>
-      <c r="R67" s="127" t="s">
+      <c r="P67" s="114"/>
+      <c r="Q67" s="114"/>
+      <c r="R67" s="122" t="s">
         <v>87</v>
       </c>
-      <c r="S67" s="128"/>
-      <c r="T67" s="129"/>
-      <c r="U67" s="130" t="s">
+      <c r="S67" s="123"/>
+      <c r="T67" s="124"/>
+      <c r="U67" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="V67" s="130"/>
-      <c r="W67" s="130"/>
-      <c r="X67" s="130" t="s">
+      <c r="V67" s="114"/>
+      <c r="W67" s="114"/>
+      <c r="X67" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="Y67" s="130"/>
-      <c r="Z67" s="130"/>
-      <c r="AA67" s="130" t="s">
+      <c r="Y67" s="114"/>
+      <c r="Z67" s="114"/>
+      <c r="AA67" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="AB67" s="130"/>
-      <c r="AC67" s="130"/>
-      <c r="AD67" s="130" t="s">
+      <c r="AB67" s="114"/>
+      <c r="AC67" s="114"/>
+      <c r="AD67" s="114" t="s">
         <v>109</v>
       </c>
-      <c r="AE67" s="130"/>
-      <c r="AF67" s="130"/>
-      <c r="AG67" s="130" t="s">
+      <c r="AE67" s="114"/>
+      <c r="AF67" s="114"/>
+      <c r="AG67" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="AH67" s="130"/>
-      <c r="AI67" s="130"/>
-      <c r="AJ67" s="130" t="s">
+      <c r="AH67" s="114"/>
+      <c r="AI67" s="114"/>
+      <c r="AJ67" s="114" t="s">
         <v>13</v>
       </c>
-      <c r="AK67" s="130"/>
-      <c r="AL67" s="130"/>
-      <c r="AM67" s="130" t="s">
+      <c r="AK67" s="114"/>
+      <c r="AL67" s="114"/>
+      <c r="AM67" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="AN67" s="130"/>
-      <c r="AO67" s="130"/>
+      <c r="AN67" s="114"/>
+      <c r="AO67" s="114"/>
     </row>
     <row r="68" spans="1:41" ht="70">
-      <c r="A68" s="136" t="s">
+      <c r="A68" s="115" t="s">
         <v>128</v>
       </c>
-      <c r="B68" s="137"/>
+      <c r="B68" s="116"/>
       <c r="C68" s="86" t="s">
         <v>99</v>
       </c>
@@ -10386,8 +10822,8 @@
       </c>
     </row>
     <row r="69" spans="1:41" ht="16" thickBot="1">
-      <c r="A69" s="138"/>
-      <c r="B69" s="139"/>
+      <c r="A69" s="117"/>
+      <c r="B69" s="118"/>
       <c r="C69" s="86">
         <v>23</v>
       </c>
@@ -10507,10 +10943,10 @@
       </c>
     </row>
     <row r="70" spans="1:41" ht="16" thickTop="1">
-      <c r="A70" s="133" t="s">
+      <c r="A70" s="119" t="s">
         <v>125</v>
       </c>
-      <c r="B70" s="133"/>
+      <c r="B70" s="119"/>
       <c r="C70">
         <f xml:space="preserve"> C69/115</f>
         <v>0.2</v>
@@ -10669,10 +11105,10 @@
       </c>
     </row>
     <row r="71" spans="1:41">
-      <c r="A71" s="134" t="s">
+      <c r="A71" s="120" t="s">
         <v>124</v>
       </c>
-      <c r="B71" s="134"/>
+      <c r="B71" s="120"/>
       <c r="C71">
         <f xml:space="preserve"> C70*65</f>
         <v>13</v>
@@ -10831,10 +11267,10 @@
       </c>
     </row>
     <row r="72" spans="1:41">
-      <c r="A72" s="135" t="s">
+      <c r="A72" s="121" t="s">
         <v>126</v>
       </c>
-      <c r="B72" s="135"/>
+      <c r="B72" s="121"/>
       <c r="C72" s="80">
         <f xml:space="preserve"> 65-C71</f>
         <v>52</v>
@@ -10999,23 +11435,41 @@
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="AJ67:AL67"/>
-    <mergeCell ref="AM67:AO67"/>
-    <mergeCell ref="A68:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="AD67:AF67"/>
-    <mergeCell ref="AG67:AI67"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="R67:T67"/>
-    <mergeCell ref="U67:W67"/>
-    <mergeCell ref="X67:Z67"/>
-    <mergeCell ref="AA67:AC67"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="I67:K67"/>
-    <mergeCell ref="L67:N67"/>
-    <mergeCell ref="O67:Q67"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="A3:A56"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="R55:T55"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="C51:C53"/>
     <mergeCell ref="AM55:AO55"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A59:B59"/>
@@ -11032,41 +11486,23 @@
     <mergeCell ref="I55:K55"/>
     <mergeCell ref="L55:N55"/>
     <mergeCell ref="O55:Q55"/>
-    <mergeCell ref="R55:T55"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="B51:B53"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="A3:A56"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="R67:T67"/>
+    <mergeCell ref="U67:W67"/>
+    <mergeCell ref="X67:Z67"/>
+    <mergeCell ref="AA67:AC67"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="I67:K67"/>
+    <mergeCell ref="L67:N67"/>
+    <mergeCell ref="O67:Q67"/>
+    <mergeCell ref="AJ67:AL67"/>
+    <mergeCell ref="AM67:AO67"/>
+    <mergeCell ref="A68:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="AD67:AF67"/>
+    <mergeCell ref="AG67:AI67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -11083,8 +11519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:J1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11110,37 +11546,37 @@
     <row r="1" spans="1:24" ht="34" customHeight="1">
       <c r="A1" s="57"/>
       <c r="B1" s="57"/>
-      <c r="C1" s="118" t="s">
+      <c r="C1" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="118" t="s">
+      <c r="D1" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="118" t="s">
+      <c r="E1" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="139" t="s">
         <v>199</v>
       </c>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="119" t="s">
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="134" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
-      <c r="N1" s="119"/>
-      <c r="O1" s="114" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="114"/>
-      <c r="Q1" s="119" t="s">
+      <c r="L1" s="134"/>
+      <c r="M1" s="134"/>
+      <c r="N1" s="134"/>
+      <c r="O1" s="135" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="135"/>
+      <c r="Q1" s="134" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="119"/>
-      <c r="S1" s="119"/>
+      <c r="R1" s="134"/>
+      <c r="S1" s="134"/>
       <c r="T1" s="71" t="s">
         <v>92</v>
       </c>
@@ -11153,16 +11589,16 @@
       <c r="W1" s="71" t="s">
         <v>133</v>
       </c>
-      <c r="X1" s="118" t="s">
+      <c r="X1" s="130" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="144">
       <c r="A2" s="57"/>
       <c r="B2" s="57"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -11217,16 +11653,16 @@
       <c r="W2" s="72" t="s">
         <v>98</v>
       </c>
-      <c r="X2" s="118"/>
+      <c r="X2" s="130"/>
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="136" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="115">
-        <v>1</v>
-      </c>
-      <c r="C3" s="118" t="s">
+      <c r="B3" s="127">
+        <v>1</v>
+      </c>
+      <c r="C3" s="130" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="54">
@@ -11294,9 +11730,9 @@
       </c>
     </row>
     <row r="4" spans="1:24">
-      <c r="A4" s="121"/>
-      <c r="B4" s="116"/>
-      <c r="C4" s="118"/>
+      <c r="A4" s="137"/>
+      <c r="B4" s="128"/>
+      <c r="C4" s="130"/>
       <c r="D4" s="54">
         <v>2010</v>
       </c>
@@ -11362,9 +11798,9 @@
       </c>
     </row>
     <row r="5" spans="1:24">
-      <c r="A5" s="121"/>
-      <c r="B5" s="117"/>
-      <c r="C5" s="118"/>
+      <c r="A5" s="137"/>
+      <c r="B5" s="129"/>
+      <c r="C5" s="130"/>
       <c r="D5" s="25">
         <v>2014</v>
       </c>
@@ -11430,11 +11866,11 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="15" customHeight="1">
-      <c r="A6" s="121"/>
-      <c r="B6" s="115">
+      <c r="A6" s="137"/>
+      <c r="B6" s="127">
         <v>2</v>
       </c>
-      <c r="C6" s="118" t="s">
+      <c r="C6" s="130" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="54">
@@ -11502,9 +11938,9 @@
       </c>
     </row>
     <row r="7" spans="1:24">
-      <c r="A7" s="121"/>
-      <c r="B7" s="116"/>
-      <c r="C7" s="118"/>
+      <c r="A7" s="137"/>
+      <c r="B7" s="128"/>
+      <c r="C7" s="130"/>
       <c r="D7" s="54">
         <v>2010</v>
       </c>
@@ -11570,9 +12006,9 @@
       </c>
     </row>
     <row r="8" spans="1:24">
-      <c r="A8" s="121"/>
-      <c r="B8" s="117"/>
-      <c r="C8" s="118"/>
+      <c r="A8" s="137"/>
+      <c r="B8" s="129"/>
+      <c r="C8" s="130"/>
       <c r="D8" s="25">
         <v>2014</v>
       </c>
@@ -11638,11 +12074,11 @@
       </c>
     </row>
     <row r="9" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A9" s="121"/>
-      <c r="B9" s="115">
+      <c r="A9" s="137"/>
+      <c r="B9" s="127">
         <v>3</v>
       </c>
-      <c r="C9" s="118" t="s">
+      <c r="C9" s="130" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="54">
@@ -11710,9 +12146,9 @@
       </c>
     </row>
     <row r="10" spans="1:24">
-      <c r="A10" s="121"/>
-      <c r="B10" s="116"/>
-      <c r="C10" s="118"/>
+      <c r="A10" s="137"/>
+      <c r="B10" s="128"/>
+      <c r="C10" s="130"/>
       <c r="D10" s="54">
         <v>2010</v>
       </c>
@@ -11778,9 +12214,9 @@
       </c>
     </row>
     <row r="11" spans="1:24">
-      <c r="A11" s="121"/>
-      <c r="B11" s="117"/>
-      <c r="C11" s="118"/>
+      <c r="A11" s="137"/>
+      <c r="B11" s="129"/>
+      <c r="C11" s="130"/>
       <c r="D11" s="25">
         <v>2014</v>
       </c>
@@ -11846,11 +12282,11 @@
       </c>
     </row>
     <row r="12" spans="1:24">
-      <c r="A12" s="121"/>
-      <c r="B12" s="115">
+      <c r="A12" s="137"/>
+      <c r="B12" s="127">
         <v>4</v>
       </c>
-      <c r="C12" s="118" t="s">
+      <c r="C12" s="130" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="54">
@@ -11918,9 +12354,9 @@
       </c>
     </row>
     <row r="13" spans="1:24">
-      <c r="A13" s="121"/>
-      <c r="B13" s="116"/>
-      <c r="C13" s="118"/>
+      <c r="A13" s="137"/>
+      <c r="B13" s="128"/>
+      <c r="C13" s="130"/>
       <c r="D13" s="54">
         <v>2010</v>
       </c>
@@ -11986,9 +12422,9 @@
       </c>
     </row>
     <row r="14" spans="1:24">
-      <c r="A14" s="121"/>
-      <c r="B14" s="117"/>
-      <c r="C14" s="118"/>
+      <c r="A14" s="137"/>
+      <c r="B14" s="129"/>
+      <c r="C14" s="130"/>
       <c r="D14" s="25">
         <v>2014</v>
       </c>
@@ -12054,11 +12490,11 @@
       </c>
     </row>
     <row r="15" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A15" s="121"/>
-      <c r="B15" s="115">
+      <c r="A15" s="137"/>
+      <c r="B15" s="127">
         <v>5</v>
       </c>
-      <c r="C15" s="118" t="s">
+      <c r="C15" s="130" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="54">
@@ -12126,9 +12562,9 @@
       </c>
     </row>
     <row r="16" spans="1:24">
-      <c r="A16" s="121"/>
-      <c r="B16" s="116"/>
-      <c r="C16" s="118"/>
+      <c r="A16" s="137"/>
+      <c r="B16" s="128"/>
+      <c r="C16" s="130"/>
       <c r="D16" s="54">
         <v>2010</v>
       </c>
@@ -12194,9 +12630,9 @@
       </c>
     </row>
     <row r="17" spans="1:24">
-      <c r="A17" s="121"/>
-      <c r="B17" s="117"/>
-      <c r="C17" s="118"/>
+      <c r="A17" s="137"/>
+      <c r="B17" s="129"/>
+      <c r="C17" s="130"/>
       <c r="D17" s="25">
         <v>2014</v>
       </c>
@@ -12262,11 +12698,11 @@
       </c>
     </row>
     <row r="18" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A18" s="121"/>
-      <c r="B18" s="115">
+      <c r="A18" s="137"/>
+      <c r="B18" s="127">
         <v>6</v>
       </c>
-      <c r="C18" s="118" t="s">
+      <c r="C18" s="130" t="s">
         <v>25</v>
       </c>
       <c r="D18" s="54">
@@ -12334,9 +12770,9 @@
       </c>
     </row>
     <row r="19" spans="1:24">
-      <c r="A19" s="121"/>
-      <c r="B19" s="116"/>
-      <c r="C19" s="118"/>
+      <c r="A19" s="137"/>
+      <c r="B19" s="128"/>
+      <c r="C19" s="130"/>
       <c r="D19" s="54">
         <v>2010</v>
       </c>
@@ -12402,9 +12838,9 @@
       </c>
     </row>
     <row r="20" spans="1:24">
-      <c r="A20" s="121"/>
-      <c r="B20" s="117"/>
-      <c r="C20" s="118"/>
+      <c r="A20" s="137"/>
+      <c r="B20" s="129"/>
+      <c r="C20" s="130"/>
       <c r="D20" s="25">
         <v>2014</v>
       </c>
@@ -12470,11 +12906,11 @@
       </c>
     </row>
     <row r="21" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A21" s="121"/>
-      <c r="B21" s="115">
+      <c r="A21" s="137"/>
+      <c r="B21" s="127">
         <v>7</v>
       </c>
-      <c r="C21" s="118" t="s">
+      <c r="C21" s="130" t="s">
         <v>70</v>
       </c>
       <c r="D21" s="54">
@@ -12542,9 +12978,9 @@
       </c>
     </row>
     <row r="22" spans="1:24">
-      <c r="A22" s="121"/>
-      <c r="B22" s="116"/>
-      <c r="C22" s="118"/>
+      <c r="A22" s="137"/>
+      <c r="B22" s="128"/>
+      <c r="C22" s="130"/>
       <c r="D22" s="54">
         <v>2010</v>
       </c>
@@ -12610,9 +13046,9 @@
       </c>
     </row>
     <row r="23" spans="1:24">
-      <c r="A23" s="121"/>
-      <c r="B23" s="117"/>
-      <c r="C23" s="118"/>
+      <c r="A23" s="137"/>
+      <c r="B23" s="129"/>
+      <c r="C23" s="130"/>
       <c r="D23" s="25">
         <v>2014</v>
       </c>
@@ -12678,11 +13114,11 @@
       </c>
     </row>
     <row r="24" spans="1:24">
-      <c r="A24" s="121"/>
-      <c r="B24" s="115">
+      <c r="A24" s="137"/>
+      <c r="B24" s="127">
         <v>8</v>
       </c>
-      <c r="C24" s="124" t="s">
+      <c r="C24" s="131" t="s">
         <v>54</v>
       </c>
       <c r="D24" s="54">
@@ -12750,9 +13186,9 @@
       </c>
     </row>
     <row r="25" spans="1:24">
-      <c r="A25" s="121"/>
-      <c r="B25" s="116"/>
-      <c r="C25" s="125"/>
+      <c r="A25" s="137"/>
+      <c r="B25" s="128"/>
+      <c r="C25" s="132"/>
       <c r="D25" s="54">
         <v>2010</v>
       </c>
@@ -12818,9 +13254,9 @@
       </c>
     </row>
     <row r="26" spans="1:24">
-      <c r="A26" s="121"/>
-      <c r="B26" s="117"/>
-      <c r="C26" s="126"/>
+      <c r="A26" s="137"/>
+      <c r="B26" s="129"/>
+      <c r="C26" s="133"/>
       <c r="D26" s="25">
         <v>2014</v>
       </c>
@@ -12886,11 +13322,11 @@
       </c>
     </row>
     <row r="27" spans="1:24">
-      <c r="A27" s="121"/>
-      <c r="B27" s="115">
+      <c r="A27" s="137"/>
+      <c r="B27" s="127">
         <v>9</v>
       </c>
-      <c r="C27" s="118" t="s">
+      <c r="C27" s="130" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="54">
@@ -12958,9 +13394,9 @@
       </c>
     </row>
     <row r="28" spans="1:24">
-      <c r="A28" s="121"/>
-      <c r="B28" s="116"/>
-      <c r="C28" s="118"/>
+      <c r="A28" s="137"/>
+      <c r="B28" s="128"/>
+      <c r="C28" s="130"/>
       <c r="D28" s="54">
         <v>2010</v>
       </c>
@@ -13026,9 +13462,9 @@
       </c>
     </row>
     <row r="29" spans="1:24">
-      <c r="A29" s="121"/>
-      <c r="B29" s="117"/>
-      <c r="C29" s="118"/>
+      <c r="A29" s="137"/>
+      <c r="B29" s="129"/>
+      <c r="C29" s="130"/>
       <c r="D29" s="25">
         <v>2014</v>
       </c>
@@ -13094,11 +13530,11 @@
       </c>
     </row>
     <row r="30" spans="1:24">
-      <c r="A30" s="121"/>
-      <c r="B30" s="115">
+      <c r="A30" s="137"/>
+      <c r="B30" s="127">
         <v>10</v>
       </c>
-      <c r="C30" s="118" t="s">
+      <c r="C30" s="130" t="s">
         <v>28</v>
       </c>
       <c r="D30" s="54">
@@ -13166,9 +13602,9 @@
       </c>
     </row>
     <row r="31" spans="1:24">
-      <c r="A31" s="121"/>
-      <c r="B31" s="116"/>
-      <c r="C31" s="118"/>
+      <c r="A31" s="137"/>
+      <c r="B31" s="128"/>
+      <c r="C31" s="130"/>
       <c r="D31" s="54">
         <v>2010</v>
       </c>
@@ -13234,9 +13670,9 @@
       </c>
     </row>
     <row r="32" spans="1:24">
-      <c r="A32" s="121"/>
-      <c r="B32" s="117"/>
-      <c r="C32" s="118"/>
+      <c r="A32" s="137"/>
+      <c r="B32" s="129"/>
+      <c r="C32" s="130"/>
       <c r="D32" s="25">
         <v>2014</v>
       </c>
@@ -13302,11 +13738,11 @@
       </c>
     </row>
     <row r="33" spans="1:41">
-      <c r="A33" s="121"/>
-      <c r="B33" s="115">
+      <c r="A33" s="137"/>
+      <c r="B33" s="127">
         <v>11</v>
       </c>
-      <c r="C33" s="118" t="s">
+      <c r="C33" s="130" t="s">
         <v>21</v>
       </c>
       <c r="D33" s="54">
@@ -13374,9 +13810,9 @@
       </c>
     </row>
     <row r="34" spans="1:41">
-      <c r="A34" s="121"/>
-      <c r="B34" s="116"/>
-      <c r="C34" s="118"/>
+      <c r="A34" s="137"/>
+      <c r="B34" s="128"/>
+      <c r="C34" s="130"/>
       <c r="D34" s="54">
         <v>2010</v>
       </c>
@@ -13442,9 +13878,9 @@
       </c>
     </row>
     <row r="35" spans="1:41">
-      <c r="A35" s="121"/>
-      <c r="B35" s="117"/>
-      <c r="C35" s="118"/>
+      <c r="A35" s="137"/>
+      <c r="B35" s="129"/>
+      <c r="C35" s="130"/>
       <c r="D35" s="25">
         <v>2014</v>
       </c>
@@ -13510,11 +13946,11 @@
       </c>
     </row>
     <row r="36" spans="1:41">
-      <c r="A36" s="121"/>
-      <c r="B36" s="115">
+      <c r="A36" s="137"/>
+      <c r="B36" s="127">
         <v>12</v>
       </c>
-      <c r="C36" s="118" t="s">
+      <c r="C36" s="130" t="s">
         <v>13</v>
       </c>
       <c r="D36" s="54">
@@ -13582,9 +14018,9 @@
       </c>
     </row>
     <row r="37" spans="1:41">
-      <c r="A37" s="121"/>
-      <c r="B37" s="116"/>
-      <c r="C37" s="118"/>
+      <c r="A37" s="137"/>
+      <c r="B37" s="128"/>
+      <c r="C37" s="130"/>
       <c r="D37" s="54">
         <v>2010</v>
       </c>
@@ -13650,9 +14086,9 @@
       </c>
     </row>
     <row r="38" spans="1:41">
-      <c r="A38" s="121"/>
-      <c r="B38" s="117"/>
-      <c r="C38" s="118"/>
+      <c r="A38" s="137"/>
+      <c r="B38" s="129"/>
+      <c r="C38" s="130"/>
       <c r="D38" s="25">
         <v>2014</v>
       </c>
@@ -13718,11 +14154,11 @@
       </c>
     </row>
     <row r="39" spans="1:41">
-      <c r="A39" s="121"/>
-      <c r="B39" s="115">
+      <c r="A39" s="137"/>
+      <c r="B39" s="127">
         <v>13</v>
       </c>
-      <c r="C39" s="118" t="s">
+      <c r="C39" s="130" t="s">
         <v>8</v>
       </c>
       <c r="D39" s="54">
@@ -13790,9 +14226,9 @@
       </c>
     </row>
     <row r="40" spans="1:41">
-      <c r="A40" s="121"/>
-      <c r="B40" s="116"/>
-      <c r="C40" s="118"/>
+      <c r="A40" s="137"/>
+      <c r="B40" s="128"/>
+      <c r="C40" s="130"/>
       <c r="D40" s="54">
         <v>2010</v>
       </c>
@@ -13858,9 +14294,9 @@
       </c>
     </row>
     <row r="41" spans="1:41">
-      <c r="A41" s="121"/>
-      <c r="B41" s="117"/>
-      <c r="C41" s="118"/>
+      <c r="A41" s="137"/>
+      <c r="B41" s="129"/>
+      <c r="C41" s="130"/>
       <c r="D41" s="25">
         <v>2014</v>
       </c>
@@ -13926,79 +14362,79 @@
       </c>
     </row>
     <row r="42" spans="1:41">
-      <c r="A42" s="121"/>
+      <c r="A42" s="137"/>
     </row>
     <row r="43" spans="1:41" s="75" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A43" s="121"/>
+      <c r="A43" s="137"/>
       <c r="B43" s="73"/>
-      <c r="C43" s="130" t="s">
+      <c r="C43" s="114" t="s">
         <v>50</v>
       </c>
-      <c r="D43" s="130"/>
-      <c r="E43" s="130"/>
-      <c r="F43" s="130" t="s">
+      <c r="D43" s="114"/>
+      <c r="E43" s="114"/>
+      <c r="F43" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="G43" s="130"/>
-      <c r="H43" s="130"/>
-      <c r="I43" s="130" t="s">
+      <c r="G43" s="114"/>
+      <c r="H43" s="114"/>
+      <c r="I43" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="J43" s="130"/>
-      <c r="K43" s="130"/>
-      <c r="L43" s="130" t="s">
+      <c r="J43" s="114"/>
+      <c r="K43" s="114"/>
+      <c r="L43" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="M43" s="130"/>
-      <c r="N43" s="130"/>
-      <c r="O43" s="130" t="s">
+      <c r="M43" s="114"/>
+      <c r="N43" s="114"/>
+      <c r="O43" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="P43" s="130"/>
-      <c r="Q43" s="130"/>
-      <c r="R43" s="127" t="s">
+      <c r="P43" s="114"/>
+      <c r="Q43" s="114"/>
+      <c r="R43" s="122" t="s">
         <v>87</v>
       </c>
-      <c r="S43" s="128"/>
-      <c r="T43" s="129"/>
-      <c r="U43" s="130" t="s">
+      <c r="S43" s="123"/>
+      <c r="T43" s="124"/>
+      <c r="U43" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="V43" s="130"/>
-      <c r="W43" s="130"/>
-      <c r="X43" s="127" t="s">
+      <c r="V43" s="114"/>
+      <c r="W43" s="114"/>
+      <c r="X43" s="122" t="s">
         <v>54</v>
       </c>
-      <c r="Y43" s="128"/>
-      <c r="Z43" s="129"/>
-      <c r="AA43" s="130" t="s">
+      <c r="Y43" s="123"/>
+      <c r="Z43" s="124"/>
+      <c r="AA43" s="114" t="s">
         <v>105</v>
       </c>
-      <c r="AB43" s="130"/>
-      <c r="AC43" s="130"/>
-      <c r="AD43" s="130" t="s">
+      <c r="AB43" s="114"/>
+      <c r="AC43" s="114"/>
+      <c r="AD43" s="114" t="s">
         <v>109</v>
       </c>
-      <c r="AE43" s="130"/>
-      <c r="AF43" s="130"/>
-      <c r="AG43" s="130" t="s">
+      <c r="AE43" s="114"/>
+      <c r="AF43" s="114"/>
+      <c r="AG43" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="AH43" s="130"/>
-      <c r="AI43" s="130"/>
-      <c r="AJ43" s="130" t="s">
+      <c r="AH43" s="114"/>
+      <c r="AI43" s="114"/>
+      <c r="AJ43" s="114" t="s">
         <v>13</v>
       </c>
-      <c r="AK43" s="130"/>
-      <c r="AL43" s="130"/>
-      <c r="AM43" s="130" t="s">
+      <c r="AK43" s="114"/>
+      <c r="AL43" s="114"/>
+      <c r="AM43" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="AN43" s="130"/>
-      <c r="AO43" s="130"/>
+      <c r="AN43" s="114"/>
+      <c r="AO43" s="114"/>
     </row>
     <row r="44" spans="1:41" s="75" customFormat="1" ht="70">
-      <c r="A44" s="122"/>
+      <c r="A44" s="138"/>
       <c r="B44" s="73"/>
       <c r="C44" s="73" t="s">
         <v>72</v>
@@ -14239,10 +14675,10 @@
       </c>
     </row>
     <row r="46" spans="1:41" s="79" customFormat="1" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A46" s="131" t="s">
+      <c r="A46" s="125" t="s">
         <v>129</v>
       </c>
-      <c r="B46" s="132"/>
+      <c r="B46" s="126"/>
       <c r="C46" s="79">
         <v>2006</v>
       </c>
@@ -14279,10 +14715,10 @@
       <c r="Y46" s="105"/>
     </row>
     <row r="47" spans="1:41" ht="16" thickTop="1">
-      <c r="A47" s="133" t="s">
+      <c r="A47" s="119" t="s">
         <v>125</v>
       </c>
-      <c r="B47" s="133"/>
+      <c r="B47" s="119"/>
       <c r="C47">
         <f xml:space="preserve"> C45/115</f>
         <v>3.4782608695652174E-2</v>
@@ -14441,10 +14877,10 @@
       </c>
     </row>
     <row r="48" spans="1:41">
-      <c r="A48" s="134" t="s">
+      <c r="A48" s="120" t="s">
         <v>124</v>
       </c>
-      <c r="B48" s="134"/>
+      <c r="B48" s="120"/>
       <c r="C48">
         <f xml:space="preserve"> C47*72</f>
         <v>2.5043478260869567</v>
@@ -14603,10 +15039,10 @@
       </c>
     </row>
     <row r="49" spans="1:41" s="80" customFormat="1">
-      <c r="A49" s="135" t="s">
+      <c r="A49" s="121" t="s">
         <v>126</v>
       </c>
-      <c r="B49" s="135"/>
+      <c r="B49" s="121"/>
       <c r="C49" s="80">
         <f xml:space="preserve"> 72-C48</f>
         <v>69.495652173913044</v>
@@ -14916,77 +15352,77 @@
       <c r="X54" s="85"/>
     </row>
     <row r="55" spans="1:41">
-      <c r="C55" s="130" t="s">
+      <c r="C55" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="D55" s="130"/>
-      <c r="E55" s="130"/>
-      <c r="F55" s="127" t="s">
+      <c r="D55" s="114"/>
+      <c r="E55" s="114"/>
+      <c r="F55" s="122" t="s">
         <v>54</v>
       </c>
-      <c r="G55" s="128"/>
-      <c r="H55" s="129"/>
-      <c r="I55" s="130" t="s">
+      <c r="G55" s="123"/>
+      <c r="H55" s="124"/>
+      <c r="I55" s="114" t="s">
         <v>105</v>
       </c>
-      <c r="J55" s="130"/>
-      <c r="K55" s="130"/>
-      <c r="L55" s="130" t="s">
+      <c r="J55" s="114"/>
+      <c r="K55" s="114"/>
+      <c r="L55" s="114" t="s">
         <v>50</v>
       </c>
-      <c r="M55" s="130"/>
-      <c r="N55" s="130"/>
-      <c r="O55" s="130" t="s">
+      <c r="M55" s="114"/>
+      <c r="N55" s="114"/>
+      <c r="O55" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="P55" s="130"/>
-      <c r="Q55" s="130"/>
-      <c r="R55" s="127" t="s">
+      <c r="P55" s="114"/>
+      <c r="Q55" s="114"/>
+      <c r="R55" s="122" t="s">
         <v>87</v>
       </c>
-      <c r="S55" s="128"/>
-      <c r="T55" s="129"/>
-      <c r="U55" s="130" t="s">
+      <c r="S55" s="123"/>
+      <c r="T55" s="124"/>
+      <c r="U55" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="V55" s="130"/>
-      <c r="W55" s="130"/>
-      <c r="X55" s="130" t="s">
+      <c r="V55" s="114"/>
+      <c r="W55" s="114"/>
+      <c r="X55" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="Y55" s="130"/>
-      <c r="Z55" s="130"/>
-      <c r="AA55" s="130" t="s">
+      <c r="Y55" s="114"/>
+      <c r="Z55" s="114"/>
+      <c r="AA55" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="AB55" s="130"/>
-      <c r="AC55" s="130"/>
-      <c r="AD55" s="130" t="s">
+      <c r="AB55" s="114"/>
+      <c r="AC55" s="114"/>
+      <c r="AD55" s="114" t="s">
         <v>109</v>
       </c>
-      <c r="AE55" s="130"/>
-      <c r="AF55" s="130"/>
-      <c r="AG55" s="130" t="s">
+      <c r="AE55" s="114"/>
+      <c r="AF55" s="114"/>
+      <c r="AG55" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="AH55" s="130"/>
-      <c r="AI55" s="130"/>
-      <c r="AJ55" s="130" t="s">
+      <c r="AH55" s="114"/>
+      <c r="AI55" s="114"/>
+      <c r="AJ55" s="114" t="s">
         <v>13</v>
       </c>
-      <c r="AK55" s="130"/>
-      <c r="AL55" s="130"/>
-      <c r="AM55" s="130" t="s">
+      <c r="AK55" s="114"/>
+      <c r="AL55" s="114"/>
+      <c r="AM55" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="AN55" s="130"/>
-      <c r="AO55" s="130"/>
+      <c r="AN55" s="114"/>
+      <c r="AO55" s="114"/>
     </row>
     <row r="56" spans="1:41" ht="70">
-      <c r="A56" s="136" t="s">
+      <c r="A56" s="115" t="s">
         <v>128</v>
       </c>
-      <c r="B56" s="137"/>
+      <c r="B56" s="116"/>
       <c r="C56" s="74" t="s">
         <v>99</v>
       </c>
@@ -15106,8 +15542,8 @@
       </c>
     </row>
     <row r="57" spans="1:41" ht="16" thickBot="1">
-      <c r="A57" s="138"/>
-      <c r="B57" s="139"/>
+      <c r="A57" s="117"/>
+      <c r="B57" s="118"/>
       <c r="C57" s="74">
         <v>23</v>
       </c>
@@ -15227,10 +15663,10 @@
       </c>
     </row>
     <row r="58" spans="1:41" ht="16" thickTop="1">
-      <c r="A58" s="133" t="s">
+      <c r="A58" s="119" t="s">
         <v>125</v>
       </c>
-      <c r="B58" s="133"/>
+      <c r="B58" s="119"/>
       <c r="C58">
         <f xml:space="preserve"> C57/115</f>
         <v>0.2</v>
@@ -15389,10 +15825,10 @@
       </c>
     </row>
     <row r="59" spans="1:41">
-      <c r="A59" s="134" t="s">
+      <c r="A59" s="120" t="s">
         <v>124</v>
       </c>
-      <c r="B59" s="134"/>
+      <c r="B59" s="120"/>
       <c r="C59">
         <f xml:space="preserve"> C58*65</f>
         <v>13</v>
@@ -15551,10 +15987,10 @@
       </c>
     </row>
     <row r="60" spans="1:41">
-      <c r="A60" s="135" t="s">
+      <c r="A60" s="121" t="s">
         <v>126</v>
       </c>
-      <c r="B60" s="135"/>
+      <c r="B60" s="121"/>
       <c r="C60" s="80">
         <f xml:space="preserve"> 65-C59</f>
         <v>52</v>
@@ -15719,6 +16155,59 @@
     </row>
   </sheetData>
   <mergeCells count="69">
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="AD43:AF43"/>
+    <mergeCell ref="AG43:AI43"/>
+    <mergeCell ref="AJ43:AL43"/>
+    <mergeCell ref="AM43:AO43"/>
+    <mergeCell ref="X43:Z43"/>
+    <mergeCell ref="AA43:AC43"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="L43:N43"/>
+    <mergeCell ref="O43:Q43"/>
+    <mergeCell ref="U43:W43"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="AM55:AO55"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="AD55:AF55"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="A3:A44"/>
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="B30:B32"/>
     <mergeCell ref="A60:B60"/>
     <mergeCell ref="A56:B57"/>
     <mergeCell ref="A46:B46"/>
@@ -15735,59 +16224,6 @@
     <mergeCell ref="I55:K55"/>
     <mergeCell ref="L55:N55"/>
     <mergeCell ref="R55:T55"/>
-    <mergeCell ref="AM55:AO55"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="AD55:AF55"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="AD43:AF43"/>
-    <mergeCell ref="AG43:AI43"/>
-    <mergeCell ref="AJ43:AL43"/>
-    <mergeCell ref="AM43:AO43"/>
-    <mergeCell ref="X43:Z43"/>
-    <mergeCell ref="AA43:AC43"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="L43:N43"/>
-    <mergeCell ref="O43:Q43"/>
-    <mergeCell ref="U43:W43"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="A3:A44"/>
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -15817,44 +16253,44 @@
     <row r="1" spans="1:19">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="118" t="s">
+      <c r="C1" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="118" t="s">
+      <c r="D1" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="118" t="s">
+      <c r="E1" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="139" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="119" t="s">
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="134" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
-      <c r="N1" s="119"/>
-      <c r="O1" s="114" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="114"/>
-      <c r="Q1" s="119" t="s">
+      <c r="L1" s="134"/>
+      <c r="M1" s="134"/>
+      <c r="N1" s="134"/>
+      <c r="O1" s="135" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="135"/>
+      <c r="Q1" s="134" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="119"/>
-      <c r="S1" s="119"/>
+      <c r="R1" s="134"/>
+      <c r="S1" s="134"/>
     </row>
     <row r="2" spans="1:19" ht="84">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -15899,7 +16335,7 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="136" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="47" t="s">
@@ -15958,7 +16394,7 @@
       </c>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="121"/>
+      <c r="A4" s="137"/>
       <c r="B4" s="45" t="s">
         <v>55</v>
       </c>
@@ -16015,7 +16451,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A5" s="121"/>
+      <c r="A5" s="137"/>
       <c r="B5" s="45" t="s">
         <v>57</v>
       </c>
@@ -16072,7 +16508,7 @@
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="121"/>
+      <c r="A6" s="137"/>
       <c r="B6" s="45" t="s">
         <v>58</v>
       </c>
@@ -16129,7 +16565,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A7" s="121"/>
+      <c r="A7" s="137"/>
       <c r="B7" s="45" t="s">
         <v>59</v>
       </c>
@@ -16186,7 +16622,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A8" s="121"/>
+      <c r="A8" s="137"/>
       <c r="B8" s="45" t="s">
         <v>60</v>
       </c>
@@ -16243,7 +16679,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A9" s="121"/>
+      <c r="A9" s="137"/>
       <c r="B9" s="45" t="s">
         <v>61</v>
       </c>
@@ -16300,7 +16736,7 @@
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="121"/>
+      <c r="A10" s="137"/>
       <c r="B10" s="45" t="s">
         <v>62</v>
       </c>
@@ -16357,7 +16793,7 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="121"/>
+      <c r="A11" s="137"/>
       <c r="B11" s="45" t="s">
         <v>56</v>
       </c>
@@ -16414,7 +16850,7 @@
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="121"/>
+      <c r="A12" s="137"/>
       <c r="B12" s="45" t="s">
         <v>63</v>
       </c>
@@ -16471,7 +16907,7 @@
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="121"/>
+      <c r="A13" s="137"/>
       <c r="B13" s="45" t="s">
         <v>64</v>
       </c>
@@ -16528,7 +16964,7 @@
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="121"/>
+      <c r="A14" s="137"/>
       <c r="B14" s="45" t="s">
         <v>65</v>
       </c>
@@ -16585,7 +17021,7 @@
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="121"/>
+      <c r="A15" s="137"/>
       <c r="B15" s="45" t="s">
         <v>66</v>
       </c>
@@ -17347,44 +17783,44 @@
     <row r="1" spans="1:19">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="118" t="s">
+      <c r="C1" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="118" t="s">
+      <c r="D1" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="118" t="s">
+      <c r="E1" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="139" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="119" t="s">
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="134" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
-      <c r="N1" s="119"/>
-      <c r="O1" s="114" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="114"/>
-      <c r="Q1" s="119" t="s">
+      <c r="L1" s="134"/>
+      <c r="M1" s="134"/>
+      <c r="N1" s="134"/>
+      <c r="O1" s="135" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="135"/>
+      <c r="Q1" s="134" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="119"/>
-      <c r="S1" s="119"/>
+      <c r="R1" s="134"/>
+      <c r="S1" s="134"/>
     </row>
     <row r="2" spans="1:19" ht="84">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -17429,7 +17865,7 @@
       </c>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="136" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="44" t="s">
@@ -17488,7 +17924,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="24">
-      <c r="A4" s="121"/>
+      <c r="A4" s="137"/>
       <c r="B4" s="45" t="s">
         <v>55</v>
       </c>
@@ -17545,7 +17981,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="25.5" customHeight="1">
-      <c r="A5" s="121"/>
+      <c r="A5" s="137"/>
       <c r="B5" s="45" t="s">
         <v>57</v>
       </c>
@@ -17602,7 +18038,7 @@
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="121"/>
+      <c r="A6" s="137"/>
       <c r="B6" s="45" t="s">
         <v>58</v>
       </c>
@@ -17659,7 +18095,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="25.5" customHeight="1">
-      <c r="A7" s="121"/>
+      <c r="A7" s="137"/>
       <c r="B7" s="45" t="s">
         <v>59</v>
       </c>
@@ -17716,7 +18152,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="24">
-      <c r="A8" s="121"/>
+      <c r="A8" s="137"/>
       <c r="B8" s="45" t="s">
         <v>60</v>
       </c>
@@ -17773,7 +18209,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="25.5" customHeight="1">
-      <c r="A9" s="121"/>
+      <c r="A9" s="137"/>
       <c r="B9" s="45" t="s">
         <v>61</v>
       </c>
@@ -17830,7 +18266,7 @@
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="121"/>
+      <c r="A10" s="137"/>
       <c r="B10" s="45" t="s">
         <v>62</v>
       </c>
@@ -17887,7 +18323,7 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="121"/>
+      <c r="A11" s="137"/>
       <c r="B11" s="45" t="s">
         <v>56</v>
       </c>
@@ -17944,7 +18380,7 @@
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="121"/>
+      <c r="A12" s="137"/>
       <c r="B12" s="45" t="s">
         <v>63</v>
       </c>
@@ -18001,7 +18437,7 @@
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="121"/>
+      <c r="A13" s="137"/>
       <c r="B13" s="45" t="s">
         <v>64</v>
       </c>
@@ -18058,7 +18494,7 @@
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="121"/>
+      <c r="A14" s="137"/>
       <c r="B14" s="45" t="s">
         <v>65</v>
       </c>
@@ -18115,7 +18551,7 @@
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="121"/>
+      <c r="A15" s="137"/>
       <c r="B15" s="45" t="s">
         <v>66</v>
       </c>
@@ -18929,44 +19365,44 @@
     <row r="1" spans="1:19">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="118" t="s">
+      <c r="C1" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="118" t="s">
+      <c r="D1" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="118" t="s">
+      <c r="E1" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="139" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="119" t="s">
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="134" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
-      <c r="N1" s="119"/>
-      <c r="O1" s="114" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="114"/>
-      <c r="Q1" s="119" t="s">
+      <c r="L1" s="134"/>
+      <c r="M1" s="134"/>
+      <c r="N1" s="134"/>
+      <c r="O1" s="135" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="135"/>
+      <c r="Q1" s="134" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="119"/>
-      <c r="S1" s="119"/>
+      <c r="R1" s="134"/>
+      <c r="S1" s="134"/>
     </row>
     <row r="2" spans="1:19" ht="84">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -19011,7 +19447,7 @@
       </c>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="136" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="44" t="s">
@@ -19070,7 +19506,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="24">
-      <c r="A4" s="121"/>
+      <c r="A4" s="137"/>
       <c r="B4" s="45" t="s">
         <v>55</v>
       </c>
@@ -19127,7 +19563,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="24">
-      <c r="A5" s="121"/>
+      <c r="A5" s="137"/>
       <c r="B5" s="45" t="s">
         <v>57</v>
       </c>
@@ -19184,7 +19620,7 @@
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="121"/>
+      <c r="A6" s="137"/>
       <c r="B6" s="45" t="s">
         <v>58</v>
       </c>
@@ -19241,7 +19677,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="24">
-      <c r="A7" s="121"/>
+      <c r="A7" s="137"/>
       <c r="B7" s="45" t="s">
         <v>59</v>
       </c>
@@ -19298,7 +19734,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="24">
-      <c r="A8" s="121"/>
+      <c r="A8" s="137"/>
       <c r="B8" s="45" t="s">
         <v>60</v>
       </c>
@@ -19355,7 +19791,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="24">
-      <c r="A9" s="121"/>
+      <c r="A9" s="137"/>
       <c r="B9" s="45" t="s">
         <v>61</v>
       </c>
@@ -19412,7 +19848,7 @@
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="121"/>
+      <c r="A10" s="137"/>
       <c r="B10" s="45" t="s">
         <v>62</v>
       </c>
@@ -19469,7 +19905,7 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="121"/>
+      <c r="A11" s="137"/>
       <c r="B11" s="45" t="s">
         <v>56</v>
       </c>
@@ -19526,7 +19962,7 @@
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="121"/>
+      <c r="A12" s="137"/>
       <c r="B12" s="45" t="s">
         <v>63</v>
       </c>
@@ -19583,7 +20019,7 @@
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="121"/>
+      <c r="A13" s="137"/>
       <c r="B13" s="45" t="s">
         <v>64</v>
       </c>
@@ -19640,7 +20076,7 @@
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="121"/>
+      <c r="A14" s="137"/>
       <c r="B14" s="45" t="s">
         <v>65</v>
       </c>
@@ -19697,7 +20133,7 @@
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="121"/>
+      <c r="A15" s="137"/>
       <c r="B15" s="45" t="s">
         <v>66</v>
       </c>
@@ -19831,158 +20267,158 @@
       <c r="K1" s="140"/>
     </row>
     <row r="2" spans="1:44" ht="20" customHeight="1">
-      <c r="C2" s="115">
-        <v>1</v>
-      </c>
-      <c r="D2" s="116"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="115">
+      <c r="C2" s="127">
+        <v>1</v>
+      </c>
+      <c r="D2" s="128"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="127">
         <v>2</v>
       </c>
-      <c r="G2" s="116"/>
-      <c r="H2" s="117"/>
-      <c r="I2" s="115">
+      <c r="G2" s="128"/>
+      <c r="H2" s="129"/>
+      <c r="I2" s="127">
         <v>3</v>
       </c>
-      <c r="J2" s="116"/>
-      <c r="K2" s="117"/>
-      <c r="L2" s="115">
+      <c r="J2" s="128"/>
+      <c r="K2" s="129"/>
+      <c r="L2" s="127">
         <v>4</v>
       </c>
-      <c r="M2" s="116"/>
-      <c r="N2" s="117"/>
-      <c r="O2" s="115">
+      <c r="M2" s="128"/>
+      <c r="N2" s="129"/>
+      <c r="O2" s="127">
         <v>5</v>
       </c>
-      <c r="P2" s="116"/>
-      <c r="Q2" s="117"/>
-      <c r="R2" s="115">
+      <c r="P2" s="128"/>
+      <c r="Q2" s="129"/>
+      <c r="R2" s="127">
         <v>6</v>
       </c>
-      <c r="S2" s="116"/>
-      <c r="T2" s="117"/>
-      <c r="U2" s="115">
+      <c r="S2" s="128"/>
+      <c r="T2" s="129"/>
+      <c r="U2" s="127">
         <v>7</v>
       </c>
-      <c r="V2" s="116"/>
-      <c r="W2" s="117"/>
-      <c r="X2" s="115">
+      <c r="V2" s="128"/>
+      <c r="W2" s="129"/>
+      <c r="X2" s="127">
         <v>8</v>
       </c>
-      <c r="Y2" s="116"/>
-      <c r="Z2" s="117"/>
-      <c r="AA2" s="115">
+      <c r="Y2" s="128"/>
+      <c r="Z2" s="129"/>
+      <c r="AA2" s="127">
         <v>14</v>
       </c>
-      <c r="AB2" s="116"/>
-      <c r="AC2" s="117"/>
-      <c r="AD2" s="115">
+      <c r="AB2" s="128"/>
+      <c r="AC2" s="129"/>
+      <c r="AD2" s="127">
         <v>9</v>
       </c>
-      <c r="AE2" s="116"/>
-      <c r="AF2" s="117"/>
-      <c r="AG2" s="115">
+      <c r="AE2" s="128"/>
+      <c r="AF2" s="129"/>
+      <c r="AG2" s="127">
         <v>10</v>
       </c>
-      <c r="AH2" s="116"/>
-      <c r="AI2" s="117"/>
-      <c r="AJ2" s="115">
+      <c r="AH2" s="128"/>
+      <c r="AI2" s="129"/>
+      <c r="AJ2" s="127">
         <v>11</v>
       </c>
-      <c r="AK2" s="116"/>
-      <c r="AL2" s="117"/>
-      <c r="AM2" s="115">
+      <c r="AK2" s="128"/>
+      <c r="AL2" s="129"/>
+      <c r="AM2" s="127">
         <v>12</v>
       </c>
-      <c r="AN2" s="116"/>
-      <c r="AO2" s="117"/>
-      <c r="AP2" s="115">
+      <c r="AN2" s="128"/>
+      <c r="AO2" s="129"/>
+      <c r="AP2" s="127">
         <v>13</v>
       </c>
-      <c r="AQ2" s="116"/>
-      <c r="AR2" s="117"/>
+      <c r="AQ2" s="128"/>
+      <c r="AR2" s="129"/>
     </row>
     <row r="3" spans="1:44" s="14" customFormat="1" ht="20" customHeight="1">
-      <c r="A3" s="118" t="s">
+      <c r="A3" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="118"/>
-      <c r="C3" s="118" t="s">
+      <c r="B3" s="130"/>
+      <c r="C3" s="130" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="118"/>
-      <c r="E3" s="118"/>
-      <c r="F3" s="118" t="s">
+      <c r="D3" s="130"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="118"/>
-      <c r="H3" s="118"/>
-      <c r="I3" s="118" t="s">
+      <c r="G3" s="130"/>
+      <c r="H3" s="130"/>
+      <c r="I3" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="118"/>
-      <c r="K3" s="118"/>
-      <c r="L3" s="118" t="s">
+      <c r="J3" s="130"/>
+      <c r="K3" s="130"/>
+      <c r="L3" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="118"/>
-      <c r="N3" s="118"/>
-      <c r="O3" s="118" t="s">
+      <c r="M3" s="130"/>
+      <c r="N3" s="130"/>
+      <c r="O3" s="130" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="118"/>
-      <c r="Q3" s="118"/>
-      <c r="R3" s="118" t="s">
+      <c r="P3" s="130"/>
+      <c r="Q3" s="130"/>
+      <c r="R3" s="130" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="118"/>
-      <c r="T3" s="118"/>
-      <c r="U3" s="118" t="s">
+      <c r="S3" s="130"/>
+      <c r="T3" s="130"/>
+      <c r="U3" s="130" t="s">
         <v>15</v>
       </c>
-      <c r="V3" s="118"/>
-      <c r="W3" s="118"/>
-      <c r="X3" s="118" t="s">
+      <c r="V3" s="130"/>
+      <c r="W3" s="130"/>
+      <c r="X3" s="130" t="s">
         <v>6</v>
       </c>
-      <c r="Y3" s="118"/>
-      <c r="Z3" s="118"/>
-      <c r="AA3" s="124" t="s">
+      <c r="Y3" s="130"/>
+      <c r="Z3" s="130"/>
+      <c r="AA3" s="131" t="s">
         <v>54</v>
       </c>
-      <c r="AB3" s="125"/>
-      <c r="AC3" s="126"/>
-      <c r="AD3" s="118" t="s">
+      <c r="AB3" s="132"/>
+      <c r="AC3" s="133"/>
+      <c r="AD3" s="130" t="s">
         <v>30</v>
       </c>
-      <c r="AE3" s="118"/>
-      <c r="AF3" s="118"/>
-      <c r="AG3" s="118" t="s">
+      <c r="AE3" s="130"/>
+      <c r="AF3" s="130"/>
+      <c r="AG3" s="130" t="s">
         <v>31</v>
       </c>
-      <c r="AH3" s="118"/>
-      <c r="AI3" s="118"/>
-      <c r="AJ3" s="118" t="s">
+      <c r="AH3" s="130"/>
+      <c r="AI3" s="130"/>
+      <c r="AJ3" s="130" t="s">
         <v>21</v>
       </c>
-      <c r="AK3" s="118"/>
-      <c r="AL3" s="118"/>
-      <c r="AM3" s="118" t="s">
+      <c r="AK3" s="130"/>
+      <c r="AL3" s="130"/>
+      <c r="AM3" s="130" t="s">
         <v>13</v>
       </c>
-      <c r="AN3" s="118"/>
-      <c r="AO3" s="118"/>
-      <c r="AP3" s="118" t="s">
+      <c r="AN3" s="130"/>
+      <c r="AO3" s="130"/>
+      <c r="AP3" s="130" t="s">
         <v>8</v>
       </c>
-      <c r="AQ3" s="118"/>
-      <c r="AR3" s="118"/>
+      <c r="AQ3" s="130"/>
+      <c r="AR3" s="130"/>
     </row>
     <row r="4" spans="1:44" s="14" customFormat="1" ht="20" customHeight="1">
-      <c r="A4" s="118" t="s">
+      <c r="A4" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="118"/>
+      <c r="B4" s="130"/>
       <c r="C4" s="14">
         <v>2006</v>
       </c>
@@ -20111,10 +20547,10 @@
       </c>
     </row>
     <row r="5" spans="1:44" s="14" customFormat="1" ht="20" customHeight="1">
-      <c r="A5" s="118" t="s">
+      <c r="A5" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="118"/>
+      <c r="B5" s="130"/>
       <c r="C5" s="14">
         <v>4</v>
       </c>
@@ -20243,7 +20679,7 @@
       </c>
     </row>
     <row r="6" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A6" s="123" t="s">
+      <c r="A6" s="139" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -20377,7 +20813,7 @@
       </c>
     </row>
     <row r="7" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A7" s="123"/>
+      <c r="A7" s="139"/>
       <c r="B7" s="16" t="s">
         <v>34</v>
       </c>
@@ -20509,7 +20945,7 @@
       </c>
     </row>
     <row r="8" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A8" s="123"/>
+      <c r="A8" s="139"/>
       <c r="B8" s="16" t="s">
         <v>35</v>
       </c>
@@ -20641,7 +21077,7 @@
       </c>
     </row>
     <row r="9" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A9" s="123"/>
+      <c r="A9" s="139"/>
       <c r="B9" s="15" t="s">
         <v>51</v>
       </c>
@@ -20773,7 +21209,7 @@
       </c>
     </row>
     <row r="10" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A10" s="123"/>
+      <c r="A10" s="139"/>
       <c r="B10" s="16" t="s">
         <v>36</v>
       </c>
@@ -20905,7 +21341,7 @@
       </c>
     </row>
     <row r="11" spans="1:44" ht="20" customHeight="1">
-      <c r="A11" s="119" t="s">
+      <c r="A11" s="134" t="s">
         <v>37</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -21039,7 +21475,7 @@
       </c>
     </row>
     <row r="12" spans="1:44" ht="20" customHeight="1">
-      <c r="A12" s="119"/>
+      <c r="A12" s="134"/>
       <c r="B12" s="6" t="s">
         <v>39</v>
       </c>
@@ -21171,7 +21607,7 @@
       </c>
     </row>
     <row r="13" spans="1:44" ht="20" customHeight="1">
-      <c r="A13" s="119"/>
+      <c r="A13" s="134"/>
       <c r="B13" s="6" t="s">
         <v>40</v>
       </c>
@@ -21303,7 +21739,7 @@
       </c>
     </row>
     <row r="14" spans="1:44" ht="20" customHeight="1">
-      <c r="A14" s="119"/>
+      <c r="A14" s="134"/>
       <c r="B14" s="6" t="s">
         <v>41</v>
       </c>
@@ -21435,7 +21871,7 @@
       </c>
     </row>
     <row r="15" spans="1:44" s="11" customFormat="1" ht="20" customHeight="1">
-      <c r="A15" s="114" t="s">
+      <c r="A15" s="135" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="10" t="s">
@@ -21569,7 +22005,7 @@
       </c>
     </row>
     <row r="16" spans="1:44" s="11" customFormat="1" ht="20" customHeight="1">
-      <c r="A16" s="114"/>
+      <c r="A16" s="135"/>
       <c r="B16" s="10" t="s">
         <v>43</v>
       </c>
@@ -21701,7 +22137,7 @@
       </c>
     </row>
     <row r="17" spans="1:44" ht="20" customHeight="1">
-      <c r="A17" s="119" t="s">
+      <c r="A17" s="134" t="s">
         <v>44</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -21835,7 +22271,7 @@
       </c>
     </row>
     <row r="18" spans="1:44" ht="20" customHeight="1">
-      <c r="A18" s="119"/>
+      <c r="A18" s="134"/>
       <c r="B18" s="6" t="s">
         <v>46</v>
       </c>
@@ -21967,7 +22403,7 @@
       </c>
     </row>
     <row r="19" spans="1:44" ht="20" customHeight="1">
-      <c r="A19" s="119"/>
+      <c r="A19" s="134"/>
       <c r="B19" s="6" t="s">
         <v>47</v>
       </c>
@@ -22625,6 +23061,29 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="AP2:AR2"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="AJ2:AL2"/>
+    <mergeCell ref="AM2:AO2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="U2:W2"/>
+    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="AD2:AF2"/>
+    <mergeCell ref="AA2:AC2"/>
+    <mergeCell ref="AJ3:AL3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AM3:AO3"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="AG3:AI3"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="X3:Z3"/>
+    <mergeCell ref="AD3:AF3"/>
+    <mergeCell ref="AA3:AC3"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="O3:Q3"/>
     <mergeCell ref="R3:T3"/>
@@ -22638,29 +23097,6 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C2:E2"/>
-    <mergeCell ref="AJ3:AL3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AM3:AO3"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="AG3:AI3"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="X3:Z3"/>
-    <mergeCell ref="AD3:AF3"/>
-    <mergeCell ref="AA3:AC3"/>
-    <mergeCell ref="AP2:AR2"/>
-    <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="AJ2:AL2"/>
-    <mergeCell ref="AM2:AO2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="U2:W2"/>
-    <mergeCell ref="X2:Z2"/>
-    <mergeCell ref="AD2:AF2"/>
-    <mergeCell ref="AA2:AC2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -22872,44 +23308,44 @@
     <row r="1" spans="1:19">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="118" t="s">
+      <c r="C1" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="118" t="s">
+      <c r="D1" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="118" t="s">
+      <c r="E1" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="139" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="119" t="s">
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="134" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
-      <c r="N1" s="119"/>
-      <c r="O1" s="114" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="114"/>
-      <c r="Q1" s="119" t="s">
+      <c r="L1" s="134"/>
+      <c r="M1" s="134"/>
+      <c r="N1" s="134"/>
+      <c r="O1" s="135" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="135"/>
+      <c r="Q1" s="134" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="119"/>
-      <c r="S1" s="119"/>
+      <c r="R1" s="134"/>
+      <c r="S1" s="134"/>
     </row>
     <row r="2" spans="1:19" ht="84">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -22954,13 +23390,13 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="136" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="115">
-        <v>1</v>
-      </c>
-      <c r="C3" s="118" t="s">
+      <c r="B3" s="127">
+        <v>1</v>
+      </c>
+      <c r="C3" s="130" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="14">
@@ -23013,9 +23449,9 @@
       </c>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="121"/>
-      <c r="B4" s="116"/>
-      <c r="C4" s="118"/>
+      <c r="A4" s="137"/>
+      <c r="B4" s="128"/>
+      <c r="C4" s="130"/>
       <c r="D4" s="14">
         <v>2010</v>
       </c>
@@ -23066,9 +23502,9 @@
       </c>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="121"/>
-      <c r="B5" s="117"/>
-      <c r="C5" s="118"/>
+      <c r="A5" s="137"/>
+      <c r="B5" s="129"/>
+      <c r="C5" s="130"/>
       <c r="D5" s="25">
         <v>2014</v>
       </c>
@@ -23119,11 +23555,11 @@
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="121"/>
-      <c r="B6" s="115">
+      <c r="A6" s="137"/>
+      <c r="B6" s="127">
         <v>2</v>
       </c>
-      <c r="C6" s="118" t="s">
+      <c r="C6" s="130" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="14">
@@ -23176,9 +23612,9 @@
       </c>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="121"/>
-      <c r="B7" s="116"/>
-      <c r="C7" s="118"/>
+      <c r="A7" s="137"/>
+      <c r="B7" s="128"/>
+      <c r="C7" s="130"/>
       <c r="D7" s="14">
         <v>2010</v>
       </c>
@@ -23229,9 +23665,9 @@
       </c>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" s="121"/>
-      <c r="B8" s="117"/>
-      <c r="C8" s="118"/>
+      <c r="A8" s="137"/>
+      <c r="B8" s="129"/>
+      <c r="C8" s="130"/>
       <c r="D8" s="25">
         <v>2014</v>
       </c>
@@ -23282,11 +23718,11 @@
       </c>
     </row>
     <row r="9" spans="1:19">
-      <c r="A9" s="121"/>
-      <c r="B9" s="115">
+      <c r="A9" s="137"/>
+      <c r="B9" s="127">
         <v>3</v>
       </c>
-      <c r="C9" s="118" t="s">
+      <c r="C9" s="130" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="14">
@@ -23339,9 +23775,9 @@
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="121"/>
-      <c r="B10" s="116"/>
-      <c r="C10" s="118"/>
+      <c r="A10" s="137"/>
+      <c r="B10" s="128"/>
+      <c r="C10" s="130"/>
       <c r="D10" s="14">
         <v>2010</v>
       </c>
@@ -23392,9 +23828,9 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="121"/>
-      <c r="B11" s="117"/>
-      <c r="C11" s="118"/>
+      <c r="A11" s="137"/>
+      <c r="B11" s="129"/>
+      <c r="C11" s="130"/>
       <c r="D11" s="25">
         <v>2014</v>
       </c>
@@ -23445,11 +23881,11 @@
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="121"/>
-      <c r="B12" s="115">
+      <c r="A12" s="137"/>
+      <c r="B12" s="127">
         <v>4</v>
       </c>
-      <c r="C12" s="118" t="s">
+      <c r="C12" s="130" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="14">
@@ -23502,9 +23938,9 @@
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="121"/>
-      <c r="B13" s="116"/>
-      <c r="C13" s="118"/>
+      <c r="A13" s="137"/>
+      <c r="B13" s="128"/>
+      <c r="C13" s="130"/>
       <c r="D13" s="14">
         <v>2010</v>
       </c>
@@ -23555,9 +23991,9 @@
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="121"/>
-      <c r="B14" s="117"/>
-      <c r="C14" s="118"/>
+      <c r="A14" s="137"/>
+      <c r="B14" s="129"/>
+      <c r="C14" s="130"/>
       <c r="D14" s="25">
         <v>2014</v>
       </c>
@@ -23608,11 +24044,11 @@
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="121"/>
-      <c r="B15" s="115">
+      <c r="A15" s="137"/>
+      <c r="B15" s="127">
         <v>5</v>
       </c>
-      <c r="C15" s="118" t="s">
+      <c r="C15" s="130" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="14">
@@ -23665,9 +24101,9 @@
       </c>
     </row>
     <row r="16" spans="1:19">
-      <c r="A16" s="121"/>
-      <c r="B16" s="116"/>
-      <c r="C16" s="118"/>
+      <c r="A16" s="137"/>
+      <c r="B16" s="128"/>
+      <c r="C16" s="130"/>
       <c r="D16" s="14">
         <v>2010</v>
       </c>
@@ -23718,9 +24154,9 @@
       </c>
     </row>
     <row r="17" spans="1:19">
-      <c r="A17" s="121"/>
-      <c r="B17" s="117"/>
-      <c r="C17" s="118"/>
+      <c r="A17" s="137"/>
+      <c r="B17" s="129"/>
+      <c r="C17" s="130"/>
       <c r="D17" s="25">
         <v>2014</v>
       </c>
@@ -23771,11 +24207,11 @@
       </c>
     </row>
     <row r="18" spans="1:19">
-      <c r="A18" s="121"/>
-      <c r="B18" s="115">
+      <c r="A18" s="137"/>
+      <c r="B18" s="127">
         <v>6</v>
       </c>
-      <c r="C18" s="118" t="s">
+      <c r="C18" s="130" t="s">
         <v>25</v>
       </c>
       <c r="D18" s="14">
@@ -23828,9 +24264,9 @@
       </c>
     </row>
     <row r="19" spans="1:19">
-      <c r="A19" s="121"/>
-      <c r="B19" s="116"/>
-      <c r="C19" s="118"/>
+      <c r="A19" s="137"/>
+      <c r="B19" s="128"/>
+      <c r="C19" s="130"/>
       <c r="D19" s="14">
         <v>2010</v>
       </c>
@@ -23881,9 +24317,9 @@
       </c>
     </row>
     <row r="20" spans="1:19">
-      <c r="A20" s="121"/>
-      <c r="B20" s="117"/>
-      <c r="C20" s="118"/>
+      <c r="A20" s="137"/>
+      <c r="B20" s="129"/>
+      <c r="C20" s="130"/>
       <c r="D20" s="25">
         <v>2014</v>
       </c>
@@ -23934,11 +24370,11 @@
       </c>
     </row>
     <row r="21" spans="1:19">
-      <c r="A21" s="121"/>
-      <c r="B21" s="115">
+      <c r="A21" s="137"/>
+      <c r="B21" s="127">
         <v>7</v>
       </c>
-      <c r="C21" s="118" t="s">
+      <c r="C21" s="130" t="s">
         <v>15</v>
       </c>
       <c r="D21" s="14">
@@ -23991,9 +24427,9 @@
       </c>
     </row>
     <row r="22" spans="1:19">
-      <c r="A22" s="121"/>
-      <c r="B22" s="116"/>
-      <c r="C22" s="118"/>
+      <c r="A22" s="137"/>
+      <c r="B22" s="128"/>
+      <c r="C22" s="130"/>
       <c r="D22" s="14">
         <v>2010</v>
       </c>
@@ -24044,9 +24480,9 @@
       </c>
     </row>
     <row r="23" spans="1:19">
-      <c r="A23" s="121"/>
-      <c r="B23" s="117"/>
-      <c r="C23" s="118"/>
+      <c r="A23" s="137"/>
+      <c r="B23" s="129"/>
+      <c r="C23" s="130"/>
       <c r="D23" s="25">
         <v>2014</v>
       </c>
@@ -24097,11 +24533,11 @@
       </c>
     </row>
     <row r="24" spans="1:19">
-      <c r="A24" s="121"/>
-      <c r="B24" s="115">
+      <c r="A24" s="137"/>
+      <c r="B24" s="127">
         <v>8</v>
       </c>
-      <c r="C24" s="118" t="s">
+      <c r="C24" s="130" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="14">
@@ -24154,9 +24590,9 @@
       </c>
     </row>
     <row r="25" spans="1:19">
-      <c r="A25" s="121"/>
-      <c r="B25" s="116"/>
-      <c r="C25" s="118"/>
+      <c r="A25" s="137"/>
+      <c r="B25" s="128"/>
+      <c r="C25" s="130"/>
       <c r="D25" s="14">
         <v>2010</v>
       </c>
@@ -24207,9 +24643,9 @@
       </c>
     </row>
     <row r="26" spans="1:19">
-      <c r="A26" s="121"/>
-      <c r="B26" s="117"/>
-      <c r="C26" s="118"/>
+      <c r="A26" s="137"/>
+      <c r="B26" s="129"/>
+      <c r="C26" s="130"/>
       <c r="D26" s="25">
         <v>2014</v>
       </c>
@@ -24260,11 +24696,11 @@
       </c>
     </row>
     <row r="27" spans="1:19">
-      <c r="A27" s="121"/>
-      <c r="B27" s="115">
+      <c r="A27" s="137"/>
+      <c r="B27" s="127">
         <v>14</v>
       </c>
-      <c r="C27" s="124" t="s">
+      <c r="C27" s="131" t="s">
         <v>54</v>
       </c>
       <c r="D27" s="14">
@@ -24317,9 +24753,9 @@
       </c>
     </row>
     <row r="28" spans="1:19">
-      <c r="A28" s="121"/>
-      <c r="B28" s="116"/>
-      <c r="C28" s="125"/>
+      <c r="A28" s="137"/>
+      <c r="B28" s="128"/>
+      <c r="C28" s="132"/>
       <c r="D28" s="14">
         <v>2010</v>
       </c>
@@ -24370,9 +24806,9 @@
       </c>
     </row>
     <row r="29" spans="1:19">
-      <c r="A29" s="121"/>
-      <c r="B29" s="117"/>
-      <c r="C29" s="126"/>
+      <c r="A29" s="137"/>
+      <c r="B29" s="129"/>
+      <c r="C29" s="133"/>
       <c r="D29" s="25">
         <v>2014</v>
       </c>
@@ -24423,11 +24859,11 @@
       </c>
     </row>
     <row r="30" spans="1:19">
-      <c r="A30" s="121"/>
-      <c r="B30" s="115">
+      <c r="A30" s="137"/>
+      <c r="B30" s="127">
         <v>9</v>
       </c>
-      <c r="C30" s="118" t="s">
+      <c r="C30" s="130" t="s">
         <v>12</v>
       </c>
       <c r="D30" s="14">
@@ -24480,9 +24916,9 @@
       </c>
     </row>
     <row r="31" spans="1:19">
-      <c r="A31" s="121"/>
-      <c r="B31" s="116"/>
-      <c r="C31" s="118"/>
+      <c r="A31" s="137"/>
+      <c r="B31" s="128"/>
+      <c r="C31" s="130"/>
       <c r="D31" s="14">
         <v>2010</v>
       </c>
@@ -24533,9 +24969,9 @@
       </c>
     </row>
     <row r="32" spans="1:19">
-      <c r="A32" s="121"/>
-      <c r="B32" s="117"/>
-      <c r="C32" s="118"/>
+      <c r="A32" s="137"/>
+      <c r="B32" s="129"/>
+      <c r="C32" s="130"/>
       <c r="D32" s="25">
         <v>2014</v>
       </c>
@@ -24586,11 +25022,11 @@
       </c>
     </row>
     <row r="33" spans="1:41">
-      <c r="A33" s="121"/>
-      <c r="B33" s="115">
+      <c r="A33" s="137"/>
+      <c r="B33" s="127">
         <v>10</v>
       </c>
-      <c r="C33" s="118" t="s">
+      <c r="C33" s="130" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="14">
@@ -24643,9 +25079,9 @@
       </c>
     </row>
     <row r="34" spans="1:41">
-      <c r="A34" s="121"/>
-      <c r="B34" s="116"/>
-      <c r="C34" s="118"/>
+      <c r="A34" s="137"/>
+      <c r="B34" s="128"/>
+      <c r="C34" s="130"/>
       <c r="D34" s="14">
         <v>2010</v>
       </c>
@@ -24696,9 +25132,9 @@
       </c>
     </row>
     <row r="35" spans="1:41">
-      <c r="A35" s="121"/>
-      <c r="B35" s="117"/>
-      <c r="C35" s="118"/>
+      <c r="A35" s="137"/>
+      <c r="B35" s="129"/>
+      <c r="C35" s="130"/>
       <c r="D35" s="25">
         <v>2014</v>
       </c>
@@ -24749,11 +25185,11 @@
       </c>
     </row>
     <row r="36" spans="1:41">
-      <c r="A36" s="121"/>
-      <c r="B36" s="115">
+      <c r="A36" s="137"/>
+      <c r="B36" s="127">
         <v>11</v>
       </c>
-      <c r="C36" s="118" t="s">
+      <c r="C36" s="130" t="s">
         <v>21</v>
       </c>
       <c r="D36" s="14">
@@ -24806,9 +25242,9 @@
       </c>
     </row>
     <row r="37" spans="1:41">
-      <c r="A37" s="121"/>
-      <c r="B37" s="116"/>
-      <c r="C37" s="118"/>
+      <c r="A37" s="137"/>
+      <c r="B37" s="128"/>
+      <c r="C37" s="130"/>
       <c r="D37" s="14">
         <v>2010</v>
       </c>
@@ -24859,9 +25295,9 @@
       </c>
     </row>
     <row r="38" spans="1:41">
-      <c r="A38" s="121"/>
-      <c r="B38" s="117"/>
-      <c r="C38" s="118"/>
+      <c r="A38" s="137"/>
+      <c r="B38" s="129"/>
+      <c r="C38" s="130"/>
       <c r="D38" s="25">
         <v>2014</v>
       </c>
@@ -24912,11 +25348,11 @@
       </c>
     </row>
     <row r="39" spans="1:41">
-      <c r="A39" s="121"/>
-      <c r="B39" s="115">
+      <c r="A39" s="137"/>
+      <c r="B39" s="127">
         <v>12</v>
       </c>
-      <c r="C39" s="118" t="s">
+      <c r="C39" s="130" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="14">
@@ -24969,9 +25405,9 @@
       </c>
     </row>
     <row r="40" spans="1:41">
-      <c r="A40" s="121"/>
-      <c r="B40" s="116"/>
-      <c r="C40" s="118"/>
+      <c r="A40" s="137"/>
+      <c r="B40" s="128"/>
+      <c r="C40" s="130"/>
       <c r="D40" s="14">
         <v>2010</v>
       </c>
@@ -25022,9 +25458,9 @@
       </c>
     </row>
     <row r="41" spans="1:41">
-      <c r="A41" s="121"/>
-      <c r="B41" s="117"/>
-      <c r="C41" s="118"/>
+      <c r="A41" s="137"/>
+      <c r="B41" s="129"/>
+      <c r="C41" s="130"/>
       <c r="D41" s="25">
         <v>2014</v>
       </c>
@@ -25075,11 +25511,11 @@
       </c>
     </row>
     <row r="42" spans="1:41">
-      <c r="A42" s="121"/>
-      <c r="B42" s="115">
+      <c r="A42" s="137"/>
+      <c r="B42" s="127">
         <v>13</v>
       </c>
-      <c r="C42" s="118" t="s">
+      <c r="C42" s="130" t="s">
         <v>8</v>
       </c>
       <c r="D42" s="14">
@@ -25132,9 +25568,9 @@
       </c>
     </row>
     <row r="43" spans="1:41">
-      <c r="A43" s="121"/>
-      <c r="B43" s="116"/>
-      <c r="C43" s="118"/>
+      <c r="A43" s="137"/>
+      <c r="B43" s="128"/>
+      <c r="C43" s="130"/>
       <c r="D43" s="14">
         <v>2010</v>
       </c>
@@ -25185,9 +25621,9 @@
       </c>
     </row>
     <row r="44" spans="1:41">
-      <c r="A44" s="122"/>
-      <c r="B44" s="117"/>
-      <c r="C44" s="118"/>
+      <c r="A44" s="138"/>
+      <c r="B44" s="129"/>
+      <c r="C44" s="130"/>
       <c r="D44" s="25">
         <v>2014</v>
       </c>
@@ -25238,81 +25674,81 @@
       </c>
     </row>
     <row r="46" spans="1:41" ht="15.75" customHeight="1">
-      <c r="A46" s="118" t="s">
+      <c r="A46" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="118"/>
-      <c r="C46" s="118" t="s">
+      <c r="B46" s="130"/>
+      <c r="C46" s="130" t="s">
         <v>50</v>
       </c>
-      <c r="D46" s="118"/>
-      <c r="E46" s="118"/>
-      <c r="F46" s="118" t="s">
+      <c r="D46" s="130"/>
+      <c r="E46" s="130"/>
+      <c r="F46" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="G46" s="118"/>
-      <c r="H46" s="118"/>
-      <c r="I46" s="118" t="s">
+      <c r="G46" s="130"/>
+      <c r="H46" s="130"/>
+      <c r="I46" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="J46" s="118"/>
-      <c r="K46" s="118"/>
-      <c r="L46" s="118" t="s">
+      <c r="J46" s="130"/>
+      <c r="K46" s="130"/>
+      <c r="L46" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="M46" s="118"/>
-      <c r="N46" s="118"/>
-      <c r="O46" s="118" t="s">
+      <c r="M46" s="130"/>
+      <c r="N46" s="130"/>
+      <c r="O46" s="130" t="s">
         <v>23</v>
       </c>
-      <c r="P46" s="118"/>
-      <c r="Q46" s="118"/>
-      <c r="R46" s="118" t="s">
+      <c r="P46" s="130"/>
+      <c r="Q46" s="130"/>
+      <c r="R46" s="130" t="s">
         <v>87</v>
       </c>
-      <c r="S46" s="118"/>
-      <c r="T46" s="118"/>
-      <c r="U46" s="124" t="s">
+      <c r="S46" s="130"/>
+      <c r="T46" s="130"/>
+      <c r="U46" s="131" t="s">
         <v>70</v>
       </c>
-      <c r="V46" s="125"/>
-      <c r="W46" s="126"/>
-      <c r="X46" s="124" t="s">
+      <c r="V46" s="132"/>
+      <c r="W46" s="133"/>
+      <c r="X46" s="131" t="s">
         <v>54</v>
       </c>
-      <c r="Y46" s="125"/>
-      <c r="Z46" s="126"/>
-      <c r="AA46" s="118" t="s">
+      <c r="Y46" s="132"/>
+      <c r="Z46" s="133"/>
+      <c r="AA46" s="130" t="s">
         <v>12</v>
       </c>
-      <c r="AB46" s="118"/>
-      <c r="AC46" s="118"/>
-      <c r="AD46" s="118" t="s">
+      <c r="AB46" s="130"/>
+      <c r="AC46" s="130"/>
+      <c r="AD46" s="130" t="s">
         <v>28</v>
       </c>
-      <c r="AE46" s="118"/>
-      <c r="AF46" s="118"/>
-      <c r="AG46" s="118" t="s">
+      <c r="AE46" s="130"/>
+      <c r="AF46" s="130"/>
+      <c r="AG46" s="130" t="s">
         <v>21</v>
       </c>
-      <c r="AH46" s="118"/>
-      <c r="AI46" s="118"/>
-      <c r="AJ46" s="118" t="s">
+      <c r="AH46" s="130"/>
+      <c r="AI46" s="130"/>
+      <c r="AJ46" s="130" t="s">
         <v>13</v>
       </c>
-      <c r="AK46" s="118"/>
-      <c r="AL46" s="118"/>
-      <c r="AM46" s="118" t="s">
+      <c r="AK46" s="130"/>
+      <c r="AL46" s="130"/>
+      <c r="AM46" s="130" t="s">
         <v>8</v>
       </c>
-      <c r="AN46" s="118"/>
-      <c r="AO46" s="118"/>
+      <c r="AN46" s="130"/>
+      <c r="AO46" s="130"/>
     </row>
     <row r="47" spans="1:41" ht="42.75" customHeight="1">
-      <c r="A47" s="118" t="s">
+      <c r="A47" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="118"/>
+      <c r="B47" s="130"/>
       <c r="C47" s="54" t="s">
         <v>72</v>
       </c>
@@ -25432,10 +25868,10 @@
       </c>
     </row>
     <row r="48" spans="1:41" ht="33" customHeight="1">
-      <c r="A48" s="118" t="s">
+      <c r="A48" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="118"/>
+      <c r="B48" s="130"/>
       <c r="C48" s="54">
         <v>4</v>
       </c>
@@ -25566,7 +26002,7 @@
       </c>
     </row>
     <row r="50" spans="2:4">
-      <c r="B50" s="134"/>
+      <c r="B50" s="120"/>
       <c r="C50" s="63">
         <v>2010</v>
       </c>
@@ -25575,7 +26011,7 @@
       </c>
     </row>
     <row r="51" spans="2:4">
-      <c r="B51" s="134"/>
+      <c r="B51" s="120"/>
       <c r="C51" s="63">
         <v>2014</v>
       </c>
@@ -25585,26 +26021,23 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="AA46:AC46"/>
+    <mergeCell ref="AD46:AF46"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="L46:N46"/>
+    <mergeCell ref="AG46:AI46"/>
+    <mergeCell ref="AJ46:AL46"/>
+    <mergeCell ref="AM46:AO46"/>
+    <mergeCell ref="O46:Q46"/>
+    <mergeCell ref="R46:T46"/>
+    <mergeCell ref="U46:W46"/>
+    <mergeCell ref="X46:Z46"/>
     <mergeCell ref="B39:B41"/>
     <mergeCell ref="C39:C41"/>
     <mergeCell ref="B42:B44"/>
@@ -25621,23 +26054,26 @@
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="C24:C26"/>
     <mergeCell ref="B27:B29"/>
-    <mergeCell ref="AG46:AI46"/>
-    <mergeCell ref="AJ46:AL46"/>
-    <mergeCell ref="AM46:AO46"/>
-    <mergeCell ref="O46:Q46"/>
-    <mergeCell ref="R46:T46"/>
-    <mergeCell ref="U46:W46"/>
-    <mergeCell ref="X46:Z46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="AA46:AC46"/>
-    <mergeCell ref="AD46:AF46"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="I46:K46"/>
-    <mergeCell ref="L46:N46"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>